<commit_message>
almost done hang in there
</commit_message>
<xml_diff>
--- a/01_Raw_data/RC log.xlsx
+++ b/01_Raw_data/RC log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Howley_Bradford_Streams\Howley_Bradford_Streams\01_Raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samanthahowley\Desktop\Howley_Bradford_Streams\01_Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF8CBCA-D112-4C8F-93DA-CFC2F9178B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F448DC-2539-4B78-B8C8-DAFF8735B261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A079E74B-2391-4069-81A1-6515CCD90540}"/>
   </bookViews>
@@ -120,9 +120,6 @@
     <t>K30</t>
   </si>
   <si>
-    <t>CO2 (mv)</t>
-  </si>
-  <si>
     <t>CO2_ppm</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>surface_height</t>
+  </si>
+  <si>
+    <t>CO2_mv</t>
   </si>
 </sst>
 </file>
@@ -3688,18 +3688,18 @@
   <dimension ref="A1:K97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X70" sqref="X70"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.40625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -3725,16 +3725,16 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
         <v>28</v>
-      </c>
-      <c r="J1" t="s">
-        <v>29</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45400</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45400</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45400</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45400</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45400</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45400</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45400</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45400</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45400</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45400</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45400</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45400</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45400</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45400</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45400</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45400</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45420</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45420</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45420</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45420</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45420</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45420</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45420</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45420</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45420</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45420</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45420</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45420</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45420</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45420</v>
       </c>
@@ -4631,7 +4631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45420</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45420</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45442</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45442</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45442</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45442</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45442</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45442</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45442</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45442</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45442</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45442</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45442</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45442</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45442</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45442</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45442</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45442</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45463</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>-0.85000000000000009</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45463</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>-1.55</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45463</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45463</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45463</v>
       </c>
@@ -5314,7 +5314,7 @@
         <v>-0.12</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45463</v>
       </c>
@@ -5338,7 +5338,7 @@
         <v>-1.24</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>45463</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>45463</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>45463</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45463</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>-2.64</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45463</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>-1.0999999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45463</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>-2.79</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45463</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>-1.4649999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45463</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>6070.24</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45463</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>-2.19</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>45463</v>
       </c>
@@ -5624,7 +5624,7 @@
         <v>-2.0049999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>45484</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>45484</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>45484</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>45484</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>45484</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>45484</v>
       </c>
@@ -5844,7 +5844,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>45484</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>45484</v>
       </c>
@@ -5918,7 +5918,7 @@
         <v>27.75</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>45484</v>
       </c>
@@ -5955,7 +5955,7 @@
         <v>25.89</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>45484</v>
       </c>
@@ -5992,7 +5992,7 @@
         <v>26.57</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>45484</v>
       </c>
@@ -6029,7 +6029,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>45484</v>
       </c>
@@ -6059,7 +6059,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>45484</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>45484</v>
       </c>
@@ -6126,7 +6126,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>45484</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>45484</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>45502</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>45502</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>45502</v>
       </c>
@@ -6292,7 +6292,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>45502</v>
       </c>
@@ -6329,7 +6329,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>45502</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>25.72</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>45502</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>45502</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>45502</v>
       </c>
@@ -6468,7 +6468,7 @@
         <v>34.33</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>45502</v>
       </c>
@@ -6501,7 +6501,7 @@
         <v>32.46</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>45502</v>
       </c>
@@ -6534,7 +6534,7 @@
         <v>29.26</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>45502</v>
       </c>
@@ -6571,7 +6571,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>45502</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>45502</v>
       </c>
@@ -6644,7 +6644,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>45502</v>
       </c>
@@ -6681,7 +6681,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>45502</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>45502</v>
       </c>
@@ -6751,15 +6751,15 @@
       <selection activeCell="E2" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.40625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -6767,13 +6767,13 @@
         <v>25</v>
       </c>
       <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>26</v>
@@ -6782,7 +6782,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>79.863910000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>76.943730000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>88.202100000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -6878,7 +6878,7 @@
         <v>76.922430000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -6902,7 +6902,7 @@
         <v>92.059330000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>76.370699999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>93.197450000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>76.815430000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -6998,7 +6998,7 @@
         <v>76.590829999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -7022,7 +7022,7 @@
         <v>76.606219999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>76.513019999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>76.622630000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>66.857730000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -7118,7 +7118,7 @@
         <v>67.045649999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>67.109120000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>66.502930000000006</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G18">
         <v>652.93119999999999</v>
       </c>
@@ -7171,7 +7171,7 @@
         <v>66.842190000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G19">
         <v>653.20910000000003</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>66.69511</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G20">
         <v>607.95830000000001</v>
       </c>
@@ -7187,7 +7187,7 @@
         <v>67.072839999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G21">
         <v>607.56110000000001</v>
       </c>
@@ -7195,7 +7195,7 @@
         <v>66.492159999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G22">
         <v>638.08180000000004</v>
       </c>
@@ -7203,7 +7203,7 @@
         <v>66.821780000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G23">
         <v>638.25340000000006</v>
       </c>
@@ -7211,7 +7211,7 @@
         <v>66.970429999999993</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G24">
         <v>623.13530000000003</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>66.743210000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G25">
         <v>607.76750000000004</v>
       </c>
@@ -7227,7 +7227,7 @@
         <v>66.741129999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G26">
         <v>592.50710000000004</v>
       </c>
@@ -7235,7 +7235,7 @@
         <v>66.642009999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G27">
         <v>577.47490000000005</v>
       </c>
@@ -7243,7 +7243,7 @@
         <v>66.604929999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G28">
         <v>562.39620000000002</v>
       </c>
@@ -7251,7 +7251,7 @@
         <v>66.727909999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G29">
         <v>562.76610000000005</v>
       </c>
@@ -7259,7 +7259,7 @@
         <v>66.755129999999994</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G30">
         <v>562.50009999999997</v>
       </c>
@@ -7267,7 +7267,7 @@
         <v>66.565960000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G31">
         <v>562.36329999999998</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>66.708879999999994</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G32">
         <v>577.42870000000005</v>
       </c>
@@ -7283,7 +7283,7 @@
         <v>66.438630000000003</v>
       </c>
     </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G33">
         <v>577.51340000000005</v>
       </c>
@@ -7291,7 +7291,7 @@
         <v>66.721999999999994</v>
       </c>
     </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G34">
         <v>622.80349999999999</v>
       </c>
@@ -7299,7 +7299,7 @@
         <v>66.502319999999997</v>
       </c>
     </row>
-    <row r="35" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G35">
         <v>698.44579999999996</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>66.603359999999995</v>
       </c>
     </row>
-    <row r="36" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G36">
         <v>728.82050000000004</v>
       </c>
@@ -7315,7 +7315,7 @@
         <v>66.735640000000004</v>
       </c>
     </row>
-    <row r="37" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G37">
         <v>744.46180000000004</v>
       </c>
@@ -7323,7 +7323,7 @@
         <v>67.009540000000001</v>
       </c>
     </row>
-    <row r="38" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G38">
         <v>728.54539999999997</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>66.730959999999996</v>
       </c>
     </row>
-    <row r="39" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="39" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G39">
         <v>728.59079999999994</v>
       </c>
@@ -7339,7 +7339,7 @@
         <v>66.700519999999997</v>
       </c>
     </row>
-    <row r="40" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="40" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G40">
         <v>728.52480000000003</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>66.432400000000001</v>
       </c>
     </row>
-    <row r="41" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="41" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G41">
         <v>744.04729999999995</v>
       </c>
@@ -7355,7 +7355,7 @@
         <v>66.440209999999993</v>
       </c>
     </row>
-    <row r="42" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="42" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G42">
         <v>744.07650000000001</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>66.810680000000005</v>
       </c>
     </row>
-    <row r="43" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="43" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G43">
         <v>759.36440000000005</v>
       </c>
@@ -7371,7 +7371,7 @@
         <v>66.765969999999996</v>
       </c>
     </row>
-    <row r="44" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="44" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G44">
         <v>774.61670000000004</v>
       </c>
@@ -7379,7 +7379,7 @@
         <v>66.688059999999993</v>
       </c>
     </row>
-    <row r="45" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="45" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G45">
         <v>774.67240000000004</v>
       </c>
@@ -7387,7 +7387,7 @@
         <v>66.708640000000003</v>
       </c>
     </row>
-    <row r="46" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="46" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G46">
         <v>789.6807</v>
       </c>
@@ -7395,7 +7395,7 @@
         <v>66.707120000000003</v>
       </c>
     </row>
-    <row r="47" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="47" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G47">
         <v>834.55520000000001</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>66.699510000000004</v>
       </c>
     </row>
-    <row r="48" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="48" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G48">
         <v>834.96130000000005</v>
       </c>
@@ -7411,7 +7411,7 @@
         <v>67.011229999999998</v>
       </c>
     </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="49" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G49">
         <v>850.197</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>66.578879999999998</v>
       </c>
     </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G50">
         <v>865.02120000000002</v>
       </c>
@@ -7427,7 +7427,7 @@
         <v>66.439570000000003</v>
       </c>
     </row>
-    <row r="51" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="51" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G51">
         <v>865.25400000000002</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>66.421679999999995</v>
       </c>
     </row>
-    <row r="52" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="52" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G52">
         <v>880.46839999999997</v>
       </c>
@@ -7443,7 +7443,7 @@
         <v>66.699039999999997</v>
       </c>
     </row>
-    <row r="53" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="53" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G53">
         <v>895.39089999999999</v>
       </c>
@@ -7451,7 +7451,7 @@
         <v>66.41798</v>
       </c>
     </row>
-    <row r="54" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="54" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G54">
         <v>895.33799999999997</v>
       </c>
@@ -7459,7 +7459,7 @@
         <v>66.555769999999995</v>
       </c>
     </row>
-    <row r="55" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="55" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G55">
         <v>910.66690000000006</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>66.713909999999998</v>
       </c>
     </row>
-    <row r="56" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="56" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G56">
         <v>925.98109999999997</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>66.679460000000006</v>
       </c>
     </row>
-    <row r="57" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="57" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G57">
         <v>940.77919999999995</v>
       </c>
@@ -7483,7 +7483,7 @@
         <v>66.716350000000006</v>
       </c>
     </row>
-    <row r="58" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="58" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G58">
         <v>955.72770000000003</v>
       </c>
@@ -7491,7 +7491,7 @@
         <v>66.600700000000003</v>
       </c>
     </row>
-    <row r="59" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="59" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G59">
         <v>970.87699999999995</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>67.232489999999999</v>
       </c>
     </row>
-    <row r="60" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="60" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G60">
         <v>986.60170000000005</v>
       </c>
@@ -7507,7 +7507,7 @@
         <v>66.475719999999995</v>
       </c>
     </row>
-    <row r="61" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="61" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G61">
         <v>1001.513</v>
       </c>
@@ -7515,7 +7515,7 @@
         <v>69.48903</v>
       </c>
     </row>
-    <row r="62" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="62" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G62">
         <v>1016.558</v>
       </c>
@@ -7523,7 +7523,7 @@
         <v>66.661689999999993</v>
       </c>
     </row>
-    <row r="63" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="63" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G63">
         <v>1031.5419999999999</v>
       </c>
@@ -7531,7 +7531,7 @@
         <v>77.511840000000007</v>
       </c>
     </row>
-    <row r="64" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="64" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G64">
         <v>1047.2439999999999</v>
       </c>
@@ -7539,7 +7539,7 @@
         <v>66.713200000000001</v>
       </c>
     </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="65" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G65">
         <v>1061.7260000000001</v>
       </c>
@@ -7547,7 +7547,7 @@
         <v>80.544539999999998</v>
       </c>
     </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G66">
         <v>1077.3230000000001</v>
       </c>
@@ -7555,7 +7555,7 @@
         <v>66.882890000000003</v>
       </c>
     </row>
-    <row r="67" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="67" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G67">
         <v>1107.306</v>
       </c>
@@ -7563,7 +7563,7 @@
         <v>82.613020000000006</v>
       </c>
     </row>
-    <row r="68" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="68" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G68">
         <v>1122.7550000000001</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>66.875720000000001</v>
       </c>
     </row>
-    <row r="69" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="69" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G69">
         <v>1167.7729999999999</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>81.679119999999998</v>
       </c>
     </row>
-    <row r="70" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="70" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G70">
         <v>1183.0219999999999</v>
       </c>
@@ -7587,7 +7587,7 @@
         <v>76.520039999999995</v>
       </c>
     </row>
-    <row r="71" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="71" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G71">
         <v>1183.3119999999999</v>
       </c>
@@ -7595,7 +7595,7 @@
         <v>76.523030000000006</v>
       </c>
     </row>
-    <row r="72" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="72" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G72">
         <v>1198.4190000000001</v>
       </c>
@@ -7603,7 +7603,7 @@
         <v>76.558539999999994</v>
       </c>
     </row>
-    <row r="73" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="73" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G73">
         <v>1213.2</v>
       </c>
@@ -7611,7 +7611,7 @@
         <v>76.322270000000003</v>
       </c>
     </row>
-    <row r="74" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="74" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G74">
         <v>1213.443</v>
       </c>
@@ -7619,7 +7619,7 @@
         <v>76.840400000000002</v>
       </c>
     </row>
-    <row r="75" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="75" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G75">
         <v>1228.8979999999999</v>
       </c>
@@ -7627,7 +7627,7 @@
         <v>76.866280000000003</v>
       </c>
     </row>
-    <row r="76" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="76" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G76">
         <v>1244.1220000000001</v>
       </c>
@@ -7635,7 +7635,7 @@
         <v>76.297600000000003</v>
       </c>
     </row>
-    <row r="77" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="77" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G77">
         <v>1259.123</v>
       </c>
@@ -7643,7 +7643,7 @@
         <v>76.881839999999997</v>
       </c>
     </row>
-    <row r="78" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="78" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G78">
         <v>1258.752</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>76.468999999999994</v>
       </c>
     </row>
-    <row r="79" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="79" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G79">
         <v>1304.1369999999999</v>
       </c>
@@ -7659,7 +7659,7 @@
         <v>76.618129999999994</v>
       </c>
     </row>
-    <row r="80" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="80" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G80">
         <v>1349.9849999999999</v>
       </c>
@@ -7667,7 +7667,7 @@
         <v>76.480620000000002</v>
       </c>
     </row>
-    <row r="81" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="81" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G81">
         <v>1350.0229999999999</v>
       </c>
@@ -7675,7 +7675,7 @@
         <v>76.648570000000007</v>
       </c>
     </row>
-    <row r="82" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="82" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G82">
         <v>1364.8150000000001</v>
       </c>
@@ -7683,7 +7683,7 @@
         <v>76.311499999999995</v>
       </c>
     </row>
-    <row r="83" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="83" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G83">
         <v>1380.152</v>
       </c>
@@ -7691,7 +7691,7 @@
         <v>76.679150000000007</v>
       </c>
     </row>
-    <row r="84" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="84" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G84">
         <v>1380.086</v>
       </c>
@@ -7699,7 +7699,7 @@
         <v>76.621639999999999</v>
       </c>
     </row>
-    <row r="85" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="85" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G85">
         <v>1379.7149999999999</v>
       </c>
@@ -7707,7 +7707,7 @@
         <v>76.371279999999999</v>
       </c>
     </row>
-    <row r="86" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="86" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G86">
         <v>1394.9970000000001</v>
       </c>
@@ -7715,7 +7715,7 @@
         <v>76.636949999999999</v>
       </c>
     </row>
-    <row r="87" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="87" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G87">
         <v>1410.3409999999999</v>
       </c>
@@ -7723,7 +7723,7 @@
         <v>76.882059999999996</v>
       </c>
     </row>
-    <row r="88" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="88" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G88">
         <v>1425.6030000000001</v>
       </c>
@@ -7731,7 +7731,7 @@
         <v>76.91395</v>
       </c>
     </row>
-    <row r="89" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="89" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G89">
         <v>1409.979</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>76.394909999999996</v>
       </c>
     </row>
-    <row r="90" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="90" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G90">
         <v>1410.248</v>
       </c>
@@ -7747,7 +7747,7 @@
         <v>76.664580000000001</v>
       </c>
     </row>
-    <row r="91" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="91" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G91">
         <v>1455.58</v>
       </c>
@@ -7755,7 +7755,7 @@
         <v>76.792010000000005</v>
       </c>
     </row>
-    <row r="92" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="92" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G92">
         <v>1486.2159999999999</v>
       </c>
@@ -7763,7 +7763,7 @@
         <v>86.622889999999998</v>
       </c>
     </row>
-    <row r="93" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="93" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G93">
         <v>1485.806</v>
       </c>
@@ -7771,7 +7771,7 @@
         <v>86.426929999999999</v>
       </c>
     </row>
-    <row r="94" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="94" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G94">
         <v>1516.0709999999999</v>
       </c>
@@ -7779,7 +7779,7 @@
         <v>86.291049999999998</v>
       </c>
     </row>
-    <row r="95" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="95" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G95">
         <v>1515.9280000000001</v>
       </c>
@@ -7787,7 +7787,7 @@
         <v>86.616039999999998</v>
       </c>
     </row>
-    <row r="96" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="96" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G96">
         <v>1516.348</v>
       </c>
@@ -7795,7 +7795,7 @@
         <v>86.725769999999997</v>
       </c>
     </row>
-    <row r="97" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="97" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G97">
         <v>1531.32</v>
       </c>
@@ -7803,7 +7803,7 @@
         <v>86.364840000000001</v>
       </c>
     </row>
-    <row r="98" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="98" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G98">
         <v>1531.4570000000001</v>
       </c>
@@ -7811,7 +7811,7 @@
         <v>86.454610000000002</v>
       </c>
     </row>
-    <row r="99" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="99" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G99">
         <v>1531.6220000000001</v>
       </c>
@@ -7819,7 +7819,7 @@
         <v>86.403989999999993</v>
       </c>
     </row>
-    <row r="100" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="100" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G100">
         <v>1531.232</v>
       </c>
@@ -7827,7 +7827,7 @@
         <v>86.471239999999995</v>
       </c>
     </row>
-    <row r="101" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="101" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G101">
         <v>1531.4369999999999</v>
       </c>
@@ -7835,7 +7835,7 @@
         <v>86.733379999999997</v>
       </c>
     </row>
-    <row r="102" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="102" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G102">
         <v>1531.0519999999999</v>
       </c>
@@ -7843,7 +7843,7 @@
         <v>86.402079999999998</v>
       </c>
     </row>
-    <row r="103" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="103" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G103">
         <v>1531.268</v>
       </c>
@@ -7851,7 +7851,7 @@
         <v>86.439710000000005</v>
       </c>
     </row>
-    <row r="104" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="104" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G104">
         <v>1546.579</v>
       </c>
@@ -7859,7 +7859,7 @@
         <v>86.730919999999998</v>
       </c>
     </row>
-    <row r="105" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="105" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G105">
         <v>1546.319</v>
       </c>
@@ -7867,7 +7867,7 @@
         <v>86.136409999999998</v>
       </c>
     </row>
-    <row r="106" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="106" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G106">
         <v>1576.8009999999999</v>
       </c>
@@ -7875,7 +7875,7 @@
         <v>86.486429999999999</v>
       </c>
     </row>
-    <row r="107" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="107" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G107">
         <v>1591.886</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>86.408940000000001</v>
       </c>
     </row>
-    <row r="108" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="108" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G108">
         <v>1607.3309999999999</v>
       </c>
@@ -7891,7 +7891,7 @@
         <v>86.266360000000006</v>
       </c>
     </row>
-    <row r="109" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="109" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G109">
         <v>1607.1669999999999</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>96.321259999999995</v>
       </c>
     </row>
-    <row r="110" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="110" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G110">
         <v>1622.027</v>
       </c>
@@ -7907,7 +7907,7 @@
         <v>95.994619999999998</v>
       </c>
     </row>
-    <row r="111" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="111" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G111">
         <v>1622.26</v>
       </c>
@@ -7915,7 +7915,7 @@
         <v>96.47484</v>
       </c>
     </row>
-    <row r="112" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="112" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G112">
         <v>1637.01</v>
       </c>
@@ -7923,7 +7923,7 @@
         <v>96.487459999999999</v>
       </c>
     </row>
-    <row r="113" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="113" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G113">
         <v>1637.1120000000001</v>
       </c>
@@ -7931,7 +7931,7 @@
         <v>95.942539999999994</v>
       </c>
     </row>
-    <row r="114" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="114" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G114">
         <v>1652.441</v>
       </c>
@@ -7939,7 +7939,7 @@
         <v>96.212249999999997</v>
       </c>
     </row>
-    <row r="115" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="115" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G115">
         <v>1652.6880000000001</v>
       </c>
@@ -7947,7 +7947,7 @@
         <v>96.16</v>
       </c>
     </row>
-    <row r="116" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="116" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G116">
         <v>1652.4690000000001</v>
       </c>
@@ -7955,7 +7955,7 @@
         <v>96.532060000000001</v>
       </c>
     </row>
-    <row r="117" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="117" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G117">
         <v>1667.163</v>
       </c>
@@ -7963,7 +7963,7 @@
         <v>96.261859999999999</v>
       </c>
     </row>
-    <row r="118" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="118" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G118">
         <v>1682.24</v>
       </c>
@@ -7971,7 +7971,7 @@
         <v>96.204570000000004</v>
       </c>
     </row>
-    <row r="119" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="119" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G119">
         <v>1682.7049999999999</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>95.947130000000001</v>
       </c>
     </row>
-    <row r="120" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="120" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G120">
         <v>1697.7449999999999</v>
       </c>
@@ -7987,7 +7987,7 @@
         <v>102.5564</v>
       </c>
     </row>
-    <row r="121" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="121" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G121">
         <v>1697.4570000000001</v>
       </c>
@@ -7995,7 +7995,7 @@
         <v>96.26979</v>
       </c>
     </row>
-    <row r="122" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="122" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G122">
         <v>1697.8979999999999</v>
       </c>
@@ -8003,7 +8003,7 @@
         <v>107.5222</v>
       </c>
     </row>
-    <row r="123" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="123" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G123">
         <v>1713.067</v>
       </c>
@@ -8011,7 +8011,7 @@
         <v>96.174220000000005</v>
       </c>
     </row>
-    <row r="124" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="124" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G124">
         <v>1713.4069999999999</v>
       </c>
@@ -8019,7 +8019,7 @@
         <v>111.3181</v>
       </c>
     </row>
-    <row r="125" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="125" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G125">
         <v>1713.269</v>
       </c>
@@ -8027,7 +8027,7 @@
         <v>96.214839999999995</v>
       </c>
     </row>
-    <row r="126" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="126" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G126">
         <v>1742.9939999999999</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>122.13800000000001</v>
       </c>
     </row>
-    <row r="127" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="127" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G127">
         <v>1773.7049999999999</v>
       </c>
@@ -8043,7 +8043,7 @@
         <v>105.7696</v>
       </c>
     </row>
-    <row r="128" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="128" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G128">
         <v>1788.712</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>106.3018</v>
       </c>
     </row>
-    <row r="129" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="129" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G129">
         <v>1803.973</v>
       </c>
@@ -8059,7 +8059,7 @@
         <v>106.0164</v>
       </c>
     </row>
-    <row r="130" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="130" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G130">
         <v>1803.799</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>106.0008</v>
       </c>
     </row>
-    <row r="131" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="131" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G131">
         <v>1788.7460000000001</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>106.2757</v>
       </c>
     </row>
-    <row r="132" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="132" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G132">
         <v>1803.846</v>
       </c>
@@ -8083,7 +8083,7 @@
         <v>105.7705</v>
       </c>
     </row>
-    <row r="133" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="133" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G133">
         <v>1788.356</v>
       </c>
@@ -8091,7 +8091,7 @@
         <v>106.0813</v>
       </c>
     </row>
-    <row r="134" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="134" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G134">
         <v>1773.8130000000001</v>
       </c>
@@ -8099,7 +8099,7 @@
         <v>106.3004</v>
       </c>
     </row>
-    <row r="135" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="135" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G135">
         <v>1773.46</v>
       </c>
@@ -8107,7 +8107,7 @@
         <v>105.8387</v>
       </c>
     </row>
-    <row r="136" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="136" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G136">
         <v>1773.855</v>
       </c>
@@ -8115,7 +8115,7 @@
         <v>106.3312</v>
       </c>
     </row>
-    <row r="137" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="137" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G137">
         <v>1758.252</v>
       </c>
@@ -8123,7 +8123,7 @@
         <v>105.94289999999999</v>
       </c>
     </row>
-    <row r="138" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="138" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G138">
         <v>1758.42</v>
       </c>
@@ -8131,7 +8131,7 @@
         <v>105.88379999999999</v>
       </c>
     </row>
-    <row r="139" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="139" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G139">
         <v>1743.6389999999999</v>
       </c>
@@ -8139,7 +8139,7 @@
         <v>105.9689</v>
       </c>
     </row>
-    <row r="140" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="140" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G140">
         <v>1743.116</v>
       </c>
@@ -8147,7 +8147,7 @@
         <v>106.07550000000001</v>
       </c>
     </row>
-    <row r="141" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="141" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G141">
         <v>1743.41</v>
       </c>
@@ -8155,7 +8155,7 @@
         <v>105.9944</v>
       </c>
     </row>
-    <row r="142" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="142" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G142">
         <v>1758.229</v>
       </c>
@@ -8163,7 +8163,7 @@
         <v>105.9682</v>
       </c>
     </row>
-    <row r="143" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="143" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G143">
         <v>1758.6110000000001</v>
       </c>
@@ -8171,7 +8171,7 @@
         <v>106.0844</v>
       </c>
     </row>
-    <row r="144" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="144" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G144">
         <v>1758.502</v>
       </c>
@@ -8179,7 +8179,7 @@
         <v>106.253</v>
       </c>
     </row>
-    <row r="145" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="145" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G145">
         <v>1758.336</v>
       </c>
@@ -8187,7 +8187,7 @@
         <v>105.9712</v>
       </c>
     </row>
-    <row r="146" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="146" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G146">
         <v>1743.46</v>
       </c>
@@ -8195,7 +8195,7 @@
         <v>105.7208</v>
       </c>
     </row>
-    <row r="147" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="147" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G147">
         <v>1743.7249999999999</v>
       </c>
@@ -8203,7 +8203,7 @@
         <v>106.00369999999999</v>
       </c>
     </row>
-    <row r="148" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="148" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G148">
         <v>1743.2550000000001</v>
       </c>
@@ -8211,7 +8211,7 @@
         <v>105.74850000000001</v>
       </c>
     </row>
-    <row r="149" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="149" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G149">
         <v>1743.2</v>
       </c>
@@ -8219,7 +8219,7 @@
         <v>105.6892</v>
       </c>
     </row>
-    <row r="150" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="150" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G150">
         <v>1743.645</v>
       </c>
@@ -8227,7 +8227,7 @@
         <v>115.9367</v>
       </c>
     </row>
-    <row r="151" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="151" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G151">
         <v>1743.6010000000001</v>
       </c>
@@ -8235,7 +8235,7 @@
         <v>115.7723</v>
       </c>
     </row>
-    <row r="152" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="152" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G152">
         <v>1743.2650000000001</v>
       </c>
@@ -8243,7 +8243,7 @@
         <v>115.5065</v>
       </c>
     </row>
-    <row r="153" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="153" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G153">
         <v>1743.1210000000001</v>
       </c>
@@ -8251,7 +8251,7 @@
         <v>116.05670000000001</v>
       </c>
     </row>
-    <row r="154" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="154" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G154">
         <v>1743.5830000000001</v>
       </c>
@@ -8259,7 +8259,7 @@
         <v>115.9269</v>
       </c>
     </row>
-    <row r="155" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="155" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G155">
         <v>1743.1949999999999</v>
       </c>
@@ -8267,7 +8267,7 @@
         <v>115.9965</v>
       </c>
     </row>
-    <row r="156" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="156" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G156">
         <v>1758.404</v>
       </c>
@@ -8275,7 +8275,7 @@
         <v>115.4991</v>
       </c>
     </row>
-    <row r="157" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="157" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G157">
         <v>1743.6780000000001</v>
       </c>
@@ -8283,7 +8283,7 @@
         <v>115.5228</v>
       </c>
     </row>
-    <row r="158" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="158" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G158">
         <v>1743.75</v>
       </c>
@@ -8291,7 +8291,7 @@
         <v>115.83710000000001</v>
       </c>
     </row>
-    <row r="159" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="159" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G159">
         <v>1743.4010000000001</v>
       </c>
@@ -8299,7 +8299,7 @@
         <v>115.67700000000001</v>
       </c>
     </row>
-    <row r="160" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="160" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G160">
         <v>1758.3130000000001</v>
       </c>
@@ -8307,7 +8307,7 @@
         <v>115.5472</v>
       </c>
     </row>
-    <row r="161" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="161" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G161">
         <v>1758.4659999999999</v>
       </c>
@@ -8315,7 +8315,7 @@
         <v>116.02809999999999</v>
       </c>
     </row>
-    <row r="162" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="162" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G162">
         <v>1758.309</v>
       </c>
@@ -8323,7 +8323,7 @@
         <v>115.7191</v>
       </c>
     </row>
-    <row r="163" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="163" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G163">
         <v>1758.383</v>
       </c>
@@ -8331,7 +8331,7 @@
         <v>115.8503</v>
       </c>
     </row>
-    <row r="164" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="164" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G164">
         <v>1758.7819999999999</v>
       </c>
@@ -8339,7 +8339,7 @@
         <v>116.01349999999999</v>
       </c>
     </row>
-    <row r="165" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="165" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G165">
         <v>1788.462</v>
       </c>
@@ -8347,7 +8347,7 @@
         <v>116.0718</v>
       </c>
     </row>
-    <row r="166" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="166" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G166">
         <v>1804.0540000000001</v>
       </c>
@@ -8355,7 +8355,7 @@
         <v>115.88200000000001</v>
       </c>
     </row>
-    <row r="167" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="167" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G167">
         <v>1804.001</v>
       </c>
@@ -8363,7 +8363,7 @@
         <v>115.82640000000001</v>
       </c>
     </row>
-    <row r="168" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="168" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G168">
         <v>1818.5730000000001</v>
       </c>
@@ -8371,7 +8371,7 @@
         <v>116.0414</v>
       </c>
     </row>
-    <row r="169" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="169" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G169">
         <v>1818.624</v>
       </c>
@@ -8379,7 +8379,7 @@
         <v>115.7786</v>
       </c>
     </row>
-    <row r="170" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="170" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G170">
         <v>1818.7860000000001</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>115.92440000000001</v>
       </c>
     </row>
-    <row r="171" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="171" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G171">
         <v>1834.075</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>116.0988</v>
       </c>
     </row>
-    <row r="172" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="172" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G172">
         <v>1834.6020000000001</v>
       </c>
@@ -8403,7 +8403,7 @@
         <v>115.9281</v>
       </c>
     </row>
-    <row r="173" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="173" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G173">
         <v>1834.0730000000001</v>
       </c>
@@ -8411,7 +8411,7 @@
         <v>115.8377</v>
       </c>
     </row>
-    <row r="174" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="174" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G174">
         <v>1834.4480000000001</v>
       </c>
@@ -8419,7 +8419,7 @@
         <v>116.0936</v>
       </c>
     </row>
-    <row r="175" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="175" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G175">
         <v>1834.4960000000001</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>115.8402</v>
       </c>
     </row>
-    <row r="176" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="176" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G176">
         <v>1849.4380000000001</v>
       </c>
@@ -8435,7 +8435,7 @@
         <v>116.17019999999999</v>
       </c>
     </row>
-    <row r="177" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="177" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G177">
         <v>1864.201</v>
       </c>
@@ -8443,7 +8443,7 @@
         <v>115.6253</v>
       </c>
     </row>
-    <row r="178" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="178" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G178">
         <v>1864.7149999999999</v>
       </c>
@@ -8451,7 +8451,7 @@
         <v>116.0719</v>
       </c>
     </row>
-    <row r="179" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="179" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G179">
         <v>1879.3689999999999</v>
       </c>
@@ -8459,7 +8459,7 @@
         <v>116.3058</v>
       </c>
     </row>
-    <row r="180" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="180" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G180">
         <v>1894.5129999999999</v>
       </c>
@@ -8467,7 +8467,7 @@
         <v>115.8853</v>
       </c>
     </row>
-    <row r="181" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="181" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G181">
         <v>1894.61</v>
       </c>
@@ -8475,7 +8475,7 @@
         <v>116.38339999999999</v>
       </c>
     </row>
-    <row r="182" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="182" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G182">
         <v>1895.0039999999999</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>116.1009</v>
       </c>
     </row>
-    <row r="183" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="183" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G183">
         <v>1909.9960000000001</v>
       </c>
@@ -8491,7 +8491,7 @@
         <v>126.40130000000001</v>
       </c>
     </row>
-    <row r="184" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="184" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G184">
         <v>1909.953</v>
       </c>
@@ -8499,7 +8499,7 @@
         <v>115.6763</v>
       </c>
     </row>
-    <row r="185" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="185" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G185">
         <v>1909.9480000000001</v>
       </c>
@@ -8507,7 +8507,7 @@
         <v>128.953</v>
       </c>
     </row>
-    <row r="186" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="186" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G186">
         <v>1925.124</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>115.9194</v>
       </c>
     </row>
-    <row r="187" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="187" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G187">
         <v>1924.905</v>
       </c>
@@ -8523,7 +8523,7 @@
         <v>131.6455</v>
       </c>
     </row>
-    <row r="188" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="188" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G188">
         <v>1939.692</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>115.86109999999999</v>
       </c>
     </row>
-    <row r="189" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="189" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G189">
         <v>1939.9169999999999</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>115.68819999999999</v>
       </c>
     </row>
-    <row r="190" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="190" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G190">
         <v>1955.596</v>
       </c>
@@ -8547,7 +8547,7 @@
         <v>116.19329999999999</v>
       </c>
     </row>
-    <row r="191" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="191" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G191">
         <v>1970.683</v>
       </c>
@@ -8555,7 +8555,7 @@
         <v>116.134</v>
       </c>
     </row>
-    <row r="192" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="192" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G192">
         <v>1970.617</v>
       </c>
@@ -8563,7 +8563,7 @@
         <v>116.1763</v>
       </c>
     </row>
-    <row r="193" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="193" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G193">
         <v>1970.1420000000001</v>
       </c>
@@ -8571,7 +8571,7 @@
         <v>116.0438</v>
       </c>
     </row>
-    <row r="194" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="194" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G194">
         <v>1985.317</v>
       </c>
@@ -8579,7 +8579,7 @@
         <v>115.9259</v>
       </c>
     </row>
-    <row r="195" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="195" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G195">
         <v>1985.1020000000001</v>
       </c>
@@ -8587,7 +8587,7 @@
         <v>116.0008</v>
       </c>
     </row>
-    <row r="196" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="196" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G196">
         <v>2000.7739999999999</v>
       </c>
@@ -8595,7 +8595,7 @@
         <v>116.0121</v>
       </c>
     </row>
-    <row r="197" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="197" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G197">
         <v>2000.3019999999999</v>
       </c>
@@ -8603,7 +8603,7 @@
         <v>115.7264</v>
       </c>
     </row>
-    <row r="198" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="198" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G198">
         <v>2015.693</v>
       </c>
@@ -8611,7 +8611,7 @@
         <v>115.9374</v>
       </c>
     </row>
-    <row r="199" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="199" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G199">
         <v>2030.57</v>
       </c>
@@ -8619,7 +8619,7 @@
         <v>115.91459999999999</v>
       </c>
     </row>
-    <row r="200" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="200" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G200">
         <v>2046.1120000000001</v>
       </c>
@@ -8627,7 +8627,7 @@
         <v>115.63939999999999</v>
       </c>
     </row>
-    <row r="201" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="201" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G201">
         <v>2076.0819999999999</v>
       </c>
@@ -8635,7 +8635,7 @@
         <v>116.1581</v>
       </c>
     </row>
-    <row r="202" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="202" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G202">
         <v>2091.7159999999999</v>
       </c>
@@ -8643,7 +8643,7 @@
         <v>115.8416</v>
       </c>
     </row>
-    <row r="203" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="203" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G203">
         <v>2106.19</v>
       </c>
@@ -8651,7 +8651,7 @@
         <v>115.8566</v>
       </c>
     </row>
-    <row r="204" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="204" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G204">
         <v>2106.2840000000001</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>115.8509</v>
       </c>
     </row>
-    <row r="205" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="205" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G205">
         <v>2121.7220000000002</v>
       </c>
@@ -8667,7 +8667,7 @@
         <v>115.8514</v>
       </c>
     </row>
-    <row r="206" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="206" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G206">
         <v>2136.712</v>
       </c>
@@ -8675,7 +8675,7 @@
         <v>125.86709999999999</v>
       </c>
     </row>
-    <row r="207" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="207" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G207">
         <v>2136.752</v>
       </c>
@@ -8683,7 +8683,7 @@
         <v>125.4483</v>
       </c>
     </row>
-    <row r="208" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="208" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G208">
         <v>2136.913</v>
       </c>
@@ -8691,7 +8691,7 @@
         <v>125.4024</v>
       </c>
     </row>
-    <row r="209" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="209" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G209">
         <v>2167.261</v>
       </c>
@@ -8699,7 +8699,7 @@
         <v>125.7238</v>
       </c>
     </row>
-    <row r="210" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="210" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G210">
         <v>2181.7249999999999</v>
       </c>
@@ -8707,7 +8707,7 @@
         <v>125.682</v>
       </c>
     </row>
-    <row r="211" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="211" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G211">
         <v>2182.0329999999999</v>
       </c>
@@ -8715,7 +8715,7 @@
         <v>125.6857</v>
       </c>
     </row>
-    <row r="212" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="212" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G212">
         <v>2197.1640000000002</v>
       </c>
@@ -8723,7 +8723,7 @@
         <v>125.4738</v>
       </c>
     </row>
-    <row r="213" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="213" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G213">
         <v>2212.6770000000001</v>
       </c>
@@ -8731,7 +8731,7 @@
         <v>125.9331</v>
       </c>
     </row>
-    <row r="214" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="214" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G214">
         <v>2227.3980000000001</v>
       </c>
@@ -8739,7 +8739,7 @@
         <v>125.37139999999999</v>
       </c>
     </row>
-    <row r="215" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="215" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G215">
         <v>2242.422</v>
       </c>
@@ -8747,7 +8747,7 @@
         <v>125.9153</v>
       </c>
     </row>
-    <row r="216" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="216" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G216">
         <v>2257.8890000000001</v>
       </c>
@@ -8755,7 +8755,7 @@
         <v>125.6576</v>
       </c>
     </row>
-    <row r="217" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="217" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G217">
         <v>2272.59</v>
       </c>
@@ -8763,7 +8763,7 @@
         <v>125.5729</v>
       </c>
     </row>
-    <row r="218" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="218" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G218">
         <v>2288.2159999999999</v>
       </c>
@@ -8771,7 +8771,7 @@
         <v>125.9589</v>
       </c>
     </row>
-    <row r="219" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="219" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G219">
         <v>2302.7950000000001</v>
       </c>
@@ -8779,7 +8779,7 @@
         <v>135.2037</v>
       </c>
     </row>
-    <row r="220" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="220" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G220">
         <v>2318.6460000000002</v>
       </c>
@@ -8787,7 +8787,7 @@
         <v>135.52789999999999</v>
       </c>
     </row>
-    <row r="221" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="221" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G221">
         <v>2333.2890000000002</v>
       </c>
@@ -8795,7 +8795,7 @@
         <v>135.4736</v>
       </c>
     </row>
-    <row r="222" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="222" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G222">
         <v>2348.8989999999999</v>
       </c>
@@ -8803,7 +8803,7 @@
         <v>135.52209999999999</v>
       </c>
     </row>
-    <row r="223" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="223" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G223">
         <v>2363.453</v>
       </c>
@@ -8811,7 +8811,7 @@
         <v>135.203</v>
       </c>
     </row>
-    <row r="224" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="224" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G224">
         <v>2379.2429999999999</v>
       </c>
@@ -8819,7 +8819,7 @@
         <v>135.62870000000001</v>
       </c>
     </row>
-    <row r="225" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="225" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G225">
         <v>2378.7959999999998</v>
       </c>
@@ -8827,7 +8827,7 @@
         <v>135.7516</v>
       </c>
     </row>
-    <row r="226" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="226" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G226">
         <v>2379.1619999999998</v>
       </c>
@@ -8835,7 +8835,7 @@
         <v>135.196</v>
       </c>
     </row>
-    <row r="227" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="227" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G227">
         <v>2363.471</v>
       </c>
@@ -8843,7 +8843,7 @@
         <v>135.72149999999999</v>
       </c>
     </row>
-    <row r="228" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="228" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G228">
         <v>2318.3110000000001</v>
       </c>
@@ -8851,7 +8851,7 @@
         <v>135.15219999999999</v>
       </c>
     </row>
-    <row r="229" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="229" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G229">
         <v>2303.3679999999999</v>
       </c>
@@ -8859,7 +8859,7 @@
         <v>135.52850000000001</v>
       </c>
     </row>
-    <row r="230" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="230" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G230">
         <v>2303.4119999999998</v>
       </c>
@@ -8867,7 +8867,7 @@
         <v>135.50040000000001</v>
       </c>
     </row>
-    <row r="231" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="231" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G231">
         <v>2272.797</v>
       </c>
@@ -8875,7 +8875,7 @@
         <v>135.14279999999999</v>
       </c>
     </row>
-    <row r="232" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="232" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G232">
         <v>2257.855</v>
       </c>
@@ -8883,7 +8883,7 @@
         <v>135.7586</v>
       </c>
     </row>
-    <row r="233" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="233" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G233">
         <v>2257.732</v>
       </c>
@@ -8891,7 +8891,7 @@
         <v>135.2062</v>
       </c>
     </row>
-    <row r="234" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="234" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G234">
         <v>2243.0100000000002</v>
       </c>
@@ -8899,7 +8899,7 @@
         <v>135.19049999999999</v>
       </c>
     </row>
-    <row r="235" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="235" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G235">
         <v>2227.8380000000002</v>
       </c>
@@ -8907,7 +8907,7 @@
         <v>135.5018</v>
       </c>
     </row>
-    <row r="236" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="236" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G236">
         <v>2227.8609999999999</v>
       </c>
@@ -8915,7 +8915,7 @@
         <v>135.70230000000001</v>
       </c>
     </row>
-    <row r="237" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="237" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G237">
         <v>2227.7280000000001</v>
       </c>
@@ -8923,7 +8923,7 @@
         <v>135.14320000000001</v>
       </c>
     </row>
-    <row r="238" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="238" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G238">
         <v>2212.5929999999998</v>
       </c>
@@ -8931,7 +8931,7 @@
         <v>135.9186</v>
       </c>
     </row>
-    <row r="239" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="239" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G239">
         <v>2212.4630000000002</v>
       </c>
@@ -8939,7 +8939,7 @@
         <v>135.1687</v>
       </c>
     </row>
-    <row r="240" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="240" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G240">
         <v>2197.69</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>136.13910000000001</v>
       </c>
     </row>
-    <row r="241" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="241" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G241">
         <v>2197.442</v>
       </c>
@@ -8955,7 +8955,7 @@
         <v>135.43340000000001</v>
       </c>
     </row>
-    <row r="242" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="242" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G242">
         <v>2197.8220000000001</v>
       </c>
@@ -8963,7 +8963,7 @@
         <v>146.0427</v>
       </c>
     </row>
-    <row r="243" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="243" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G243">
         <v>2181.6410000000001</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v>135.41380000000001</v>
       </c>
     </row>
-    <row r="244" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="244" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G244">
         <v>2181.77</v>
       </c>
@@ -8979,7 +8979,7 @@
         <v>148.27549999999999</v>
       </c>
     </row>
-    <row r="245" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="245" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G245">
         <v>2182.2109999999998</v>
       </c>
@@ -8987,7 +8987,7 @@
         <v>135.7269</v>
       </c>
     </row>
-    <row r="246" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="246" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G246">
         <v>2166.9209999999998</v>
       </c>
@@ -8995,7 +8995,7 @@
         <v>150.4016</v>
       </c>
     </row>
-    <row r="247" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="247" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G247">
         <v>2167.4630000000002</v>
       </c>
@@ -9003,7 +9003,7 @@
         <v>135.68629999999999</v>
       </c>
     </row>
-    <row r="248" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="248" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G248">
         <v>2166.9349999999999</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>149.3246</v>
       </c>
     </row>
-    <row r="249" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="249" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G249">
         <v>2152.0659999999998</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>135.16829999999999</v>
       </c>
     </row>
-    <row r="250" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="250" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G250">
         <v>2151.8969999999999</v>
       </c>
@@ -9027,7 +9027,7 @@
         <v>135.63730000000001</v>
       </c>
     </row>
-    <row r="251" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="251" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G251">
         <v>2151.701</v>
       </c>
@@ -9035,7 +9035,7 @@
         <v>135.42089999999999</v>
       </c>
     </row>
-    <row r="252" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="252" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G252">
         <v>2152.1179999999999</v>
       </c>
@@ -9043,7 +9043,7 @@
         <v>135.44110000000001</v>
       </c>
     </row>
-    <row r="253" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="253" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G253">
         <v>2137.1120000000001</v>
       </c>
@@ -9051,7 +9051,7 @@
         <v>135.73140000000001</v>
       </c>
     </row>
-    <row r="254" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="254" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G254">
         <v>2152.1480000000001</v>
       </c>
@@ -9059,7 +9059,7 @@
         <v>135.52979999999999</v>
       </c>
     </row>
-    <row r="255" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="255" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G255">
         <v>2136.7139999999999</v>
       </c>
@@ -9067,7 +9067,7 @@
         <v>135.16589999999999</v>
       </c>
     </row>
-    <row r="256" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="256" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G256">
         <v>2136.7220000000002</v>
       </c>
@@ -9075,7 +9075,7 @@
         <v>135.43109999999999</v>
       </c>
     </row>
-    <row r="257" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="257" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G257">
         <v>2137.1190000000001</v>
       </c>
@@ -9083,7 +9083,7 @@
         <v>135.6944</v>
       </c>
     </row>
-    <row r="258" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="258" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G258">
         <v>2137.2060000000001</v>
       </c>
@@ -9091,7 +9091,7 @@
         <v>135.5111</v>
       </c>
     </row>
-    <row r="259" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="259" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G259">
         <v>2137.136</v>
       </c>
@@ -9099,7 +9099,7 @@
         <v>135.74529999999999</v>
       </c>
     </row>
-    <row r="260" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="260" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G260">
         <v>2136.998</v>
       </c>
@@ -9107,7 +9107,7 @@
         <v>135.589</v>
       </c>
     </row>
-    <row r="261" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="261" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G261">
         <v>2137.0430000000001</v>
       </c>
@@ -9115,7 +9115,7 @@
         <v>135.4787</v>
       </c>
     </row>
-    <row r="262" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="262" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G262">
         <v>2136.9940000000001</v>
       </c>
@@ -9123,7 +9123,7 @@
         <v>135.501</v>
       </c>
     </row>
-    <row r="263" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="263" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G263">
         <v>2151.7600000000002</v>
       </c>
@@ -9131,7 +9131,7 @@
         <v>135.68340000000001</v>
       </c>
     </row>
-    <row r="264" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="264" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G264">
         <v>2136.674</v>
       </c>
@@ -9139,7 +9139,7 @@
         <v>135.40479999999999</v>
       </c>
     </row>
-    <row r="265" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="265" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G265">
         <v>2151.973</v>
       </c>
@@ -9147,7 +9147,7 @@
         <v>135.34440000000001</v>
       </c>
     </row>
-    <row r="266" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="266" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G266">
         <v>2151.9319999999998</v>
       </c>
@@ -9155,7 +9155,7 @@
         <v>135.4581</v>
       </c>
     </row>
-    <row r="267" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="267" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G267">
         <v>2151.9209999999998</v>
       </c>
@@ -9163,7 +9163,7 @@
         <v>135.1977</v>
       </c>
     </row>
-    <row r="268" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="268" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G268">
         <v>2151.9989999999998</v>
       </c>
@@ -9171,7 +9171,7 @@
         <v>135.34399999999999</v>
       </c>
     </row>
-    <row r="269" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="269" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G269">
         <v>2166.6460000000002</v>
       </c>
@@ -9179,7 +9179,7 @@
         <v>135.76349999999999</v>
       </c>
     </row>
-    <row r="270" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="270" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G270">
         <v>2152.134</v>
       </c>
@@ -9187,7 +9187,7 @@
         <v>135.49199999999999</v>
       </c>
     </row>
-    <row r="271" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="271" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G271">
         <v>2167.125</v>
       </c>
@@ -9195,7 +9195,7 @@
         <v>135.47919999999999</v>
       </c>
     </row>
-    <row r="272" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="272" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G272">
         <v>2166.8739999999998</v>
       </c>
@@ -9203,7 +9203,7 @@
         <v>135.7834</v>
       </c>
     </row>
-    <row r="273" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="273" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G273">
         <v>2182.17</v>
       </c>
@@ -9211,7 +9211,7 @@
         <v>135.50450000000001</v>
       </c>
     </row>
-    <row r="274" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="274" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G274">
         <v>2182.067</v>
       </c>
@@ -9219,7 +9219,7 @@
         <v>135.22200000000001</v>
       </c>
     </row>
-    <row r="275" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="275" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G275">
         <v>2197.5309999999999</v>
       </c>
@@ -9227,7 +9227,7 @@
         <v>135.49209999999999</v>
       </c>
     </row>
-    <row r="276" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="276" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G276">
         <v>2197.299</v>
       </c>
@@ -9235,7 +9235,7 @@
         <v>135.19800000000001</v>
       </c>
     </row>
-    <row r="277" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="277" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G277">
         <v>2212.5549999999998</v>
       </c>
@@ -9243,7 +9243,7 @@
         <v>135.47669999999999</v>
       </c>
     </row>
-    <row r="278" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="278" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G278">
         <v>2227.5909999999999</v>
       </c>
@@ -9251,7 +9251,7 @@
         <v>135.24359999999999</v>
       </c>
     </row>
-    <row r="279" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="279" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G279">
         <v>2242.674</v>
       </c>
@@ -9259,7 +9259,7 @@
         <v>135.78200000000001</v>
       </c>
     </row>
-    <row r="280" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="280" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G280">
         <v>2242.6320000000001</v>
       </c>
@@ -9267,7 +9267,7 @@
         <v>135.61869999999999</v>
       </c>
     </row>
-    <row r="281" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="281" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G281">
         <v>2257.8119999999999</v>
       </c>
@@ -9275,7 +9275,7 @@
         <v>135.5112</v>
       </c>
     </row>
-    <row r="282" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="282" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G282">
         <v>2257.9879999999998</v>
       </c>
@@ -9283,7 +9283,7 @@
         <v>135.25960000000001</v>
       </c>
     </row>
-    <row r="283" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="283" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G283">
         <v>2273.31</v>
       </c>
@@ -9291,7 +9291,7 @@
         <v>135.57429999999999</v>
       </c>
     </row>
-    <row r="284" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="284" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G284">
         <v>2272.7620000000002</v>
       </c>
@@ -9299,7 +9299,7 @@
         <v>135.48140000000001</v>
       </c>
     </row>
-    <row r="285" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="285" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G285">
         <v>2272.7910000000002</v>
       </c>
@@ -9307,7 +9307,7 @@
         <v>135.24860000000001</v>
       </c>
     </row>
-    <row r="286" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="286" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G286">
         <v>2303.0889999999999</v>
       </c>
@@ -9315,7 +9315,7 @@
         <v>135.2543</v>
       </c>
     </row>
-    <row r="287" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="287" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G287">
         <v>2318.8209999999999</v>
       </c>
@@ -9323,7 +9323,7 @@
         <v>135.78460000000001</v>
       </c>
     </row>
-    <row r="288" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="288" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G288">
         <v>2334.0030000000002</v>
       </c>
@@ -9331,7 +9331,7 @@
         <v>135.56190000000001</v>
       </c>
     </row>
-    <row r="289" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="289" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G289">
         <v>2348.922</v>
       </c>
@@ -9339,7 +9339,7 @@
         <v>135.61609999999999</v>
       </c>
     </row>
-    <row r="290" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="290" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G290">
         <v>2348.8249999999998</v>
       </c>
@@ -9347,7 +9347,7 @@
         <v>135.52010000000001</v>
       </c>
     </row>
-    <row r="291" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="291" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G291">
         <v>2348.7159999999999</v>
       </c>
@@ -9355,7 +9355,7 @@
         <v>135.76300000000001</v>
       </c>
     </row>
-    <row r="292" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="292" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G292">
         <v>2363.6129999999998</v>
       </c>
@@ -9363,7 +9363,7 @@
         <v>135.53290000000001</v>
       </c>
     </row>
-    <row r="293" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="293" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G293">
         <v>2378.8510000000001</v>
       </c>
@@ -9371,7 +9371,7 @@
         <v>135.28210000000001</v>
       </c>
     </row>
-    <row r="294" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="294" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G294">
         <v>2379.19</v>
       </c>
@@ -9379,7 +9379,7 @@
         <v>135.48609999999999</v>
       </c>
     </row>
-    <row r="295" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="295" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G295">
         <v>2394.2730000000001</v>
       </c>
@@ -9387,7 +9387,7 @@
         <v>135.55950000000001</v>
       </c>
     </row>
-    <row r="296" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="296" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G296">
         <v>2393.9299999999998</v>
       </c>
@@ -9395,7 +9395,7 @@
         <v>135.2533</v>
       </c>
     </row>
-    <row r="297" spans="7:8" x14ac:dyDescent="0.75">
+    <row r="297" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G297">
         <v>2394.2550000000001</v>
       </c>
@@ -9410,11 +9410,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0ed78115-f4df-42b0-9376-ad3306022cc8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9671,27 +9672,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0ed78115-f4df-42b0-9376-ad3306022cc8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE3CDB75-004F-4418-A9D1-0A5E1B428212}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7D38091-7891-4922-BDA4-DDCC3109030A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="0ed78115-f4df-42b0-9376-ad3306022cc8"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="94b7f148-c09a-42e6-baca-973a9a7cd962"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9716,9 +9707,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7D38091-7891-4922-BDA4-DDCC3109030A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE3CDB75-004F-4418-A9D1-0A5E1B428212}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="0ed78115-f4df-42b0-9376-ad3306022cc8"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="94b7f148-c09a-42e6-baca-973a9a7cd962"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
shimadzue results from august field days
</commit_message>
<xml_diff>
--- a/01_Raw_data/RC log.xlsx
+++ b/01_Raw_data/RC log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samanthahowley\Desktop\Howley_Bradford_Streams\01_Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F448DC-2539-4B78-B8C8-DAFF8735B261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59D8DCE-C860-4E09-8A36-BE178A97DF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A079E74B-2391-4069-81A1-6515CCD90540}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{A079E74B-2391-4069-81A1-6515CCD90540}"/>
   </bookViews>
   <sheets>
     <sheet name="RC log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -46,12 +46,6 @@
   </si>
   <si>
     <t>Site</t>
-  </si>
-  <si>
-    <t>WT to Well</t>
-  </si>
-  <si>
-    <t>WTdepth</t>
   </si>
   <si>
     <t>pH</t>
@@ -136,6 +130,12 @@
   </si>
   <si>
     <t>CO2_mv</t>
+  </si>
+  <si>
+    <t>WT to Well (m)</t>
+  </si>
+  <si>
+    <t>Wtdepth (m)</t>
   </si>
 </sst>
 </file>
@@ -3685,17 +3685,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04E7760-F87C-4D84-A63F-D473D279D553}">
-  <dimension ref="A1:K97"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G103" sqref="G103:G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3713,25 +3714,25 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3745,16 +3746,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>0.2</v>
+        <v>6</v>
       </c>
       <c r="F2">
         <v>1.54</v>
       </c>
       <c r="G2">
-        <f>E2-F2</f>
+        <f>Sheet1!E2-'RC log'!F2</f>
         <v>-1.34</v>
       </c>
       <c r="H2">
@@ -3775,16 +3773,13 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>0.42</v>
+        <v>7</v>
       </c>
       <c r="F3">
         <v>1.47</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G66" si="0">E3-F3</f>
+        <f>Sheet1!E3-'RC log'!F3</f>
         <v>-1.05</v>
       </c>
       <c r="H3">
@@ -3805,16 +3800,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>0.755</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>1.25</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E4-'RC log'!F4</f>
         <v>-0.495</v>
       </c>
       <c r="H4">
@@ -3835,16 +3827,13 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>0.24</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>1.63</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E5-'RC log'!F5</f>
         <v>-1.39</v>
       </c>
       <c r="H5">
@@ -3865,16 +3854,13 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>0.75</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>0.86</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E6-'RC log'!F6</f>
         <v>-0.10999999999999999</v>
       </c>
       <c r="H6">
@@ -3895,20 +3881,17 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7">
-        <v>7.0000000000000007E-2</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>1.33</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E7-'RC log'!F7</f>
         <v>-1.26</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K7">
         <v>26</v>
@@ -3925,20 +3908,17 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E8-'RC log'!F8</f>
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K8">
         <v>26</v>
@@ -3955,16 +3935,13 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9">
-        <v>0.08</v>
+        <v>14</v>
       </c>
       <c r="F9">
         <v>1.1299999999999999</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E9-'RC log'!F9</f>
         <v>-1.0499999999999998</v>
       </c>
       <c r="H9">
@@ -3985,16 +3962,13 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10">
-        <v>0.84</v>
+        <v>15</v>
       </c>
       <c r="F10">
         <v>0.82</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E10-'RC log'!F10</f>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="H10">
@@ -4015,16 +3989,13 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F11">
         <v>1.42</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E11-'RC log'!F11</f>
         <v>-1.42</v>
       </c>
       <c r="H11">
@@ -4045,16 +4016,13 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12">
-        <v>0.81</v>
+        <v>17</v>
       </c>
       <c r="F12">
         <v>0.45</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E12-'RC log'!F12</f>
         <v>0.36000000000000004</v>
       </c>
       <c r="H12">
@@ -4075,16 +4043,13 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F13">
         <v>2.17</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E13-'RC log'!F13</f>
         <v>-1.17</v>
       </c>
       <c r="K13">
@@ -4102,16 +4067,13 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14">
-        <v>0.245</v>
+        <v>19</v>
       </c>
       <c r="F14">
         <v>0.55000000000000004</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E14-'RC log'!F14</f>
         <v>-0.30500000000000005</v>
       </c>
       <c r="H14">
@@ -4132,16 +4094,13 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F15">
         <v>0.83</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E15-'RC log'!F15</f>
         <v>-0.83</v>
       </c>
       <c r="H15">
@@ -4162,16 +4121,13 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16">
-        <v>-0.08</v>
+        <v>21</v>
       </c>
       <c r="F16">
         <v>1.33</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E16-'RC log'!F16</f>
         <v>-1.4100000000000001</v>
       </c>
       <c r="H16">
@@ -4192,16 +4148,13 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17">
-        <v>0.34499999999999997</v>
+        <v>22</v>
       </c>
       <c r="F17">
         <v>1.1599999999999999</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <f>Sheet1!E17-'RC log'!F17</f>
         <v>-0.81499999999999995</v>
       </c>
       <c r="H17">
@@ -4222,7 +4175,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E18">
         <v>0.2</v>
@@ -4231,11 +4184,11 @@
         <v>1.03</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
-        <v>-0.83000000000000007</v>
+        <f>Sheet1!E18-'RC log'!F18</f>
+        <v>-1.03</v>
       </c>
       <c r="H18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K18">
         <v>26</v>
@@ -4252,7 +4205,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E19">
         <v>0.42</v>
@@ -4261,7 +4214,7 @@
         <v>0.71</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G19:G50" si="0">E19-F19</f>
         <v>-0.28999999999999998</v>
       </c>
       <c r="H19">
@@ -4282,7 +4235,7 @@
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E20">
         <v>0.755</v>
@@ -4312,7 +4265,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E21">
         <v>0.24</v>
@@ -4342,7 +4295,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E22">
         <v>0.75</v>
@@ -4372,7 +4325,7 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E23">
         <v>7.0000000000000007E-2</v>
@@ -4402,7 +4355,7 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -4415,7 +4368,7 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K24">
         <v>26</v>
@@ -4432,7 +4385,7 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E25">
         <v>0.08</v>
@@ -4445,7 +4398,7 @@
         <v>-0.55000000000000004</v>
       </c>
       <c r="H25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K25">
         <v>26</v>
@@ -4462,7 +4415,7 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E26">
         <v>0.84</v>
@@ -4492,7 +4445,7 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4505,7 +4458,7 @@
         <v>-1.07</v>
       </c>
       <c r="H27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K27">
         <v>26</v>
@@ -4522,7 +4475,7 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E28">
         <v>0.81</v>
@@ -4535,7 +4488,7 @@
         <v>0.12000000000000011</v>
       </c>
       <c r="H28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K28">
         <v>26</v>
@@ -4552,7 +4505,7 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -4582,7 +4535,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E30">
         <v>0.245</v>
@@ -4612,7 +4565,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -4642,7 +4595,7 @@
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E32">
         <v>-0.08</v>
@@ -4672,7 +4625,7 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E33">
         <v>0.34499999999999997</v>
@@ -4702,7 +4655,7 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E34">
         <v>0.2</v>
@@ -4715,7 +4668,7 @@
         <v>-0.83000000000000007</v>
       </c>
       <c r="H34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K34">
         <v>26</v>
@@ -4732,7 +4685,7 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E35">
         <v>0.42</v>
@@ -4762,7 +4715,7 @@
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E36">
         <v>0.755</v>
@@ -4792,7 +4745,7 @@
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E37">
         <v>0.24</v>
@@ -4822,7 +4775,7 @@
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E38">
         <v>0.75</v>
@@ -4852,7 +4805,7 @@
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E39">
         <v>7.0000000000000007E-2</v>
@@ -4882,20 +4835,20 @@
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G40" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="H40" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K40">
         <v>26</v>
@@ -4912,7 +4865,7 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E41">
         <v>0.08</v>
@@ -4925,7 +4878,7 @@
         <v>-1.0289999999999999</v>
       </c>
       <c r="H41" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K41">
         <v>26</v>
@@ -4942,7 +4895,7 @@
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E42">
         <v>0.84</v>
@@ -4955,7 +4908,7 @@
         <v>0.12</v>
       </c>
       <c r="H42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K42">
         <v>26</v>
@@ -4972,7 +4925,7 @@
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -4985,7 +4938,7 @@
         <v>-1.33</v>
       </c>
       <c r="H43" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K43">
         <v>26</v>
@@ -5002,7 +4955,7 @@
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E44">
         <v>0.81</v>
@@ -5015,7 +4968,7 @@
         <v>0.1100000000000001</v>
       </c>
       <c r="H44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K44">
         <v>26</v>
@@ -5032,7 +4985,7 @@
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -5045,7 +4998,7 @@
         <v>-1.1600000000000001</v>
       </c>
       <c r="H45" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K45">
         <v>26</v>
@@ -5062,7 +5015,7 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E46">
         <v>0.245</v>
@@ -5092,7 +5045,7 @@
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -5119,7 +5072,7 @@
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E48">
         <v>-0.08</v>
@@ -5149,7 +5102,7 @@
         <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E49">
         <v>0.34499999999999997</v>
@@ -5179,7 +5132,7 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E50">
         <v>0.2</v>
@@ -5203,7 +5156,7 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E51">
         <v>0.42</v>
@@ -5212,7 +5165,7 @@
         <v>1.97</v>
       </c>
       <c r="G51">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G51:G82" si="1">E51-F51</f>
         <v>-1.55</v>
       </c>
     </row>
@@ -5227,7 +5180,7 @@
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E52">
         <v>0.755</v>
@@ -5236,7 +5189,7 @@
         <v>1.51</v>
       </c>
       <c r="G52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.755</v>
       </c>
       <c r="H52">
@@ -5244,10 +5197,6 @@
       </c>
       <c r="I52">
         <v>708</v>
-      </c>
-      <c r="J52">
-        <f>I52*6.33+702.4</f>
-        <v>5184.04</v>
       </c>
       <c r="K52">
         <v>27</v>
@@ -5264,7 +5213,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E53">
         <v>0.24</v>
@@ -5273,7 +5222,7 @@
         <v>1.49</v>
       </c>
       <c r="G53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.25</v>
       </c>
       <c r="H53">
@@ -5281,10 +5230,6 @@
       </c>
       <c r="I53">
         <v>246</v>
-      </c>
-      <c r="J53">
-        <f>I53*6.33+702.4</f>
-        <v>2259.58</v>
       </c>
       <c r="K53">
         <v>27</v>
@@ -5301,7 +5246,7 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E54">
         <v>0.75</v>
@@ -5310,7 +5255,7 @@
         <v>0.87</v>
       </c>
       <c r="G54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.12</v>
       </c>
     </row>
@@ -5325,7 +5270,7 @@
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E55">
         <v>7.0000000000000007E-2</v>
@@ -5334,7 +5279,7 @@
         <v>1.31</v>
       </c>
       <c r="G55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.24</v>
       </c>
     </row>
@@ -5349,7 +5294,7 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -5358,7 +5303,7 @@
         <v>2.46</v>
       </c>
       <c r="G56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.46</v>
       </c>
       <c r="H56">
@@ -5366,10 +5311,6 @@
       </c>
       <c r="I56">
         <v>473</v>
-      </c>
-      <c r="J56">
-        <f t="shared" ref="J56:J96" si="1">I56*6.33+702.4</f>
-        <v>3696.4900000000002</v>
       </c>
       <c r="K56">
         <v>26</v>
@@ -5386,7 +5327,7 @@
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E57">
         <v>0.08</v>
@@ -5395,7 +5336,7 @@
         <v>1.89</v>
       </c>
       <c r="G57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.8099999999999998</v>
       </c>
       <c r="H57">
@@ -5403,10 +5344,6 @@
       </c>
       <c r="I57">
         <v>101</v>
-      </c>
-      <c r="J57">
-        <f t="shared" si="1"/>
-        <v>1341.73</v>
       </c>
       <c r="K57">
         <v>26</v>
@@ -5423,7 +5360,7 @@
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E58">
         <v>0.84</v>
@@ -5432,7 +5369,7 @@
         <v>2.33</v>
       </c>
       <c r="G58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.4900000000000002</v>
       </c>
       <c r="H58">
@@ -5440,10 +5377,6 @@
       </c>
       <c r="I58">
         <v>116</v>
-      </c>
-      <c r="J58">
-        <f t="shared" si="1"/>
-        <v>1436.6799999999998</v>
       </c>
       <c r="K58">
         <v>26</v>
@@ -5460,7 +5393,7 @@
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -5469,7 +5402,7 @@
         <v>2.64</v>
       </c>
       <c r="G59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.64</v>
       </c>
     </row>
@@ -5484,7 +5417,7 @@
         <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E60">
         <v>0.81</v>
@@ -5493,7 +5426,7 @@
         <v>1.91</v>
       </c>
       <c r="G60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.0999999999999999</v>
       </c>
     </row>
@@ -5508,7 +5441,7 @@
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -5517,7 +5450,7 @@
         <v>3.79</v>
       </c>
       <c r="G61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.79</v>
       </c>
     </row>
@@ -5532,7 +5465,7 @@
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E62">
         <v>0.245</v>
@@ -5541,7 +5474,7 @@
         <v>1.71</v>
       </c>
       <c r="G62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.4649999999999999</v>
       </c>
     </row>
@@ -5556,7 +5489,7 @@
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -5565,15 +5498,11 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="G63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.1800000000000002</v>
       </c>
       <c r="I63">
         <v>848</v>
-      </c>
-      <c r="J63">
-        <f t="shared" si="1"/>
-        <v>6070.24</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -5587,7 +5516,7 @@
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E64">
         <v>-0.08</v>
@@ -5596,7 +5525,7 @@
         <v>2.11</v>
       </c>
       <c r="G64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.19</v>
       </c>
     </row>
@@ -5611,7 +5540,7 @@
         <v>4</v>
       </c>
       <c r="D65" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E65">
         <v>0.34499999999999997</v>
@@ -5620,7 +5549,7 @@
         <v>2.35</v>
       </c>
       <c r="G65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.0049999999999999</v>
       </c>
     </row>
@@ -5635,7 +5564,7 @@
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E66">
         <v>0.2</v>
@@ -5644,7 +5573,7 @@
         <v>0</v>
       </c>
       <c r="G66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="H66">
@@ -5652,10 +5581,6 @@
       </c>
       <c r="I66">
         <v>103</v>
-      </c>
-      <c r="J66">
-        <f t="shared" si="1"/>
-        <v>1354.3899999999999</v>
       </c>
       <c r="K66">
         <v>26</v>
@@ -5672,7 +5597,7 @@
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E67">
         <v>0.42</v>
@@ -5681,7 +5606,7 @@
         <v>0</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G81" si="2">E67-F67</f>
+        <f t="shared" si="1"/>
         <v>0.42</v>
       </c>
       <c r="H67">
@@ -5689,10 +5614,6 @@
       </c>
       <c r="I67">
         <v>92</v>
-      </c>
-      <c r="J67">
-        <f t="shared" si="1"/>
-        <v>1284.76</v>
       </c>
       <c r="K67">
         <v>25.7</v>
@@ -5709,7 +5630,7 @@
         <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E68">
         <v>0.755</v>
@@ -5725,10 +5646,6 @@
       </c>
       <c r="I68">
         <v>333</v>
-      </c>
-      <c r="J68">
-        <f t="shared" si="1"/>
-        <v>2810.29</v>
       </c>
       <c r="K68">
         <v>24.9</v>
@@ -5745,7 +5662,7 @@
         <v>4</v>
       </c>
       <c r="D69" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E69">
         <v>0.24</v>
@@ -5754,7 +5671,7 @@
         <v>0.47</v>
       </c>
       <c r="G69">
-        <f t="shared" si="2"/>
+        <f>E69-F69</f>
         <v>-0.22999999999999998</v>
       </c>
       <c r="H69">
@@ -5762,10 +5679,6 @@
       </c>
       <c r="I69">
         <v>649</v>
-      </c>
-      <c r="J69">
-        <f t="shared" si="1"/>
-        <v>4810.57</v>
       </c>
       <c r="K69">
         <v>25.9</v>
@@ -5782,7 +5695,7 @@
         <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E70">
         <v>0.75</v>
@@ -5798,10 +5711,6 @@
       </c>
       <c r="I70">
         <v>348</v>
-      </c>
-      <c r="J70">
-        <f t="shared" si="1"/>
-        <v>2905.2400000000002</v>
       </c>
       <c r="K70">
         <v>25.9</v>
@@ -5818,7 +5727,7 @@
         <v>6</v>
       </c>
       <c r="D71" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E71">
         <v>7.0000000000000007E-2</v>
@@ -5827,7 +5736,7 @@
         <v>0.25</v>
       </c>
       <c r="G71">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G71:G81" si="2">E71-F71</f>
         <v>-0.18</v>
       </c>
       <c r="H71">
@@ -5835,10 +5744,6 @@
       </c>
       <c r="I71">
         <v>603</v>
-      </c>
-      <c r="J71">
-        <f t="shared" si="1"/>
-        <v>4519.3900000000003</v>
       </c>
       <c r="K71">
         <v>27</v>
@@ -5855,7 +5760,7 @@
         <v>7</v>
       </c>
       <c r="D72" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -5873,10 +5778,6 @@
       <c r="I72">
         <v>103</v>
       </c>
-      <c r="J72">
-        <f t="shared" si="1"/>
-        <v>1354.3899999999999</v>
-      </c>
       <c r="K72">
         <v>23</v>
       </c>
@@ -5892,7 +5793,7 @@
         <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E73">
         <v>0.08</v>
@@ -5910,10 +5811,6 @@
       <c r="I73">
         <v>4425</v>
       </c>
-      <c r="J73">
-        <f t="shared" si="1"/>
-        <v>28712.65</v>
-      </c>
       <c r="K73">
         <v>27.75</v>
       </c>
@@ -5929,7 +5826,7 @@
         <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E74">
         <v>0.84</v>
@@ -5947,10 +5844,6 @@
       <c r="I74">
         <v>1791</v>
       </c>
-      <c r="J74">
-        <f t="shared" si="1"/>
-        <v>12039.43</v>
-      </c>
       <c r="K74">
         <v>25.89</v>
       </c>
@@ -5966,7 +5859,7 @@
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -5984,10 +5877,6 @@
       <c r="I75">
         <v>3358</v>
       </c>
-      <c r="J75">
-        <f t="shared" si="1"/>
-        <v>21958.54</v>
-      </c>
       <c r="K75">
         <v>26.57</v>
       </c>
@@ -6003,7 +5892,7 @@
         <v>4</v>
       </c>
       <c r="D76" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E76">
         <v>0.81</v>
@@ -6021,10 +5910,6 @@
       <c r="I76">
         <v>3828</v>
       </c>
-      <c r="J76">
-        <f t="shared" si="1"/>
-        <v>24933.640000000003</v>
-      </c>
       <c r="K76">
         <v>28</v>
       </c>
@@ -6040,7 +5925,7 @@
         <v>5</v>
       </c>
       <c r="D77" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -6052,11 +5937,8 @@
         <f t="shared" si="2"/>
         <v>-2.14</v>
       </c>
-      <c r="J77" t="s">
-        <v>14</v>
-      </c>
       <c r="K77" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -6070,7 +5952,7 @@
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E78">
         <v>0.245</v>
@@ -6082,11 +5964,8 @@
         <f t="shared" si="2"/>
         <v>-0.8849999999999999</v>
       </c>
-      <c r="J78" t="s">
-        <v>14</v>
-      </c>
       <c r="K78" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -6100,7 +5979,7 @@
         <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -6118,10 +5997,6 @@
       <c r="I79">
         <v>3703</v>
       </c>
-      <c r="J79">
-        <f t="shared" si="1"/>
-        <v>24142.390000000003</v>
-      </c>
       <c r="K79">
         <v>28.7</v>
       </c>
@@ -6137,7 +6012,7 @@
         <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E80">
         <v>-0.08</v>
@@ -6155,10 +6030,6 @@
       <c r="I80">
         <v>2916</v>
       </c>
-      <c r="J80">
-        <f t="shared" si="1"/>
-        <v>19160.68</v>
-      </c>
       <c r="K80">
         <v>30.6</v>
       </c>
@@ -6174,7 +6045,7 @@
         <v>4</v>
       </c>
       <c r="D81" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E81">
         <v>0.34499999999999997</v>
@@ -6186,11 +6057,8 @@
         <f t="shared" si="2"/>
         <v>-1.2450000000000001</v>
       </c>
-      <c r="J81" t="s">
-        <v>14</v>
-      </c>
       <c r="K81" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -6204,7 +6072,7 @@
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E82">
         <v>0.2</v>
@@ -6217,10 +6085,6 @@
       </c>
       <c r="I82">
         <v>515</v>
-      </c>
-      <c r="J82">
-        <f t="shared" si="1"/>
-        <v>3962.35</v>
       </c>
       <c r="K82">
         <v>25.8</v>
@@ -6237,7 +6101,7 @@
         <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E83">
         <v>0.42</v>
@@ -6250,10 +6114,6 @@
       </c>
       <c r="I83">
         <v>2950</v>
-      </c>
-      <c r="J83">
-        <f t="shared" si="1"/>
-        <v>19375.900000000001</v>
       </c>
       <c r="K83">
         <v>26</v>
@@ -6270,7 +6130,7 @@
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E84">
         <v>0.755</v>
@@ -6283,10 +6143,6 @@
       </c>
       <c r="I84">
         <v>934</v>
-      </c>
-      <c r="J84">
-        <f t="shared" si="1"/>
-        <v>6614.62</v>
       </c>
       <c r="K84">
         <v>24</v>
@@ -6303,7 +6159,7 @@
         <v>4</v>
       </c>
       <c r="D85" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E85">
         <v>0.24</v>
@@ -6312,7 +6168,7 @@
         <v>0.64</v>
       </c>
       <c r="G85">
-        <f t="shared" ref="G85" si="3">E85-F85</f>
+        <f>E85-F85</f>
         <v>-0.4</v>
       </c>
       <c r="H85">
@@ -6320,10 +6176,6 @@
       </c>
       <c r="I85">
         <v>1310</v>
-      </c>
-      <c r="J85">
-        <f t="shared" si="1"/>
-        <v>8994.6999999999989</v>
       </c>
       <c r="K85">
         <v>26</v>
@@ -6340,7 +6192,7 @@
         <v>5</v>
       </c>
       <c r="D86" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E86">
         <v>0.75</v>
@@ -6353,10 +6205,6 @@
       </c>
       <c r="I86">
         <v>1290</v>
-      </c>
-      <c r="J86">
-        <f t="shared" si="1"/>
-        <v>8868.1</v>
       </c>
       <c r="K86">
         <v>25.72</v>
@@ -6373,7 +6221,7 @@
         <v>6</v>
       </c>
       <c r="D87" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E87">
         <v>7.0000000000000007E-2</v>
@@ -6382,7 +6230,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="G87">
-        <f t="shared" ref="G87" si="4">E87-F87</f>
+        <f>E87-F87</f>
         <v>-0.10499999999999998</v>
       </c>
       <c r="H87">
@@ -6390,10 +6238,6 @@
       </c>
       <c r="I87">
         <v>530</v>
-      </c>
-      <c r="J87">
-        <f t="shared" si="1"/>
-        <v>4057.3</v>
       </c>
       <c r="K87">
         <v>24</v>
@@ -6410,7 +6254,7 @@
         <v>7</v>
       </c>
       <c r="D88" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E88">
         <v>0</v>
@@ -6422,13 +6266,10 @@
         <v>5</v>
       </c>
       <c r="I88" t="s">
-        <v>14</v>
-      </c>
-      <c r="J88" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K88" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
@@ -6442,7 +6283,7 @@
         <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E89">
         <v>0.08</v>
@@ -6451,7 +6292,7 @@
         <v>0.49</v>
       </c>
       <c r="G89">
-        <f t="shared" ref="G89" si="5">E89-F89</f>
+        <f>E89-F89</f>
         <v>-0.41</v>
       </c>
       <c r="H89">
@@ -6459,10 +6300,6 @@
       </c>
       <c r="I89">
         <v>5453</v>
-      </c>
-      <c r="J89">
-        <f t="shared" si="1"/>
-        <v>35219.89</v>
       </c>
       <c r="K89">
         <v>34.33</v>
@@ -6479,7 +6316,7 @@
         <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E90">
         <v>0.84</v>
@@ -6492,10 +6329,6 @@
       </c>
       <c r="I90">
         <v>4554</v>
-      </c>
-      <c r="J90">
-        <f t="shared" si="1"/>
-        <v>29529.22</v>
       </c>
       <c r="K90">
         <v>32.46</v>
@@ -6512,7 +6345,7 @@
         <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -6525,10 +6358,6 @@
       </c>
       <c r="I91">
         <v>909</v>
-      </c>
-      <c r="J91">
-        <f t="shared" si="1"/>
-        <v>6456.37</v>
       </c>
       <c r="K91">
         <v>29.26</v>
@@ -6545,7 +6374,7 @@
         <v>4</v>
       </c>
       <c r="D92" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E92">
         <v>0.81</v>
@@ -6554,7 +6383,7 @@
         <v>1.41</v>
       </c>
       <c r="G92">
-        <f t="shared" ref="G92:G97" si="6">E92-F92</f>
+        <f>E92-F92</f>
         <v>-0.59999999999999987</v>
       </c>
       <c r="H92">
@@ -6562,10 +6391,6 @@
       </c>
       <c r="I92">
         <v>1541</v>
-      </c>
-      <c r="J92">
-        <f t="shared" si="1"/>
-        <v>10456.93</v>
       </c>
       <c r="K92">
         <v>28</v>
@@ -6582,7 +6407,7 @@
         <v>5</v>
       </c>
       <c r="D93" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E93">
         <v>1</v>
@@ -6591,20 +6416,17 @@
         <v>2.5</v>
       </c>
       <c r="G93">
-        <f t="shared" si="6"/>
+        <f>E93-F93</f>
         <v>-1.5</v>
       </c>
       <c r="H93" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I93" t="s">
-        <v>14</v>
-      </c>
-      <c r="J93" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K93" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -6618,7 +6440,7 @@
         <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E94">
         <v>0.245</v>
@@ -6627,7 +6449,7 @@
         <v>0.54</v>
       </c>
       <c r="G94">
-        <f t="shared" si="6"/>
+        <f>E94-F94</f>
         <v>-0.29500000000000004</v>
       </c>
       <c r="H94">
@@ -6635,10 +6457,6 @@
       </c>
       <c r="I94">
         <v>1519</v>
-      </c>
-      <c r="J94">
-        <f t="shared" si="1"/>
-        <v>10317.67</v>
       </c>
       <c r="K94">
         <v>28</v>
@@ -6655,7 +6473,7 @@
         <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -6664,7 +6482,7 @@
         <v>0.59</v>
       </c>
       <c r="G95">
-        <f t="shared" si="6"/>
+        <f>E95-F95</f>
         <v>-0.59</v>
       </c>
       <c r="H95">
@@ -6672,10 +6490,6 @@
       </c>
       <c r="I95">
         <v>1531</v>
-      </c>
-      <c r="J95">
-        <f t="shared" si="1"/>
-        <v>10393.629999999999</v>
       </c>
       <c r="K95">
         <v>28</v>
@@ -6692,7 +6506,7 @@
         <v>3</v>
       </c>
       <c r="D96" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E96">
         <v>-0.08</v>
@@ -6706,15 +6520,11 @@
       <c r="I96">
         <v>3013</v>
       </c>
-      <c r="J96">
-        <f t="shared" si="1"/>
-        <v>19774.690000000002</v>
-      </c>
       <c r="K96">
         <v>28</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>45502</v>
       </c>
@@ -6725,7 +6535,7 @@
         <v>4</v>
       </c>
       <c r="D97" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E97">
         <v>0.34499999999999997</v>
@@ -6734,8 +6544,468 @@
         <v>1.38</v>
       </c>
       <c r="G97">
-        <f t="shared" si="6"/>
+        <f>E97-F97</f>
         <v>-1.0349999999999999</v>
+      </c>
+      <c r="H97">
+        <v>5.41</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B98">
+        <v>5</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98">
+        <v>0.2</v>
+      </c>
+      <c r="G98">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="H98">
+        <v>5.41</v>
+      </c>
+      <c r="I98">
+        <v>1280</v>
+      </c>
+      <c r="K98">
+        <v>26.04</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B99">
+        <v>5</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99">
+        <v>0.42</v>
+      </c>
+      <c r="G99">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H99">
+        <v>5.34</v>
+      </c>
+      <c r="I99">
+        <v>1776</v>
+      </c>
+      <c r="K99">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B100">
+        <v>5</v>
+      </c>
+      <c r="C100">
+        <v>3</v>
+      </c>
+      <c r="D100" t="s">
+        <v>8</v>
+      </c>
+      <c r="E100">
+        <v>0.755</v>
+      </c>
+      <c r="F100">
+        <f>0.83-0.72</f>
+        <v>0.10999999999999999</v>
+      </c>
+      <c r="G100">
+        <f>F100-E100</f>
+        <v>-0.64500000000000002</v>
+      </c>
+      <c r="H100">
+        <v>5.37</v>
+      </c>
+      <c r="I100">
+        <v>647.4</v>
+      </c>
+      <c r="K100">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B101">
+        <v>5</v>
+      </c>
+      <c r="C101">
+        <v>4</v>
+      </c>
+      <c r="D101" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101">
+        <v>0.24</v>
+      </c>
+      <c r="F101">
+        <f>1.68-0.9</f>
+        <v>0.77999999999999992</v>
+      </c>
+      <c r="G101">
+        <f t="shared" ref="G101:G102" si="3">F101-E101</f>
+        <v>0.53999999999999992</v>
+      </c>
+      <c r="H101">
+        <v>5.16</v>
+      </c>
+      <c r="I101">
+        <v>1738</v>
+      </c>
+      <c r="K101">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B102">
+        <v>5</v>
+      </c>
+      <c r="C102">
+        <v>5</v>
+      </c>
+      <c r="D102" t="s">
+        <v>10</v>
+      </c>
+      <c r="E102">
+        <v>0.75</v>
+      </c>
+      <c r="F102">
+        <f>0.82-0.76</f>
+        <v>5.9999999999999942E-2</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="3"/>
+        <v>-0.69000000000000006</v>
+      </c>
+      <c r="H102">
+        <v>4.45</v>
+      </c>
+      <c r="I102">
+        <v>1572</v>
+      </c>
+      <c r="K102">
+        <v>26.43</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B103">
+        <v>5</v>
+      </c>
+      <c r="C103">
+        <v>6</v>
+      </c>
+      <c r="D103" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="I103">
+        <v>1488</v>
+      </c>
+      <c r="K103">
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B104">
+        <v>5</v>
+      </c>
+      <c r="C104">
+        <v>7</v>
+      </c>
+      <c r="D104" t="s">
+        <v>13</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B105">
+        <v>6</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105" t="s">
+        <v>14</v>
+      </c>
+      <c r="E105">
+        <v>0.08</v>
+      </c>
+      <c r="G105">
+        <v>-0.19</v>
+      </c>
+      <c r="H105">
+        <v>4.22</v>
+      </c>
+      <c r="I105">
+        <v>1330</v>
+      </c>
+      <c r="K105">
+        <v>27.11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B106">
+        <v>6</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
+      </c>
+      <c r="D106" t="s">
+        <v>15</v>
+      </c>
+      <c r="E106">
+        <v>0.84</v>
+      </c>
+      <c r="G106">
+        <v>0.06</v>
+      </c>
+      <c r="H106">
+        <v>4.37</v>
+      </c>
+      <c r="I106">
+        <v>4850</v>
+      </c>
+      <c r="K106">
+        <v>26.01</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B107">
+        <v>6</v>
+      </c>
+      <c r="C107">
+        <v>3</v>
+      </c>
+      <c r="D107" t="s">
+        <v>16</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="G107">
+        <v>-0.51</v>
+      </c>
+      <c r="H107">
+        <v>4.71</v>
+      </c>
+      <c r="I107">
+        <v>830</v>
+      </c>
+      <c r="K107">
+        <v>26.23</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B108">
+        <v>6</v>
+      </c>
+      <c r="C108">
+        <v>4</v>
+      </c>
+      <c r="D108" t="s">
+        <v>17</v>
+      </c>
+      <c r="E108">
+        <v>0.81</v>
+      </c>
+      <c r="G108">
+        <v>-0.04</v>
+      </c>
+      <c r="H108">
+        <v>4.41</v>
+      </c>
+      <c r="I108">
+        <v>500</v>
+      </c>
+      <c r="K108">
+        <v>26.62</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B109">
+        <v>6</v>
+      </c>
+      <c r="C109">
+        <v>5</v>
+      </c>
+      <c r="D109" t="s">
+        <v>18</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="G109">
+        <f>0.99-1.97</f>
+        <v>-0.98</v>
+      </c>
+      <c r="H109">
+        <v>4.34</v>
+      </c>
+      <c r="I109">
+        <v>1144</v>
+      </c>
+      <c r="K109">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B110">
+        <v>9</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110" t="s">
+        <v>19</v>
+      </c>
+      <c r="E110">
+        <v>0.245</v>
+      </c>
+      <c r="G110">
+        <f>0.24-0.4</f>
+        <v>-0.16000000000000003</v>
+      </c>
+      <c r="H110">
+        <v>3.83</v>
+      </c>
+      <c r="I110">
+        <v>2900</v>
+      </c>
+      <c r="K110">
+        <v>29.07</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B111">
+        <v>9</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+      <c r="D111" t="s">
+        <v>20</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="G111">
+        <v>-0.4</v>
+      </c>
+      <c r="H111">
+        <v>3.97</v>
+      </c>
+      <c r="I111">
+        <v>3560</v>
+      </c>
+      <c r="K111">
+        <v>28.69</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B112">
+        <v>9</v>
+      </c>
+      <c r="C112">
+        <v>3</v>
+      </c>
+      <c r="D112" t="s">
+        <v>21</v>
+      </c>
+      <c r="E112">
+        <v>-0.08</v>
+      </c>
+      <c r="G112">
+        <v>-0.39</v>
+      </c>
+      <c r="H112">
+        <v>3.85</v>
+      </c>
+      <c r="I112">
+        <v>3732</v>
+      </c>
+      <c r="K112">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B113">
+        <v>9</v>
+      </c>
+      <c r="C113">
+        <v>4</v>
+      </c>
+      <c r="D113" t="s">
+        <v>22</v>
+      </c>
+      <c r="E113">
+        <v>0.34499999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -6764,27 +7034,27 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -6808,7 +7078,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -6832,7 +7102,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -6856,7 +7126,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -6880,7 +7150,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>16</v>
@@ -6904,7 +7174,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>25</v>
@@ -6928,7 +7198,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>40</v>
@@ -6952,7 +7222,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -6976,7 +7246,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -7000,7 +7270,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>26</v>
@@ -7024,7 +7294,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -7048,7 +7318,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>25</v>
@@ -7072,7 +7342,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -7096,7 +7366,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -7120,7 +7390,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>14</v>
@@ -7144,7 +7414,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
prepping long and RC datasets
</commit_message>
<xml_diff>
--- a/01_Raw_data/RC log.xlsx
+++ b/01_Raw_data/RC log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samanthahowley\Desktop\Howley_Bradford_Streams\01_Raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Howley_Bradford_Streams\Howley_Bradford_Streams\01_Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59D8DCE-C860-4E09-8A36-BE178A97DF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06BFE4F-EDC3-4DEA-9D7F-8ECF606B9554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{A079E74B-2391-4069-81A1-6515CCD90540}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="14400" windowHeight="7455" xr2:uid="{A079E74B-2391-4069-81A1-6515CCD90540}"/>
   </bookViews>
   <sheets>
     <sheet name="RC log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -3688,19 +3688,19 @@
   <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G103" sqref="G103:G112"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.40625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" s="1">
         <v>45400</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" s="1">
         <v>45400</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" s="1">
         <v>45400</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" s="1">
         <v>45400</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" s="1">
         <v>45400</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" s="1">
         <v>45400</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" s="1">
         <v>45400</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" s="1">
         <v>45400</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" s="1">
         <v>45400</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" s="1">
         <v>45400</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" s="1">
         <v>45400</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13" s="1">
         <v>45400</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A14" s="1">
         <v>45400</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A15" s="1">
         <v>45400</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A16" s="1">
         <v>45400</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A17" s="1">
         <v>45400</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A18" s="1">
         <v>45420</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A19" s="1">
         <v>45420</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A20" s="1">
         <v>45420</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A21" s="1">
         <v>45420</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A22" s="1">
         <v>45420</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A23" s="1">
         <v>45420</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A24" s="1">
         <v>45420</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A25" s="1">
         <v>45420</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A26" s="1">
         <v>45420</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A27" s="1">
         <v>45420</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A28" s="1">
         <v>45420</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A29" s="1">
         <v>45420</v>
       </c>
@@ -4524,7 +4524,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A30" s="1">
         <v>45420</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A31" s="1">
         <v>45420</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A32" s="1">
         <v>45420</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A33" s="1">
         <v>45420</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A34" s="1">
         <v>45442</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A35" s="1">
         <v>45442</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A36" s="1">
         <v>45442</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A37" s="1">
         <v>45442</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A38" s="1">
         <v>45442</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A39" s="1">
         <v>45442</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A40" s="1">
         <v>45442</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A41" s="1">
         <v>45442</v>
       </c>
@@ -4884,7 +4884,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A42" s="1">
         <v>45442</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A43" s="1">
         <v>45442</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A44" s="1">
         <v>45442</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A45" s="1">
         <v>45442</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A46" s="1">
         <v>45442</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A47" s="1">
         <v>45442</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A48" s="1">
         <v>45442</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A49" s="1">
         <v>45442</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A50" s="1">
         <v>45463</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>-0.85000000000000009</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A51" s="1">
         <v>45463</v>
       </c>
@@ -5165,11 +5165,11 @@
         <v>1.97</v>
       </c>
       <c r="G51">
-        <f t="shared" ref="G51:G82" si="1">E51-F51</f>
+        <f t="shared" ref="G51:G67" si="1">E51-F51</f>
         <v>-1.55</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A52" s="1">
         <v>45463</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A53" s="1">
         <v>45463</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A54" s="1">
         <v>45463</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>-0.12</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A55" s="1">
         <v>45463</v>
       </c>
@@ -5283,7 +5283,7 @@
         <v>-1.24</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A56" s="1">
         <v>45463</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A57" s="1">
         <v>45463</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A58" s="1">
         <v>45463</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A59" s="1">
         <v>45463</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>-2.64</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A60" s="1">
         <v>45463</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>-1.0999999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A61" s="1">
         <v>45463</v>
       </c>
@@ -5454,7 +5454,7 @@
         <v>-2.79</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A62" s="1">
         <v>45463</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>-1.4649999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A63" s="1">
         <v>45463</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A64" s="1">
         <v>45463</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>-2.19</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A65" s="1">
         <v>45463</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>-2.0049999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A66" s="1">
         <v>45484</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A67" s="1">
         <v>45484</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A68" s="1">
         <v>45484</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A69" s="1">
         <v>45484</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A70" s="1">
         <v>45484</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A71" s="1">
         <v>45484</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A72" s="1">
         <v>45484</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A73" s="1">
         <v>45484</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>27.75</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A74" s="1">
         <v>45484</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>25.89</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A75" s="1">
         <v>45484</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>26.57</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A76" s="1">
         <v>45484</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A77" s="1">
         <v>45484</v>
       </c>
@@ -5941,7 +5941,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A78" s="1">
         <v>45484</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A79" s="1">
         <v>45484</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A80" s="1">
         <v>45484</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A81" s="1">
         <v>45484</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A82" s="1">
         <v>45502</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A83" s="1">
         <v>45502</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A84" s="1">
         <v>45502</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A85" s="1">
         <v>45502</v>
       </c>
@@ -6181,7 +6181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A86" s="1">
         <v>45502</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>25.72</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A87" s="1">
         <v>45502</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A88" s="1">
         <v>45502</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A89" s="1">
         <v>45502</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>34.33</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A90" s="1">
         <v>45502</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>32.46</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A91" s="1">
         <v>45502</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>29.26</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A92" s="1">
         <v>45502</v>
       </c>
@@ -6396,7 +6396,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A93" s="1">
         <v>45502</v>
       </c>
@@ -6419,17 +6419,8 @@
         <f>E93-F93</f>
         <v>-1.5</v>
       </c>
-      <c r="H93" t="s">
-        <v>12</v>
-      </c>
-      <c r="I93" t="s">
-        <v>12</v>
-      </c>
-      <c r="K93" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A94" s="1">
         <v>45502</v>
       </c>
@@ -6462,7 +6453,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A95" s="1">
         <v>45502</v>
       </c>
@@ -6495,7 +6486,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A96" s="1">
         <v>45502</v>
       </c>
@@ -6524,7 +6515,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A97" s="1">
         <v>45502</v>
       </c>
@@ -6551,7 +6542,7 @@
         <v>5.41</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A98" s="1">
         <v>45534</v>
       </c>
@@ -6580,7 +6571,7 @@
         <v>26.04</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A99" s="1">
         <v>45534</v>
       </c>
@@ -6609,7 +6600,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A100" s="1">
         <v>45534</v>
       </c>
@@ -6643,7 +6634,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A101" s="1">
         <v>45534</v>
       </c>
@@ -6677,7 +6668,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A102" s="1">
         <v>45534</v>
       </c>
@@ -6711,7 +6702,7 @@
         <v>26.43</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A103" s="1">
         <v>45534</v>
       </c>
@@ -6740,7 +6731,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A104" s="1">
         <v>45534</v>
       </c>
@@ -6757,7 +6748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A105" s="1">
         <v>45534</v>
       </c>
@@ -6786,7 +6777,7 @@
         <v>27.11</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A106" s="1">
         <v>45534</v>
       </c>
@@ -6815,7 +6806,7 @@
         <v>26.01</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A107" s="1">
         <v>45534</v>
       </c>
@@ -6844,7 +6835,7 @@
         <v>26.23</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A108" s="1">
         <v>45534</v>
       </c>
@@ -6873,7 +6864,7 @@
         <v>26.62</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A109" s="1">
         <v>45534</v>
       </c>
@@ -6903,7 +6894,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A110" s="1">
         <v>45534</v>
       </c>
@@ -6933,7 +6924,7 @@
         <v>29.07</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A111" s="1">
         <v>45534</v>
       </c>
@@ -6962,7 +6953,7 @@
         <v>28.69</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A112" s="1">
         <v>45534</v>
       </c>
@@ -6991,7 +6982,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A113" s="1">
         <v>45534</v>
       </c>
@@ -7021,15 +7012,15 @@
       <selection activeCell="E2" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.40625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -7052,7 +7043,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -7076,7 +7067,7 @@
         <v>79.863910000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -7100,7 +7091,7 @@
         <v>76.943730000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -7124,7 +7115,7 @@
         <v>88.202100000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -7148,7 +7139,7 @@
         <v>76.922430000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -7172,7 +7163,7 @@
         <v>92.059330000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -7196,7 +7187,7 @@
         <v>76.370699999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -7220,7 +7211,7 @@
         <v>93.197450000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -7244,7 +7235,7 @@
         <v>76.815430000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -7268,7 +7259,7 @@
         <v>76.590829999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -7292,7 +7283,7 @@
         <v>76.606219999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -7316,7 +7307,7 @@
         <v>76.513019999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -7340,7 +7331,7 @@
         <v>76.622630000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -7364,7 +7355,7 @@
         <v>66.857730000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -7388,7 +7379,7 @@
         <v>67.045649999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -7412,7 +7403,7 @@
         <v>67.109120000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -7433,7 +7424,7 @@
         <v>66.502930000000006</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G18">
         <v>652.93119999999999</v>
       </c>
@@ -7441,7 +7432,7 @@
         <v>66.842190000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G19">
         <v>653.20910000000003</v>
       </c>
@@ -7449,7 +7440,7 @@
         <v>66.69511</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G20">
         <v>607.95830000000001</v>
       </c>
@@ -7457,7 +7448,7 @@
         <v>67.072839999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G21">
         <v>607.56110000000001</v>
       </c>
@@ -7465,7 +7456,7 @@
         <v>66.492159999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G22">
         <v>638.08180000000004</v>
       </c>
@@ -7473,7 +7464,7 @@
         <v>66.821780000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G23">
         <v>638.25340000000006</v>
       </c>
@@ -7481,7 +7472,7 @@
         <v>66.970429999999993</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G24">
         <v>623.13530000000003</v>
       </c>
@@ -7489,7 +7480,7 @@
         <v>66.743210000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G25">
         <v>607.76750000000004</v>
       </c>
@@ -7497,7 +7488,7 @@
         <v>66.741129999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G26">
         <v>592.50710000000004</v>
       </c>
@@ -7505,7 +7496,7 @@
         <v>66.642009999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G27">
         <v>577.47490000000005</v>
       </c>
@@ -7513,7 +7504,7 @@
         <v>66.604929999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G28">
         <v>562.39620000000002</v>
       </c>
@@ -7521,7 +7512,7 @@
         <v>66.727909999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G29">
         <v>562.76610000000005</v>
       </c>
@@ -7529,7 +7520,7 @@
         <v>66.755129999999994</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G30">
         <v>562.50009999999997</v>
       </c>
@@ -7537,7 +7528,7 @@
         <v>66.565960000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G31">
         <v>562.36329999999998</v>
       </c>
@@ -7545,7 +7536,7 @@
         <v>66.708879999999994</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G32">
         <v>577.42870000000005</v>
       </c>
@@ -7553,7 +7544,7 @@
         <v>66.438630000000003</v>
       </c>
     </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G33">
         <v>577.51340000000005</v>
       </c>
@@ -7561,7 +7552,7 @@
         <v>66.721999999999994</v>
       </c>
     </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G34">
         <v>622.80349999999999</v>
       </c>
@@ -7569,7 +7560,7 @@
         <v>66.502319999999997</v>
       </c>
     </row>
-    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G35">
         <v>698.44579999999996</v>
       </c>
@@ -7577,7 +7568,7 @@
         <v>66.603359999999995</v>
       </c>
     </row>
-    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G36">
         <v>728.82050000000004</v>
       </c>
@@ -7585,7 +7576,7 @@
         <v>66.735640000000004</v>
       </c>
     </row>
-    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G37">
         <v>744.46180000000004</v>
       </c>
@@ -7593,7 +7584,7 @@
         <v>67.009540000000001</v>
       </c>
     </row>
-    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G38">
         <v>728.54539999999997</v>
       </c>
@@ -7601,7 +7592,7 @@
         <v>66.730959999999996</v>
       </c>
     </row>
-    <row r="39" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G39">
         <v>728.59079999999994</v>
       </c>
@@ -7609,7 +7600,7 @@
         <v>66.700519999999997</v>
       </c>
     </row>
-    <row r="40" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G40">
         <v>728.52480000000003</v>
       </c>
@@ -7617,7 +7608,7 @@
         <v>66.432400000000001</v>
       </c>
     </row>
-    <row r="41" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G41">
         <v>744.04729999999995</v>
       </c>
@@ -7625,7 +7616,7 @@
         <v>66.440209999999993</v>
       </c>
     </row>
-    <row r="42" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G42">
         <v>744.07650000000001</v>
       </c>
@@ -7633,7 +7624,7 @@
         <v>66.810680000000005</v>
       </c>
     </row>
-    <row r="43" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G43">
         <v>759.36440000000005</v>
       </c>
@@ -7641,7 +7632,7 @@
         <v>66.765969999999996</v>
       </c>
     </row>
-    <row r="44" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G44">
         <v>774.61670000000004</v>
       </c>
@@ -7649,7 +7640,7 @@
         <v>66.688059999999993</v>
       </c>
     </row>
-    <row r="45" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G45">
         <v>774.67240000000004</v>
       </c>
@@ -7657,7 +7648,7 @@
         <v>66.708640000000003</v>
       </c>
     </row>
-    <row r="46" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G46">
         <v>789.6807</v>
       </c>
@@ -7665,7 +7656,7 @@
         <v>66.707120000000003</v>
       </c>
     </row>
-    <row r="47" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G47">
         <v>834.55520000000001</v>
       </c>
@@ -7673,7 +7664,7 @@
         <v>66.699510000000004</v>
       </c>
     </row>
-    <row r="48" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G48">
         <v>834.96130000000005</v>
       </c>
@@ -7681,7 +7672,7 @@
         <v>67.011229999999998</v>
       </c>
     </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G49">
         <v>850.197</v>
       </c>
@@ -7689,7 +7680,7 @@
         <v>66.578879999999998</v>
       </c>
     </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G50">
         <v>865.02120000000002</v>
       </c>
@@ -7697,7 +7688,7 @@
         <v>66.439570000000003</v>
       </c>
     </row>
-    <row r="51" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G51">
         <v>865.25400000000002</v>
       </c>
@@ -7705,7 +7696,7 @@
         <v>66.421679999999995</v>
       </c>
     </row>
-    <row r="52" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G52">
         <v>880.46839999999997</v>
       </c>
@@ -7713,7 +7704,7 @@
         <v>66.699039999999997</v>
       </c>
     </row>
-    <row r="53" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G53">
         <v>895.39089999999999</v>
       </c>
@@ -7721,7 +7712,7 @@
         <v>66.41798</v>
       </c>
     </row>
-    <row r="54" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G54">
         <v>895.33799999999997</v>
       </c>
@@ -7729,7 +7720,7 @@
         <v>66.555769999999995</v>
       </c>
     </row>
-    <row r="55" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G55">
         <v>910.66690000000006</v>
       </c>
@@ -7737,7 +7728,7 @@
         <v>66.713909999999998</v>
       </c>
     </row>
-    <row r="56" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G56">
         <v>925.98109999999997</v>
       </c>
@@ -7745,7 +7736,7 @@
         <v>66.679460000000006</v>
       </c>
     </row>
-    <row r="57" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G57">
         <v>940.77919999999995</v>
       </c>
@@ -7753,7 +7744,7 @@
         <v>66.716350000000006</v>
       </c>
     </row>
-    <row r="58" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G58">
         <v>955.72770000000003</v>
       </c>
@@ -7761,7 +7752,7 @@
         <v>66.600700000000003</v>
       </c>
     </row>
-    <row r="59" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G59">
         <v>970.87699999999995</v>
       </c>
@@ -7769,7 +7760,7 @@
         <v>67.232489999999999</v>
       </c>
     </row>
-    <row r="60" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G60">
         <v>986.60170000000005</v>
       </c>
@@ -7777,7 +7768,7 @@
         <v>66.475719999999995</v>
       </c>
     </row>
-    <row r="61" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G61">
         <v>1001.513</v>
       </c>
@@ -7785,7 +7776,7 @@
         <v>69.48903</v>
       </c>
     </row>
-    <row r="62" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G62">
         <v>1016.558</v>
       </c>
@@ -7793,7 +7784,7 @@
         <v>66.661689999999993</v>
       </c>
     </row>
-    <row r="63" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G63">
         <v>1031.5419999999999</v>
       </c>
@@ -7801,7 +7792,7 @@
         <v>77.511840000000007</v>
       </c>
     </row>
-    <row r="64" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G64">
         <v>1047.2439999999999</v>
       </c>
@@ -7809,7 +7800,7 @@
         <v>66.713200000000001</v>
       </c>
     </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G65">
         <v>1061.7260000000001</v>
       </c>
@@ -7817,7 +7808,7 @@
         <v>80.544539999999998</v>
       </c>
     </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G66">
         <v>1077.3230000000001</v>
       </c>
@@ -7825,7 +7816,7 @@
         <v>66.882890000000003</v>
       </c>
     </row>
-    <row r="67" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G67">
         <v>1107.306</v>
       </c>
@@ -7833,7 +7824,7 @@
         <v>82.613020000000006</v>
       </c>
     </row>
-    <row r="68" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G68">
         <v>1122.7550000000001</v>
       </c>
@@ -7841,7 +7832,7 @@
         <v>66.875720000000001</v>
       </c>
     </row>
-    <row r="69" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G69">
         <v>1167.7729999999999</v>
       </c>
@@ -7849,7 +7840,7 @@
         <v>81.679119999999998</v>
       </c>
     </row>
-    <row r="70" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G70">
         <v>1183.0219999999999</v>
       </c>
@@ -7857,7 +7848,7 @@
         <v>76.520039999999995</v>
       </c>
     </row>
-    <row r="71" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G71">
         <v>1183.3119999999999</v>
       </c>
@@ -7865,7 +7856,7 @@
         <v>76.523030000000006</v>
       </c>
     </row>
-    <row r="72" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G72">
         <v>1198.4190000000001</v>
       </c>
@@ -7873,7 +7864,7 @@
         <v>76.558539999999994</v>
       </c>
     </row>
-    <row r="73" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G73">
         <v>1213.2</v>
       </c>
@@ -7881,7 +7872,7 @@
         <v>76.322270000000003</v>
       </c>
     </row>
-    <row r="74" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G74">
         <v>1213.443</v>
       </c>
@@ -7889,7 +7880,7 @@
         <v>76.840400000000002</v>
       </c>
     </row>
-    <row r="75" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G75">
         <v>1228.8979999999999</v>
       </c>
@@ -7897,7 +7888,7 @@
         <v>76.866280000000003</v>
       </c>
     </row>
-    <row r="76" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G76">
         <v>1244.1220000000001</v>
       </c>
@@ -7905,7 +7896,7 @@
         <v>76.297600000000003</v>
       </c>
     </row>
-    <row r="77" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G77">
         <v>1259.123</v>
       </c>
@@ -7913,7 +7904,7 @@
         <v>76.881839999999997</v>
       </c>
     </row>
-    <row r="78" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G78">
         <v>1258.752</v>
       </c>
@@ -7921,7 +7912,7 @@
         <v>76.468999999999994</v>
       </c>
     </row>
-    <row r="79" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G79">
         <v>1304.1369999999999</v>
       </c>
@@ -7929,7 +7920,7 @@
         <v>76.618129999999994</v>
       </c>
     </row>
-    <row r="80" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G80">
         <v>1349.9849999999999</v>
       </c>
@@ -7937,7 +7928,7 @@
         <v>76.480620000000002</v>
       </c>
     </row>
-    <row r="81" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G81">
         <v>1350.0229999999999</v>
       </c>
@@ -7945,7 +7936,7 @@
         <v>76.648570000000007</v>
       </c>
     </row>
-    <row r="82" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G82">
         <v>1364.8150000000001</v>
       </c>
@@ -7953,7 +7944,7 @@
         <v>76.311499999999995</v>
       </c>
     </row>
-    <row r="83" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G83">
         <v>1380.152</v>
       </c>
@@ -7961,7 +7952,7 @@
         <v>76.679150000000007</v>
       </c>
     </row>
-    <row r="84" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G84">
         <v>1380.086</v>
       </c>
@@ -7969,7 +7960,7 @@
         <v>76.621639999999999</v>
       </c>
     </row>
-    <row r="85" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G85">
         <v>1379.7149999999999</v>
       </c>
@@ -7977,7 +7968,7 @@
         <v>76.371279999999999</v>
       </c>
     </row>
-    <row r="86" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G86">
         <v>1394.9970000000001</v>
       </c>
@@ -7985,7 +7976,7 @@
         <v>76.636949999999999</v>
       </c>
     </row>
-    <row r="87" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G87">
         <v>1410.3409999999999</v>
       </c>
@@ -7993,7 +7984,7 @@
         <v>76.882059999999996</v>
       </c>
     </row>
-    <row r="88" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G88">
         <v>1425.6030000000001</v>
       </c>
@@ -8001,7 +7992,7 @@
         <v>76.91395</v>
       </c>
     </row>
-    <row r="89" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G89">
         <v>1409.979</v>
       </c>
@@ -8009,7 +8000,7 @@
         <v>76.394909999999996</v>
       </c>
     </row>
-    <row r="90" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G90">
         <v>1410.248</v>
       </c>
@@ -8017,7 +8008,7 @@
         <v>76.664580000000001</v>
       </c>
     </row>
-    <row r="91" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G91">
         <v>1455.58</v>
       </c>
@@ -8025,7 +8016,7 @@
         <v>76.792010000000005</v>
       </c>
     </row>
-    <row r="92" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G92">
         <v>1486.2159999999999</v>
       </c>
@@ -8033,7 +8024,7 @@
         <v>86.622889999999998</v>
       </c>
     </row>
-    <row r="93" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G93">
         <v>1485.806</v>
       </c>
@@ -8041,7 +8032,7 @@
         <v>86.426929999999999</v>
       </c>
     </row>
-    <row r="94" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G94">
         <v>1516.0709999999999</v>
       </c>
@@ -8049,7 +8040,7 @@
         <v>86.291049999999998</v>
       </c>
     </row>
-    <row r="95" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G95">
         <v>1515.9280000000001</v>
       </c>
@@ -8057,7 +8048,7 @@
         <v>86.616039999999998</v>
       </c>
     </row>
-    <row r="96" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G96">
         <v>1516.348</v>
       </c>
@@ -8065,7 +8056,7 @@
         <v>86.725769999999997</v>
       </c>
     </row>
-    <row r="97" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G97">
         <v>1531.32</v>
       </c>
@@ -8073,7 +8064,7 @@
         <v>86.364840000000001</v>
       </c>
     </row>
-    <row r="98" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G98">
         <v>1531.4570000000001</v>
       </c>
@@ -8081,7 +8072,7 @@
         <v>86.454610000000002</v>
       </c>
     </row>
-    <row r="99" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G99">
         <v>1531.6220000000001</v>
       </c>
@@ -8089,7 +8080,7 @@
         <v>86.403989999999993</v>
       </c>
     </row>
-    <row r="100" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G100">
         <v>1531.232</v>
       </c>
@@ -8097,7 +8088,7 @@
         <v>86.471239999999995</v>
       </c>
     </row>
-    <row r="101" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G101">
         <v>1531.4369999999999</v>
       </c>
@@ -8105,7 +8096,7 @@
         <v>86.733379999999997</v>
       </c>
     </row>
-    <row r="102" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G102">
         <v>1531.0519999999999</v>
       </c>
@@ -8113,7 +8104,7 @@
         <v>86.402079999999998</v>
       </c>
     </row>
-    <row r="103" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G103">
         <v>1531.268</v>
       </c>
@@ -8121,7 +8112,7 @@
         <v>86.439710000000005</v>
       </c>
     </row>
-    <row r="104" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G104">
         <v>1546.579</v>
       </c>
@@ -8129,7 +8120,7 @@
         <v>86.730919999999998</v>
       </c>
     </row>
-    <row r="105" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G105">
         <v>1546.319</v>
       </c>
@@ -8137,7 +8128,7 @@
         <v>86.136409999999998</v>
       </c>
     </row>
-    <row r="106" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G106">
         <v>1576.8009999999999</v>
       </c>
@@ -8145,7 +8136,7 @@
         <v>86.486429999999999</v>
       </c>
     </row>
-    <row r="107" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G107">
         <v>1591.886</v>
       </c>
@@ -8153,7 +8144,7 @@
         <v>86.408940000000001</v>
       </c>
     </row>
-    <row r="108" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G108">
         <v>1607.3309999999999</v>
       </c>
@@ -8161,7 +8152,7 @@
         <v>86.266360000000006</v>
       </c>
     </row>
-    <row r="109" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G109">
         <v>1607.1669999999999</v>
       </c>
@@ -8169,7 +8160,7 @@
         <v>96.321259999999995</v>
       </c>
     </row>
-    <row r="110" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G110">
         <v>1622.027</v>
       </c>
@@ -8177,7 +8168,7 @@
         <v>95.994619999999998</v>
       </c>
     </row>
-    <row r="111" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G111">
         <v>1622.26</v>
       </c>
@@ -8185,7 +8176,7 @@
         <v>96.47484</v>
       </c>
     </row>
-    <row r="112" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G112">
         <v>1637.01</v>
       </c>
@@ -8193,7 +8184,7 @@
         <v>96.487459999999999</v>
       </c>
     </row>
-    <row r="113" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G113">
         <v>1637.1120000000001</v>
       </c>
@@ -8201,7 +8192,7 @@
         <v>95.942539999999994</v>
       </c>
     </row>
-    <row r="114" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G114">
         <v>1652.441</v>
       </c>
@@ -8209,7 +8200,7 @@
         <v>96.212249999999997</v>
       </c>
     </row>
-    <row r="115" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G115">
         <v>1652.6880000000001</v>
       </c>
@@ -8217,7 +8208,7 @@
         <v>96.16</v>
       </c>
     </row>
-    <row r="116" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G116">
         <v>1652.4690000000001</v>
       </c>
@@ -8225,7 +8216,7 @@
         <v>96.532060000000001</v>
       </c>
     </row>
-    <row r="117" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G117">
         <v>1667.163</v>
       </c>
@@ -8233,7 +8224,7 @@
         <v>96.261859999999999</v>
       </c>
     </row>
-    <row r="118" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G118">
         <v>1682.24</v>
       </c>
@@ -8241,7 +8232,7 @@
         <v>96.204570000000004</v>
       </c>
     </row>
-    <row r="119" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G119">
         <v>1682.7049999999999</v>
       </c>
@@ -8249,7 +8240,7 @@
         <v>95.947130000000001</v>
       </c>
     </row>
-    <row r="120" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G120">
         <v>1697.7449999999999</v>
       </c>
@@ -8257,7 +8248,7 @@
         <v>102.5564</v>
       </c>
     </row>
-    <row r="121" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G121">
         <v>1697.4570000000001</v>
       </c>
@@ -8265,7 +8256,7 @@
         <v>96.26979</v>
       </c>
     </row>
-    <row r="122" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G122">
         <v>1697.8979999999999</v>
       </c>
@@ -8273,7 +8264,7 @@
         <v>107.5222</v>
       </c>
     </row>
-    <row r="123" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G123">
         <v>1713.067</v>
       </c>
@@ -8281,7 +8272,7 @@
         <v>96.174220000000005</v>
       </c>
     </row>
-    <row r="124" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G124">
         <v>1713.4069999999999</v>
       </c>
@@ -8289,7 +8280,7 @@
         <v>111.3181</v>
       </c>
     </row>
-    <row r="125" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G125">
         <v>1713.269</v>
       </c>
@@ -8297,7 +8288,7 @@
         <v>96.214839999999995</v>
       </c>
     </row>
-    <row r="126" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G126">
         <v>1742.9939999999999</v>
       </c>
@@ -8305,7 +8296,7 @@
         <v>122.13800000000001</v>
       </c>
     </row>
-    <row r="127" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G127">
         <v>1773.7049999999999</v>
       </c>
@@ -8313,7 +8304,7 @@
         <v>105.7696</v>
       </c>
     </row>
-    <row r="128" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G128">
         <v>1788.712</v>
       </c>
@@ -8321,7 +8312,7 @@
         <v>106.3018</v>
       </c>
     </row>
-    <row r="129" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G129">
         <v>1803.973</v>
       </c>
@@ -8329,7 +8320,7 @@
         <v>106.0164</v>
       </c>
     </row>
-    <row r="130" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G130">
         <v>1803.799</v>
       </c>
@@ -8337,7 +8328,7 @@
         <v>106.0008</v>
       </c>
     </row>
-    <row r="131" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G131">
         <v>1788.7460000000001</v>
       </c>
@@ -8345,7 +8336,7 @@
         <v>106.2757</v>
       </c>
     </row>
-    <row r="132" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G132">
         <v>1803.846</v>
       </c>
@@ -8353,7 +8344,7 @@
         <v>105.7705</v>
       </c>
     </row>
-    <row r="133" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G133">
         <v>1788.356</v>
       </c>
@@ -8361,7 +8352,7 @@
         <v>106.0813</v>
       </c>
     </row>
-    <row r="134" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G134">
         <v>1773.8130000000001</v>
       </c>
@@ -8369,7 +8360,7 @@
         <v>106.3004</v>
       </c>
     </row>
-    <row r="135" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G135">
         <v>1773.46</v>
       </c>
@@ -8377,7 +8368,7 @@
         <v>105.8387</v>
       </c>
     </row>
-    <row r="136" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G136">
         <v>1773.855</v>
       </c>
@@ -8385,7 +8376,7 @@
         <v>106.3312</v>
       </c>
     </row>
-    <row r="137" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G137">
         <v>1758.252</v>
       </c>
@@ -8393,7 +8384,7 @@
         <v>105.94289999999999</v>
       </c>
     </row>
-    <row r="138" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G138">
         <v>1758.42</v>
       </c>
@@ -8401,7 +8392,7 @@
         <v>105.88379999999999</v>
       </c>
     </row>
-    <row r="139" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G139">
         <v>1743.6389999999999</v>
       </c>
@@ -8409,7 +8400,7 @@
         <v>105.9689</v>
       </c>
     </row>
-    <row r="140" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G140">
         <v>1743.116</v>
       </c>
@@ -8417,7 +8408,7 @@
         <v>106.07550000000001</v>
       </c>
     </row>
-    <row r="141" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G141">
         <v>1743.41</v>
       </c>
@@ -8425,7 +8416,7 @@
         <v>105.9944</v>
       </c>
     </row>
-    <row r="142" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G142">
         <v>1758.229</v>
       </c>
@@ -8433,7 +8424,7 @@
         <v>105.9682</v>
       </c>
     </row>
-    <row r="143" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G143">
         <v>1758.6110000000001</v>
       </c>
@@ -8441,7 +8432,7 @@
         <v>106.0844</v>
       </c>
     </row>
-    <row r="144" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G144">
         <v>1758.502</v>
       </c>
@@ -8449,7 +8440,7 @@
         <v>106.253</v>
       </c>
     </row>
-    <row r="145" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G145">
         <v>1758.336</v>
       </c>
@@ -8457,7 +8448,7 @@
         <v>105.9712</v>
       </c>
     </row>
-    <row r="146" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G146">
         <v>1743.46</v>
       </c>
@@ -8465,7 +8456,7 @@
         <v>105.7208</v>
       </c>
     </row>
-    <row r="147" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G147">
         <v>1743.7249999999999</v>
       </c>
@@ -8473,7 +8464,7 @@
         <v>106.00369999999999</v>
       </c>
     </row>
-    <row r="148" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G148">
         <v>1743.2550000000001</v>
       </c>
@@ -8481,7 +8472,7 @@
         <v>105.74850000000001</v>
       </c>
     </row>
-    <row r="149" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G149">
         <v>1743.2</v>
       </c>
@@ -8489,7 +8480,7 @@
         <v>105.6892</v>
       </c>
     </row>
-    <row r="150" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G150">
         <v>1743.645</v>
       </c>
@@ -8497,7 +8488,7 @@
         <v>115.9367</v>
       </c>
     </row>
-    <row r="151" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G151">
         <v>1743.6010000000001</v>
       </c>
@@ -8505,7 +8496,7 @@
         <v>115.7723</v>
       </c>
     </row>
-    <row r="152" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G152">
         <v>1743.2650000000001</v>
       </c>
@@ -8513,7 +8504,7 @@
         <v>115.5065</v>
       </c>
     </row>
-    <row r="153" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G153">
         <v>1743.1210000000001</v>
       </c>
@@ -8521,7 +8512,7 @@
         <v>116.05670000000001</v>
       </c>
     </row>
-    <row r="154" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G154">
         <v>1743.5830000000001</v>
       </c>
@@ -8529,7 +8520,7 @@
         <v>115.9269</v>
       </c>
     </row>
-    <row r="155" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G155">
         <v>1743.1949999999999</v>
       </c>
@@ -8537,7 +8528,7 @@
         <v>115.9965</v>
       </c>
     </row>
-    <row r="156" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G156">
         <v>1758.404</v>
       </c>
@@ -8545,7 +8536,7 @@
         <v>115.4991</v>
       </c>
     </row>
-    <row r="157" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G157">
         <v>1743.6780000000001</v>
       </c>
@@ -8553,7 +8544,7 @@
         <v>115.5228</v>
       </c>
     </row>
-    <row r="158" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G158">
         <v>1743.75</v>
       </c>
@@ -8561,7 +8552,7 @@
         <v>115.83710000000001</v>
       </c>
     </row>
-    <row r="159" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G159">
         <v>1743.4010000000001</v>
       </c>
@@ -8569,7 +8560,7 @@
         <v>115.67700000000001</v>
       </c>
     </row>
-    <row r="160" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G160">
         <v>1758.3130000000001</v>
       </c>
@@ -8577,7 +8568,7 @@
         <v>115.5472</v>
       </c>
     </row>
-    <row r="161" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G161">
         <v>1758.4659999999999</v>
       </c>
@@ -8585,7 +8576,7 @@
         <v>116.02809999999999</v>
       </c>
     </row>
-    <row r="162" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G162">
         <v>1758.309</v>
       </c>
@@ -8593,7 +8584,7 @@
         <v>115.7191</v>
       </c>
     </row>
-    <row r="163" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G163">
         <v>1758.383</v>
       </c>
@@ -8601,7 +8592,7 @@
         <v>115.8503</v>
       </c>
     </row>
-    <row r="164" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G164">
         <v>1758.7819999999999</v>
       </c>
@@ -8609,7 +8600,7 @@
         <v>116.01349999999999</v>
       </c>
     </row>
-    <row r="165" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G165">
         <v>1788.462</v>
       </c>
@@ -8617,7 +8608,7 @@
         <v>116.0718</v>
       </c>
     </row>
-    <row r="166" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G166">
         <v>1804.0540000000001</v>
       </c>
@@ -8625,7 +8616,7 @@
         <v>115.88200000000001</v>
       </c>
     </row>
-    <row r="167" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G167">
         <v>1804.001</v>
       </c>
@@ -8633,7 +8624,7 @@
         <v>115.82640000000001</v>
       </c>
     </row>
-    <row r="168" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G168">
         <v>1818.5730000000001</v>
       </c>
@@ -8641,7 +8632,7 @@
         <v>116.0414</v>
       </c>
     </row>
-    <row r="169" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G169">
         <v>1818.624</v>
       </c>
@@ -8649,7 +8640,7 @@
         <v>115.7786</v>
       </c>
     </row>
-    <row r="170" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G170">
         <v>1818.7860000000001</v>
       </c>
@@ -8657,7 +8648,7 @@
         <v>115.92440000000001</v>
       </c>
     </row>
-    <row r="171" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G171">
         <v>1834.075</v>
       </c>
@@ -8665,7 +8656,7 @@
         <v>116.0988</v>
       </c>
     </row>
-    <row r="172" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G172">
         <v>1834.6020000000001</v>
       </c>
@@ -8673,7 +8664,7 @@
         <v>115.9281</v>
       </c>
     </row>
-    <row r="173" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G173">
         <v>1834.0730000000001</v>
       </c>
@@ -8681,7 +8672,7 @@
         <v>115.8377</v>
       </c>
     </row>
-    <row r="174" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G174">
         <v>1834.4480000000001</v>
       </c>
@@ -8689,7 +8680,7 @@
         <v>116.0936</v>
       </c>
     </row>
-    <row r="175" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G175">
         <v>1834.4960000000001</v>
       </c>
@@ -8697,7 +8688,7 @@
         <v>115.8402</v>
       </c>
     </row>
-    <row r="176" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G176">
         <v>1849.4380000000001</v>
       </c>
@@ -8705,7 +8696,7 @@
         <v>116.17019999999999</v>
       </c>
     </row>
-    <row r="177" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G177">
         <v>1864.201</v>
       </c>
@@ -8713,7 +8704,7 @@
         <v>115.6253</v>
       </c>
     </row>
-    <row r="178" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G178">
         <v>1864.7149999999999</v>
       </c>
@@ -8721,7 +8712,7 @@
         <v>116.0719</v>
       </c>
     </row>
-    <row r="179" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G179">
         <v>1879.3689999999999</v>
       </c>
@@ -8729,7 +8720,7 @@
         <v>116.3058</v>
       </c>
     </row>
-    <row r="180" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G180">
         <v>1894.5129999999999</v>
       </c>
@@ -8737,7 +8728,7 @@
         <v>115.8853</v>
       </c>
     </row>
-    <row r="181" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G181">
         <v>1894.61</v>
       </c>
@@ -8745,7 +8736,7 @@
         <v>116.38339999999999</v>
       </c>
     </row>
-    <row r="182" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G182">
         <v>1895.0039999999999</v>
       </c>
@@ -8753,7 +8744,7 @@
         <v>116.1009</v>
       </c>
     </row>
-    <row r="183" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G183">
         <v>1909.9960000000001</v>
       </c>
@@ -8761,7 +8752,7 @@
         <v>126.40130000000001</v>
       </c>
     </row>
-    <row r="184" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G184">
         <v>1909.953</v>
       </c>
@@ -8769,7 +8760,7 @@
         <v>115.6763</v>
       </c>
     </row>
-    <row r="185" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G185">
         <v>1909.9480000000001</v>
       </c>
@@ -8777,7 +8768,7 @@
         <v>128.953</v>
       </c>
     </row>
-    <row r="186" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G186">
         <v>1925.124</v>
       </c>
@@ -8785,7 +8776,7 @@
         <v>115.9194</v>
       </c>
     </row>
-    <row r="187" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G187">
         <v>1924.905</v>
       </c>
@@ -8793,7 +8784,7 @@
         <v>131.6455</v>
       </c>
     </row>
-    <row r="188" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G188">
         <v>1939.692</v>
       </c>
@@ -8801,7 +8792,7 @@
         <v>115.86109999999999</v>
       </c>
     </row>
-    <row r="189" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G189">
         <v>1939.9169999999999</v>
       </c>
@@ -8809,7 +8800,7 @@
         <v>115.68819999999999</v>
       </c>
     </row>
-    <row r="190" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G190">
         <v>1955.596</v>
       </c>
@@ -8817,7 +8808,7 @@
         <v>116.19329999999999</v>
       </c>
     </row>
-    <row r="191" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G191">
         <v>1970.683</v>
       </c>
@@ -8825,7 +8816,7 @@
         <v>116.134</v>
       </c>
     </row>
-    <row r="192" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G192">
         <v>1970.617</v>
       </c>
@@ -8833,7 +8824,7 @@
         <v>116.1763</v>
       </c>
     </row>
-    <row r="193" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G193">
         <v>1970.1420000000001</v>
       </c>
@@ -8841,7 +8832,7 @@
         <v>116.0438</v>
       </c>
     </row>
-    <row r="194" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G194">
         <v>1985.317</v>
       </c>
@@ -8849,7 +8840,7 @@
         <v>115.9259</v>
       </c>
     </row>
-    <row r="195" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G195">
         <v>1985.1020000000001</v>
       </c>
@@ -8857,7 +8848,7 @@
         <v>116.0008</v>
       </c>
     </row>
-    <row r="196" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G196">
         <v>2000.7739999999999</v>
       </c>
@@ -8865,7 +8856,7 @@
         <v>116.0121</v>
       </c>
     </row>
-    <row r="197" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G197">
         <v>2000.3019999999999</v>
       </c>
@@ -8873,7 +8864,7 @@
         <v>115.7264</v>
       </c>
     </row>
-    <row r="198" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G198">
         <v>2015.693</v>
       </c>
@@ -8881,7 +8872,7 @@
         <v>115.9374</v>
       </c>
     </row>
-    <row r="199" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G199">
         <v>2030.57</v>
       </c>
@@ -8889,7 +8880,7 @@
         <v>115.91459999999999</v>
       </c>
     </row>
-    <row r="200" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G200">
         <v>2046.1120000000001</v>
       </c>
@@ -8897,7 +8888,7 @@
         <v>115.63939999999999</v>
       </c>
     </row>
-    <row r="201" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G201">
         <v>2076.0819999999999</v>
       </c>
@@ -8905,7 +8896,7 @@
         <v>116.1581</v>
       </c>
     </row>
-    <row r="202" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G202">
         <v>2091.7159999999999</v>
       </c>
@@ -8913,7 +8904,7 @@
         <v>115.8416</v>
       </c>
     </row>
-    <row r="203" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G203">
         <v>2106.19</v>
       </c>
@@ -8921,7 +8912,7 @@
         <v>115.8566</v>
       </c>
     </row>
-    <row r="204" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G204">
         <v>2106.2840000000001</v>
       </c>
@@ -8929,7 +8920,7 @@
         <v>115.8509</v>
       </c>
     </row>
-    <row r="205" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G205">
         <v>2121.7220000000002</v>
       </c>
@@ -8937,7 +8928,7 @@
         <v>115.8514</v>
       </c>
     </row>
-    <row r="206" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G206">
         <v>2136.712</v>
       </c>
@@ -8945,7 +8936,7 @@
         <v>125.86709999999999</v>
       </c>
     </row>
-    <row r="207" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G207">
         <v>2136.752</v>
       </c>
@@ -8953,7 +8944,7 @@
         <v>125.4483</v>
       </c>
     </row>
-    <row r="208" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G208">
         <v>2136.913</v>
       </c>
@@ -8961,7 +8952,7 @@
         <v>125.4024</v>
       </c>
     </row>
-    <row r="209" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G209">
         <v>2167.261</v>
       </c>
@@ -8969,7 +8960,7 @@
         <v>125.7238</v>
       </c>
     </row>
-    <row r="210" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G210">
         <v>2181.7249999999999</v>
       </c>
@@ -8977,7 +8968,7 @@
         <v>125.682</v>
       </c>
     </row>
-    <row r="211" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G211">
         <v>2182.0329999999999</v>
       </c>
@@ -8985,7 +8976,7 @@
         <v>125.6857</v>
       </c>
     </row>
-    <row r="212" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G212">
         <v>2197.1640000000002</v>
       </c>
@@ -8993,7 +8984,7 @@
         <v>125.4738</v>
       </c>
     </row>
-    <row r="213" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G213">
         <v>2212.6770000000001</v>
       </c>
@@ -9001,7 +8992,7 @@
         <v>125.9331</v>
       </c>
     </row>
-    <row r="214" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G214">
         <v>2227.3980000000001</v>
       </c>
@@ -9009,7 +9000,7 @@
         <v>125.37139999999999</v>
       </c>
     </row>
-    <row r="215" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G215">
         <v>2242.422</v>
       </c>
@@ -9017,7 +9008,7 @@
         <v>125.9153</v>
       </c>
     </row>
-    <row r="216" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G216">
         <v>2257.8890000000001</v>
       </c>
@@ -9025,7 +9016,7 @@
         <v>125.6576</v>
       </c>
     </row>
-    <row r="217" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G217">
         <v>2272.59</v>
       </c>
@@ -9033,7 +9024,7 @@
         <v>125.5729</v>
       </c>
     </row>
-    <row r="218" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G218">
         <v>2288.2159999999999</v>
       </c>
@@ -9041,7 +9032,7 @@
         <v>125.9589</v>
       </c>
     </row>
-    <row r="219" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G219">
         <v>2302.7950000000001</v>
       </c>
@@ -9049,7 +9040,7 @@
         <v>135.2037</v>
       </c>
     </row>
-    <row r="220" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G220">
         <v>2318.6460000000002</v>
       </c>
@@ -9057,7 +9048,7 @@
         <v>135.52789999999999</v>
       </c>
     </row>
-    <row r="221" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G221">
         <v>2333.2890000000002</v>
       </c>
@@ -9065,7 +9056,7 @@
         <v>135.4736</v>
       </c>
     </row>
-    <row r="222" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G222">
         <v>2348.8989999999999</v>
       </c>
@@ -9073,7 +9064,7 @@
         <v>135.52209999999999</v>
       </c>
     </row>
-    <row r="223" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G223">
         <v>2363.453</v>
       </c>
@@ -9081,7 +9072,7 @@
         <v>135.203</v>
       </c>
     </row>
-    <row r="224" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G224">
         <v>2379.2429999999999</v>
       </c>
@@ -9089,7 +9080,7 @@
         <v>135.62870000000001</v>
       </c>
     </row>
-    <row r="225" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G225">
         <v>2378.7959999999998</v>
       </c>
@@ -9097,7 +9088,7 @@
         <v>135.7516</v>
       </c>
     </row>
-    <row r="226" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G226">
         <v>2379.1619999999998</v>
       </c>
@@ -9105,7 +9096,7 @@
         <v>135.196</v>
       </c>
     </row>
-    <row r="227" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G227">
         <v>2363.471</v>
       </c>
@@ -9113,7 +9104,7 @@
         <v>135.72149999999999</v>
       </c>
     </row>
-    <row r="228" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G228">
         <v>2318.3110000000001</v>
       </c>
@@ -9121,7 +9112,7 @@
         <v>135.15219999999999</v>
       </c>
     </row>
-    <row r="229" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G229">
         <v>2303.3679999999999</v>
       </c>
@@ -9129,7 +9120,7 @@
         <v>135.52850000000001</v>
       </c>
     </row>
-    <row r="230" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G230">
         <v>2303.4119999999998</v>
       </c>
@@ -9137,7 +9128,7 @@
         <v>135.50040000000001</v>
       </c>
     </row>
-    <row r="231" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G231">
         <v>2272.797</v>
       </c>
@@ -9145,7 +9136,7 @@
         <v>135.14279999999999</v>
       </c>
     </row>
-    <row r="232" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G232">
         <v>2257.855</v>
       </c>
@@ -9153,7 +9144,7 @@
         <v>135.7586</v>
       </c>
     </row>
-    <row r="233" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G233">
         <v>2257.732</v>
       </c>
@@ -9161,7 +9152,7 @@
         <v>135.2062</v>
       </c>
     </row>
-    <row r="234" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G234">
         <v>2243.0100000000002</v>
       </c>
@@ -9169,7 +9160,7 @@
         <v>135.19049999999999</v>
       </c>
     </row>
-    <row r="235" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G235">
         <v>2227.8380000000002</v>
       </c>
@@ -9177,7 +9168,7 @@
         <v>135.5018</v>
       </c>
     </row>
-    <row r="236" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G236">
         <v>2227.8609999999999</v>
       </c>
@@ -9185,7 +9176,7 @@
         <v>135.70230000000001</v>
       </c>
     </row>
-    <row r="237" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G237">
         <v>2227.7280000000001</v>
       </c>
@@ -9193,7 +9184,7 @@
         <v>135.14320000000001</v>
       </c>
     </row>
-    <row r="238" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G238">
         <v>2212.5929999999998</v>
       </c>
@@ -9201,7 +9192,7 @@
         <v>135.9186</v>
       </c>
     </row>
-    <row r="239" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G239">
         <v>2212.4630000000002</v>
       </c>
@@ -9209,7 +9200,7 @@
         <v>135.1687</v>
       </c>
     </row>
-    <row r="240" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G240">
         <v>2197.69</v>
       </c>
@@ -9217,7 +9208,7 @@
         <v>136.13910000000001</v>
       </c>
     </row>
-    <row r="241" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G241">
         <v>2197.442</v>
       </c>
@@ -9225,7 +9216,7 @@
         <v>135.43340000000001</v>
       </c>
     </row>
-    <row r="242" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G242">
         <v>2197.8220000000001</v>
       </c>
@@ -9233,7 +9224,7 @@
         <v>146.0427</v>
       </c>
     </row>
-    <row r="243" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G243">
         <v>2181.6410000000001</v>
       </c>
@@ -9241,7 +9232,7 @@
         <v>135.41380000000001</v>
       </c>
     </row>
-    <row r="244" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G244">
         <v>2181.77</v>
       </c>
@@ -9249,7 +9240,7 @@
         <v>148.27549999999999</v>
       </c>
     </row>
-    <row r="245" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G245">
         <v>2182.2109999999998</v>
       </c>
@@ -9257,7 +9248,7 @@
         <v>135.7269</v>
       </c>
     </row>
-    <row r="246" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G246">
         <v>2166.9209999999998</v>
       </c>
@@ -9265,7 +9256,7 @@
         <v>150.4016</v>
       </c>
     </row>
-    <row r="247" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G247">
         <v>2167.4630000000002</v>
       </c>
@@ -9273,7 +9264,7 @@
         <v>135.68629999999999</v>
       </c>
     </row>
-    <row r="248" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G248">
         <v>2166.9349999999999</v>
       </c>
@@ -9281,7 +9272,7 @@
         <v>149.3246</v>
       </c>
     </row>
-    <row r="249" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G249">
         <v>2152.0659999999998</v>
       </c>
@@ -9289,7 +9280,7 @@
         <v>135.16829999999999</v>
       </c>
     </row>
-    <row r="250" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G250">
         <v>2151.8969999999999</v>
       </c>
@@ -9297,7 +9288,7 @@
         <v>135.63730000000001</v>
       </c>
     </row>
-    <row r="251" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G251">
         <v>2151.701</v>
       </c>
@@ -9305,7 +9296,7 @@
         <v>135.42089999999999</v>
       </c>
     </row>
-    <row r="252" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G252">
         <v>2152.1179999999999</v>
       </c>
@@ -9313,7 +9304,7 @@
         <v>135.44110000000001</v>
       </c>
     </row>
-    <row r="253" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G253">
         <v>2137.1120000000001</v>
       </c>
@@ -9321,7 +9312,7 @@
         <v>135.73140000000001</v>
       </c>
     </row>
-    <row r="254" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G254">
         <v>2152.1480000000001</v>
       </c>
@@ -9329,7 +9320,7 @@
         <v>135.52979999999999</v>
       </c>
     </row>
-    <row r="255" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G255">
         <v>2136.7139999999999</v>
       </c>
@@ -9337,7 +9328,7 @@
         <v>135.16589999999999</v>
       </c>
     </row>
-    <row r="256" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G256">
         <v>2136.7220000000002</v>
       </c>
@@ -9345,7 +9336,7 @@
         <v>135.43109999999999</v>
       </c>
     </row>
-    <row r="257" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G257">
         <v>2137.1190000000001</v>
       </c>
@@ -9353,7 +9344,7 @@
         <v>135.6944</v>
       </c>
     </row>
-    <row r="258" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G258">
         <v>2137.2060000000001</v>
       </c>
@@ -9361,7 +9352,7 @@
         <v>135.5111</v>
       </c>
     </row>
-    <row r="259" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G259">
         <v>2137.136</v>
       </c>
@@ -9369,7 +9360,7 @@
         <v>135.74529999999999</v>
       </c>
     </row>
-    <row r="260" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G260">
         <v>2136.998</v>
       </c>
@@ -9377,7 +9368,7 @@
         <v>135.589</v>
       </c>
     </row>
-    <row r="261" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G261">
         <v>2137.0430000000001</v>
       </c>
@@ -9385,7 +9376,7 @@
         <v>135.4787</v>
       </c>
     </row>
-    <row r="262" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G262">
         <v>2136.9940000000001</v>
       </c>
@@ -9393,7 +9384,7 @@
         <v>135.501</v>
       </c>
     </row>
-    <row r="263" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G263">
         <v>2151.7600000000002</v>
       </c>
@@ -9401,7 +9392,7 @@
         <v>135.68340000000001</v>
       </c>
     </row>
-    <row r="264" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G264">
         <v>2136.674</v>
       </c>
@@ -9409,7 +9400,7 @@
         <v>135.40479999999999</v>
       </c>
     </row>
-    <row r="265" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G265">
         <v>2151.973</v>
       </c>
@@ -9417,7 +9408,7 @@
         <v>135.34440000000001</v>
       </c>
     </row>
-    <row r="266" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G266">
         <v>2151.9319999999998</v>
       </c>
@@ -9425,7 +9416,7 @@
         <v>135.4581</v>
       </c>
     </row>
-    <row r="267" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G267">
         <v>2151.9209999999998</v>
       </c>
@@ -9433,7 +9424,7 @@
         <v>135.1977</v>
       </c>
     </row>
-    <row r="268" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G268">
         <v>2151.9989999999998</v>
       </c>
@@ -9441,7 +9432,7 @@
         <v>135.34399999999999</v>
       </c>
     </row>
-    <row r="269" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G269">
         <v>2166.6460000000002</v>
       </c>
@@ -9449,7 +9440,7 @@
         <v>135.76349999999999</v>
       </c>
     </row>
-    <row r="270" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G270">
         <v>2152.134</v>
       </c>
@@ -9457,7 +9448,7 @@
         <v>135.49199999999999</v>
       </c>
     </row>
-    <row r="271" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G271">
         <v>2167.125</v>
       </c>
@@ -9465,7 +9456,7 @@
         <v>135.47919999999999</v>
       </c>
     </row>
-    <row r="272" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G272">
         <v>2166.8739999999998</v>
       </c>
@@ -9473,7 +9464,7 @@
         <v>135.7834</v>
       </c>
     </row>
-    <row r="273" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="273" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G273">
         <v>2182.17</v>
       </c>
@@ -9481,7 +9472,7 @@
         <v>135.50450000000001</v>
       </c>
     </row>
-    <row r="274" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="274" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G274">
         <v>2182.067</v>
       </c>
@@ -9489,7 +9480,7 @@
         <v>135.22200000000001</v>
       </c>
     </row>
-    <row r="275" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G275">
         <v>2197.5309999999999</v>
       </c>
@@ -9497,7 +9488,7 @@
         <v>135.49209999999999</v>
       </c>
     </row>
-    <row r="276" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G276">
         <v>2197.299</v>
       </c>
@@ -9505,7 +9496,7 @@
         <v>135.19800000000001</v>
       </c>
     </row>
-    <row r="277" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G277">
         <v>2212.5549999999998</v>
       </c>
@@ -9513,7 +9504,7 @@
         <v>135.47669999999999</v>
       </c>
     </row>
-    <row r="278" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G278">
         <v>2227.5909999999999</v>
       </c>
@@ -9521,7 +9512,7 @@
         <v>135.24359999999999</v>
       </c>
     </row>
-    <row r="279" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="279" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G279">
         <v>2242.674</v>
       </c>
@@ -9529,7 +9520,7 @@
         <v>135.78200000000001</v>
       </c>
     </row>
-    <row r="280" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="280" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G280">
         <v>2242.6320000000001</v>
       </c>
@@ -9537,7 +9528,7 @@
         <v>135.61869999999999</v>
       </c>
     </row>
-    <row r="281" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G281">
         <v>2257.8119999999999</v>
       </c>
@@ -9545,7 +9536,7 @@
         <v>135.5112</v>
       </c>
     </row>
-    <row r="282" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="282" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G282">
         <v>2257.9879999999998</v>
       </c>
@@ -9553,7 +9544,7 @@
         <v>135.25960000000001</v>
       </c>
     </row>
-    <row r="283" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="283" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G283">
         <v>2273.31</v>
       </c>
@@ -9561,7 +9552,7 @@
         <v>135.57429999999999</v>
       </c>
     </row>
-    <row r="284" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="284" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G284">
         <v>2272.7620000000002</v>
       </c>
@@ -9569,7 +9560,7 @@
         <v>135.48140000000001</v>
       </c>
     </row>
-    <row r="285" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="285" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G285">
         <v>2272.7910000000002</v>
       </c>
@@ -9577,7 +9568,7 @@
         <v>135.24860000000001</v>
       </c>
     </row>
-    <row r="286" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="286" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G286">
         <v>2303.0889999999999</v>
       </c>
@@ -9585,7 +9576,7 @@
         <v>135.2543</v>
       </c>
     </row>
-    <row r="287" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="287" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G287">
         <v>2318.8209999999999</v>
       </c>
@@ -9593,7 +9584,7 @@
         <v>135.78460000000001</v>
       </c>
     </row>
-    <row r="288" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="288" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G288">
         <v>2334.0030000000002</v>
       </c>
@@ -9601,7 +9592,7 @@
         <v>135.56190000000001</v>
       </c>
     </row>
-    <row r="289" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G289">
         <v>2348.922</v>
       </c>
@@ -9609,7 +9600,7 @@
         <v>135.61609999999999</v>
       </c>
     </row>
-    <row r="290" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="290" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G290">
         <v>2348.8249999999998</v>
       </c>
@@ -9617,7 +9608,7 @@
         <v>135.52010000000001</v>
       </c>
     </row>
-    <row r="291" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G291">
         <v>2348.7159999999999</v>
       </c>
@@ -9625,7 +9616,7 @@
         <v>135.76300000000001</v>
       </c>
     </row>
-    <row r="292" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G292">
         <v>2363.6129999999998</v>
       </c>
@@ -9633,7 +9624,7 @@
         <v>135.53290000000001</v>
       </c>
     </row>
-    <row r="293" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="293" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G293">
         <v>2378.8510000000001</v>
       </c>
@@ -9641,7 +9632,7 @@
         <v>135.28210000000001</v>
       </c>
     </row>
-    <row r="294" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="294" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G294">
         <v>2379.19</v>
       </c>
@@ -9649,7 +9640,7 @@
         <v>135.48609999999999</v>
       </c>
     </row>
-    <row r="295" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="295" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G295">
         <v>2394.2730000000001</v>
       </c>
@@ -9657,7 +9648,7 @@
         <v>135.55950000000001</v>
       </c>
     </row>
-    <row r="296" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="296" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G296">
         <v>2393.9299999999998</v>
       </c>
@@ -9665,7 +9656,7 @@
         <v>135.2533</v>
       </c>
     </row>
-    <row r="297" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="297" spans="7:8" x14ac:dyDescent="0.75">
       <c r="G297">
         <v>2394.2550000000001</v>
       </c>
@@ -9689,6 +9680,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0ed78115-f4df-42b0-9376-ad3306022cc8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100205AA101E2883C419D53A6EAA58BE6E4" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0732453c88b6c24a50b901808cd2a95">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0ed78115-f4df-42b0-9376-ad3306022cc8" xmlns:ns4="94b7f148-c09a-42e6-baca-973a9a7cd962" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c3ce456d5e9a668ce7bebc57d13ab49" ns3:_="" ns4:_="">
     <xsd:import namespace="0ed78115-f4df-42b0-9376-ad3306022cc8"/>
@@ -9941,14 +9940,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0ed78115-f4df-42b0-9376-ad3306022cc8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7D38091-7891-4922-BDA4-DDCC3109030A}">
   <ds:schemaRefs>
@@ -9958,6 +9949,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE3CDB75-004F-4418-A9D1-0A5E1B428212}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="0ed78115-f4df-42b0-9376-ad3306022cc8"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="94b7f148-c09a-42e6-baca-973a9a7cd962"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88B5DFD5-AF32-4053-8117-B9F97580063E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9974,21 +9982,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE3CDB75-004F-4418-A9D1-0A5E1B428212}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="0ed78115-f4df-42b0-9376-ad3306022cc8"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="94b7f148-c09a-42e6-baca-973a9a7cd962"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed the shimadzu code. I think
</commit_message>
<xml_diff>
--- a/01_Raw_data/RC log.xlsx
+++ b/01_Raw_data/RC log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Howley_Bradford_Streams\Howley_Bradford_Streams\01_Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435A66C9-1E26-4E9F-8BB3-E7D1C03548D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0711D6A-DDC6-40FA-B225-2DCAF2780976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9525" yWindow="0" windowWidth="9750" windowHeight="10155" xr2:uid="{A079E74B-2391-4069-81A1-6515CCD90540}"/>
+    <workbookView xWindow="-28920" yWindow="3405" windowWidth="29040" windowHeight="15720" xr2:uid="{A079E74B-2391-4069-81A1-6515CCD90540}"/>
   </bookViews>
   <sheets>
     <sheet name="RC log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -3708,20 +3708,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04E7760-F87C-4D84-A63F-D473D279D553}">
-  <dimension ref="A1:K163"/>
+  <dimension ref="A1:K180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K165" sqref="K165"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R174" sqref="R174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="9.40625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.31640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.1328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.75">
@@ -3747,16 +3747,16 @@
         <v>30</v>
       </c>
       <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>26</v>
-      </c>
-      <c r="K1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.75">
@@ -3780,10 +3780,10 @@
         <v>-1.34</v>
       </c>
       <c r="H2">
+        <v>26</v>
+      </c>
+      <c r="I2">
         <v>5.41</v>
-      </c>
-      <c r="K2">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.75">
@@ -3807,10 +3807,10 @@
         <v>-1.05</v>
       </c>
       <c r="H3">
+        <v>26</v>
+      </c>
+      <c r="I3">
         <v>5.8</v>
-      </c>
-      <c r="K3">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.75">
@@ -3834,10 +3834,10 @@
         <v>-0.495</v>
       </c>
       <c r="H4">
+        <v>26</v>
+      </c>
+      <c r="I4">
         <v>6.1</v>
-      </c>
-      <c r="K4">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.75">
@@ -3861,10 +3861,10 @@
         <v>-1.39</v>
       </c>
       <c r="H5">
+        <v>26</v>
+      </c>
+      <c r="I5">
         <v>6.67</v>
-      </c>
-      <c r="K5">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.75">
@@ -3888,10 +3888,10 @@
         <v>-0.10999999999999999</v>
       </c>
       <c r="H6">
+        <v>26</v>
+      </c>
+      <c r="I6">
         <v>6.2</v>
-      </c>
-      <c r="K6">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.75">
@@ -3914,11 +3914,11 @@
         <f>Sheet1!F7-'RC log'!F7</f>
         <v>-1.26</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7">
+        <v>26</v>
+      </c>
+      <c r="I7" t="s">
         <v>12</v>
-      </c>
-      <c r="K7">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.75">
@@ -3941,11 +3941,11 @@
         <f>Sheet1!F8-'RC log'!F8</f>
         <v>0</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
         <v>12</v>
-      </c>
-      <c r="K8">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.75">
@@ -3969,10 +3969,10 @@
         <v>-1.0499999999999998</v>
       </c>
       <c r="H9">
+        <v>26</v>
+      </c>
+      <c r="I9">
         <v>4.76</v>
-      </c>
-      <c r="K9">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.75">
@@ -3996,10 +3996,10 @@
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="H10">
+        <v>26</v>
+      </c>
+      <c r="I10">
         <v>4.5999999999999996</v>
-      </c>
-      <c r="K10">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.75">
@@ -4023,10 +4023,10 @@
         <v>-1.42</v>
       </c>
       <c r="H11">
+        <v>26</v>
+      </c>
+      <c r="I11">
         <v>5.0999999999999996</v>
-      </c>
-      <c r="K11">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.75">
@@ -4050,10 +4050,10 @@
         <v>0.36000000000000004</v>
       </c>
       <c r="H12">
+        <v>26</v>
+      </c>
+      <c r="I12">
         <v>4.7</v>
-      </c>
-      <c r="K12">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.75">
@@ -4076,7 +4076,7 @@
         <f>Sheet1!F13-'RC log'!F13</f>
         <v>-1.17</v>
       </c>
-      <c r="K13">
+      <c r="H13">
         <v>26</v>
       </c>
     </row>
@@ -4101,10 +4101,10 @@
         <v>-0.30500000000000005</v>
       </c>
       <c r="H14">
+        <v>26</v>
+      </c>
+      <c r="I14">
         <v>4.7699999999999996</v>
-      </c>
-      <c r="K14">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.75">
@@ -4128,10 +4128,10 @@
         <v>-0.83</v>
       </c>
       <c r="H15">
+        <v>26</v>
+      </c>
+      <c r="I15">
         <v>4.72</v>
-      </c>
-      <c r="K15">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.75">
@@ -4155,13 +4155,13 @@
         <v>-1.4100000000000001</v>
       </c>
       <c r="H16">
+        <v>26</v>
+      </c>
+      <c r="I16">
         <v>4.84</v>
       </c>
-      <c r="K16">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A17" s="1">
         <v>45400</v>
       </c>
@@ -4182,13 +4182,13 @@
         <v>-0.81499999999999995</v>
       </c>
       <c r="H17">
+        <v>26</v>
+      </c>
+      <c r="I17">
         <v>5.1870000000000003</v>
       </c>
-      <c r="K17">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A18" s="1">
         <v>45420</v>
       </c>
@@ -4211,14 +4211,14 @@
         <f>Sheet1!F18-'RC log'!F18</f>
         <v>-1.03</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18">
+        <v>26</v>
+      </c>
+      <c r="I18" t="s">
         <v>12</v>
       </c>
-      <c r="K18">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A19" s="1">
         <v>45420</v>
       </c>
@@ -4242,13 +4242,13 @@
         <v>-0.28999999999999998</v>
       </c>
       <c r="H19">
+        <v>26</v>
+      </c>
+      <c r="I19">
         <v>5.36</v>
       </c>
-      <c r="K19">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A20" s="1">
         <v>45420</v>
       </c>
@@ -4272,13 +4272,13 @@
         <v>0.28500000000000003</v>
       </c>
       <c r="H20">
+        <v>26</v>
+      </c>
+      <c r="I20">
         <v>5.024</v>
       </c>
-      <c r="K20">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A21" s="1">
         <v>45420</v>
       </c>
@@ -4302,13 +4302,13 @@
         <v>-0.82000000000000006</v>
       </c>
       <c r="H21">
+        <v>26</v>
+      </c>
+      <c r="I21">
         <v>6.36</v>
       </c>
-      <c r="K21">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A22" s="1">
         <v>45420</v>
       </c>
@@ -4332,13 +4332,13 @@
         <v>0.34</v>
       </c>
       <c r="H22">
+        <v>26</v>
+      </c>
+      <c r="I22">
         <v>4.7</v>
       </c>
-      <c r="K22">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A23" s="1">
         <v>45420</v>
       </c>
@@ -4362,13 +4362,13 @@
         <v>-0.94</v>
       </c>
       <c r="H23">
+        <v>26</v>
+      </c>
+      <c r="I23">
         <v>4.9000000000000004</v>
       </c>
-      <c r="K23">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A24" s="1">
         <v>45420</v>
       </c>
@@ -4391,14 +4391,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24">
+        <v>26</v>
+      </c>
+      <c r="I24" t="s">
         <v>12</v>
       </c>
-      <c r="K24">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A25" s="1">
         <v>45420</v>
       </c>
@@ -4421,14 +4421,14 @@
         <f t="shared" si="0"/>
         <v>-0.55000000000000004</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25">
+        <v>26</v>
+      </c>
+      <c r="I25" t="s">
         <v>12</v>
       </c>
-      <c r="K25">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A26" s="1">
         <v>45420</v>
       </c>
@@ -4452,13 +4452,13 @@
         <v>0.35</v>
       </c>
       <c r="H26">
+        <v>26</v>
+      </c>
+      <c r="I26">
         <v>4.4000000000000004</v>
       </c>
-      <c r="K26">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A27" s="1">
         <v>45420</v>
       </c>
@@ -4481,14 +4481,14 @@
         <f t="shared" si="0"/>
         <v>-1.07</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27">
+        <v>26</v>
+      </c>
+      <c r="I27" t="s">
         <v>12</v>
       </c>
-      <c r="K27">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A28" s="1">
         <v>45420</v>
       </c>
@@ -4511,14 +4511,14 @@
         <f t="shared" si="0"/>
         <v>0.12000000000000011</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28">
+        <v>26</v>
+      </c>
+      <c r="I28" t="s">
         <v>12</v>
       </c>
-      <c r="K28">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A29" s="1">
         <v>45420</v>
       </c>
@@ -4542,13 +4542,13 @@
         <v>-0.8899999999999999</v>
       </c>
       <c r="H29">
+        <v>26</v>
+      </c>
+      <c r="I29">
         <v>5.8</v>
       </c>
-      <c r="K29">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A30" s="1">
         <v>45420</v>
       </c>
@@ -4572,13 +4572,13 @@
         <v>-0.40500000000000003</v>
       </c>
       <c r="H30">
+        <v>26</v>
+      </c>
+      <c r="I30">
         <v>5</v>
       </c>
-      <c r="K30">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A31" s="1">
         <v>45420</v>
       </c>
@@ -4602,13 +4602,13 @@
         <v>-0.93</v>
       </c>
       <c r="H31">
+        <v>26</v>
+      </c>
+      <c r="I31">
         <v>4.7699999999999996</v>
       </c>
-      <c r="K31">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A32" s="1">
         <v>45420</v>
       </c>
@@ -4632,13 +4632,13 @@
         <v>-0.76999999999999991</v>
       </c>
       <c r="H32">
+        <v>26</v>
+      </c>
+      <c r="I32">
         <v>4.42</v>
       </c>
-      <c r="K32">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A33" s="1">
         <v>45420</v>
       </c>
@@ -4662,13 +4662,13 @@
         <v>-0.99500000000000011</v>
       </c>
       <c r="H33">
+        <v>26</v>
+      </c>
+      <c r="I33">
         <v>4.74</v>
       </c>
-      <c r="K33">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A34" s="1">
         <v>45442</v>
       </c>
@@ -4691,14 +4691,14 @@
         <f t="shared" si="0"/>
         <v>-0.83000000000000007</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34">
+        <v>26</v>
+      </c>
+      <c r="I34" t="s">
         <v>12</v>
       </c>
-      <c r="K34">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A35" s="1">
         <v>45442</v>
       </c>
@@ -4722,13 +4722,13 @@
         <v>-0.35000000000000003</v>
       </c>
       <c r="H35">
+        <v>26</v>
+      </c>
+      <c r="I35">
         <v>6.4</v>
       </c>
-      <c r="K35">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A36" s="1">
         <v>45442</v>
       </c>
@@ -4752,13 +4752,13 @@
         <v>0.22499999999999998</v>
       </c>
       <c r="H36">
+        <v>26</v>
+      </c>
+      <c r="I36">
         <v>6.8</v>
       </c>
-      <c r="K36">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A37" s="1">
         <v>45442</v>
       </c>
@@ -4782,13 +4782,13 @@
         <v>-0.8600000000000001</v>
       </c>
       <c r="H37">
+        <v>26</v>
+      </c>
+      <c r="I37">
         <v>6.35</v>
       </c>
-      <c r="K37">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A38" s="1">
         <v>45442</v>
       </c>
@@ -4812,13 +4812,13 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="H38">
+        <v>26</v>
+      </c>
+      <c r="I38">
         <v>6.13</v>
       </c>
-      <c r="K38">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A39" s="1">
         <v>45442</v>
       </c>
@@ -4842,13 +4842,13 @@
         <v>-0.94</v>
       </c>
       <c r="H39">
+        <v>26</v>
+      </c>
+      <c r="I39">
         <v>5.66</v>
       </c>
-      <c r="K39">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A40" s="1">
         <v>45442</v>
       </c>
@@ -4871,14 +4871,14 @@
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40">
+        <v>26</v>
+      </c>
+      <c r="I40" t="s">
         <v>12</v>
       </c>
-      <c r="K40">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A41" s="1">
         <v>45442</v>
       </c>
@@ -4901,14 +4901,14 @@
         <f t="shared" si="0"/>
         <v>-1.0289999999999999</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41">
+        <v>26</v>
+      </c>
+      <c r="I41" t="s">
         <v>12</v>
       </c>
-      <c r="K41">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A42" s="1">
         <v>45442</v>
       </c>
@@ -4931,14 +4931,14 @@
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42">
+        <v>26</v>
+      </c>
+      <c r="I42" t="s">
         <v>12</v>
       </c>
-      <c r="K42">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A43" s="1">
         <v>45442</v>
       </c>
@@ -4961,14 +4961,14 @@
         <f t="shared" si="0"/>
         <v>-1.33</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43">
+        <v>26</v>
+      </c>
+      <c r="I43" t="s">
         <v>12</v>
       </c>
-      <c r="K43">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A44" s="1">
         <v>45442</v>
       </c>
@@ -4991,14 +4991,14 @@
         <f t="shared" si="0"/>
         <v>0.1100000000000001</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44">
+        <v>26</v>
+      </c>
+      <c r="I44" t="s">
         <v>12</v>
       </c>
-      <c r="K44">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A45" s="1">
         <v>45442</v>
       </c>
@@ -5021,14 +5021,14 @@
         <f t="shared" si="0"/>
         <v>-1.1600000000000001</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45">
+        <v>26</v>
+      </c>
+      <c r="I45" t="s">
         <v>12</v>
       </c>
-      <c r="K45">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A46" s="1">
         <v>45442</v>
       </c>
@@ -5052,13 +5052,13 @@
         <v>-0.76500000000000001</v>
       </c>
       <c r="H46">
+        <v>26</v>
+      </c>
+      <c r="I46">
         <v>4.6500000000000004</v>
       </c>
-      <c r="K46">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A47" s="1">
         <v>45442</v>
       </c>
@@ -5081,11 +5081,11 @@
         <f t="shared" si="0"/>
         <v>-1.24</v>
       </c>
-      <c r="K47">
+      <c r="H47">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A48" s="1">
         <v>45442</v>
       </c>
@@ -5109,13 +5109,13 @@
         <v>-0.96</v>
       </c>
       <c r="H48">
+        <v>26</v>
+      </c>
+      <c r="I48">
         <v>4.03</v>
       </c>
-      <c r="K48">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A49" s="1">
         <v>45442</v>
       </c>
@@ -5139,13 +5139,13 @@
         <v>-1.155</v>
       </c>
       <c r="H49">
+        <v>26</v>
+      </c>
+      <c r="I49">
         <v>3.66</v>
       </c>
-      <c r="K49">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A50" s="1">
         <v>45463</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>-0.85000000000000009</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A51" s="1">
         <v>45463</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>-1.55</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A52" s="1">
         <v>45463</v>
       </c>
@@ -5217,16 +5217,16 @@
         <v>-0.755</v>
       </c>
       <c r="H52">
+        <v>27</v>
+      </c>
+      <c r="I52">
         <v>5.37</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>708</v>
       </c>
-      <c r="K52">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A53" s="1">
         <v>45463</v>
       </c>
@@ -5250,16 +5250,16 @@
         <v>-1.25</v>
       </c>
       <c r="H53">
+        <v>27</v>
+      </c>
+      <c r="I53">
         <v>4.87</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>246</v>
       </c>
-      <c r="K53">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A54" s="1">
         <v>45463</v>
       </c>
@@ -5283,7 +5283,7 @@
         <v>-0.12</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A55" s="1">
         <v>45463</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>-1.24</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A56" s="1">
         <v>45463</v>
       </c>
@@ -5331,16 +5331,16 @@
         <v>-2.46</v>
       </c>
       <c r="H56">
+        <v>26</v>
+      </c>
+      <c r="I56">
         <v>5.05</v>
       </c>
-      <c r="I56">
+      <c r="J56">
         <v>473</v>
       </c>
-      <c r="K56">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A57" s="1">
         <v>45463</v>
       </c>
@@ -5364,16 +5364,16 @@
         <v>-1.8099999999999998</v>
       </c>
       <c r="H57">
+        <v>26</v>
+      </c>
+      <c r="I57">
         <v>4.8</v>
       </c>
-      <c r="I57">
+      <c r="J57">
         <v>101</v>
       </c>
-      <c r="K57">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A58" s="1">
         <v>45463</v>
       </c>
@@ -5397,16 +5397,16 @@
         <v>-1.4900000000000002</v>
       </c>
       <c r="H58">
+        <v>26</v>
+      </c>
+      <c r="I58">
         <v>4.7699999999999996</v>
       </c>
-      <c r="I58">
+      <c r="J58">
         <v>116</v>
       </c>
-      <c r="K58">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A59" s="1">
         <v>45463</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>-2.64</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A60" s="1">
         <v>45463</v>
       </c>
@@ -5454,7 +5454,7 @@
         <v>-1.0999999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A61" s="1">
         <v>45463</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>-2.79</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A62" s="1">
         <v>45463</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>-1.4649999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A63" s="1">
         <v>45463</v>
       </c>
@@ -5525,11 +5525,11 @@
         <f t="shared" si="1"/>
         <v>-2.1800000000000002</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <v>848</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A64" s="1">
         <v>45463</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>-2.19</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A65" s="1">
         <v>45463</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>-2.0049999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A66" s="1">
         <v>45484</v>
       </c>
@@ -5601,16 +5601,16 @@
         <v>0.2</v>
       </c>
       <c r="H66">
+        <v>26</v>
+      </c>
+      <c r="I66">
         <v>5.0999999999999996</v>
       </c>
-      <c r="I66">
+      <c r="J66">
         <v>103</v>
       </c>
-      <c r="K66">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A67" s="1">
         <v>45484</v>
       </c>
@@ -5634,16 +5634,16 @@
         <v>0.42</v>
       </c>
       <c r="H67">
+        <v>25.7</v>
+      </c>
+      <c r="I67">
         <v>5.47</v>
       </c>
-      <c r="I67">
+      <c r="J67">
         <v>92</v>
       </c>
-      <c r="K67">
-        <v>25.7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A68" s="1">
         <v>45484</v>
       </c>
@@ -5666,16 +5666,16 @@
         <v>0.3</v>
       </c>
       <c r="H68">
+        <v>24.9</v>
+      </c>
+      <c r="I68">
         <v>5.47</v>
       </c>
-      <c r="I68">
+      <c r="J68">
         <v>333</v>
       </c>
-      <c r="K68">
-        <v>24.9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A69" s="1">
         <v>45484</v>
       </c>
@@ -5699,16 +5699,16 @@
         <v>-0.22999999999999998</v>
       </c>
       <c r="H69">
+        <v>25.9</v>
+      </c>
+      <c r="I69">
         <v>4.97</v>
       </c>
-      <c r="I69">
+      <c r="J69">
         <v>649</v>
       </c>
-      <c r="K69">
-        <v>25.9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A70" s="1">
         <v>45484</v>
       </c>
@@ -5731,16 +5731,16 @@
         <v>0.3</v>
       </c>
       <c r="H70">
+        <v>25.9</v>
+      </c>
+      <c r="I70">
         <v>3.8</v>
       </c>
-      <c r="I70">
+      <c r="J70">
         <v>348</v>
       </c>
-      <c r="K70">
-        <v>25.9</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A71" s="1">
         <v>45484</v>
       </c>
@@ -5764,16 +5764,16 @@
         <v>-0.18</v>
       </c>
       <c r="H71">
+        <v>27</v>
+      </c>
+      <c r="I71">
         <v>3.87</v>
       </c>
-      <c r="I71">
+      <c r="J71">
         <v>603</v>
       </c>
-      <c r="K71">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A72" s="1">
         <v>45484</v>
       </c>
@@ -5797,16 +5797,16 @@
         <v>-3.5</v>
       </c>
       <c r="H72">
+        <v>23</v>
+      </c>
+      <c r="I72">
         <v>5.2</v>
       </c>
-      <c r="I72">
+      <c r="J72">
         <v>103</v>
       </c>
-      <c r="K72">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A73" s="1">
         <v>45484</v>
       </c>
@@ -5830,16 +5830,16 @@
         <v>-1.0899999999999999</v>
       </c>
       <c r="H73">
+        <v>27.75</v>
+      </c>
+      <c r="I73">
         <v>3.72</v>
       </c>
-      <c r="I73">
+      <c r="J73">
         <v>4425</v>
       </c>
-      <c r="K73">
-        <v>27.75</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A74" s="1">
         <v>45484</v>
       </c>
@@ -5863,16 +5863,16 @@
         <v>-0.48000000000000009</v>
       </c>
       <c r="H74">
+        <v>25.89</v>
+      </c>
+      <c r="I74">
         <v>3.5</v>
       </c>
-      <c r="I74">
+      <c r="J74">
         <v>1791</v>
       </c>
-      <c r="K74">
-        <v>25.89</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A75" s="1">
         <v>45484</v>
       </c>
@@ -5896,16 +5896,16 @@
         <v>-1.72</v>
       </c>
       <c r="H75">
+        <v>26.57</v>
+      </c>
+      <c r="I75">
         <v>3.89</v>
       </c>
-      <c r="I75">
+      <c r="J75">
         <v>3358</v>
       </c>
-      <c r="K75">
-        <v>26.57</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A76" s="1">
         <v>45484</v>
       </c>
@@ -5929,16 +5929,16 @@
         <v>0.27</v>
       </c>
       <c r="H76">
+        <v>28</v>
+      </c>
+      <c r="I76">
         <v>3.68</v>
       </c>
-      <c r="I76">
+      <c r="J76">
         <v>3828</v>
       </c>
-      <c r="K76">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A77" s="1">
         <v>45484</v>
       </c>
@@ -5961,11 +5961,11 @@
         <f t="shared" si="2"/>
         <v>-2.14</v>
       </c>
-      <c r="K77" t="s">
+      <c r="H77" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A78" s="1">
         <v>45484</v>
       </c>
@@ -5988,11 +5988,11 @@
         <f t="shared" si="2"/>
         <v>-0.8849999999999999</v>
       </c>
-      <c r="K78" t="s">
+      <c r="H78" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A79" s="1">
         <v>45484</v>
       </c>
@@ -6016,16 +6016,16 @@
         <v>-1.98</v>
       </c>
       <c r="H79">
+        <v>28.7</v>
+      </c>
+      <c r="I79">
         <v>3.76</v>
       </c>
-      <c r="I79">
+      <c r="J79">
         <v>3703</v>
       </c>
-      <c r="K79">
-        <v>28.7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A80" s="1">
         <v>45484</v>
       </c>
@@ -6049,16 +6049,16 @@
         <v>-2.1800000000000002</v>
       </c>
       <c r="H80">
+        <v>30.6</v>
+      </c>
+      <c r="I80">
         <v>3.63</v>
       </c>
-      <c r="I80">
+      <c r="J80">
         <v>2916</v>
       </c>
-      <c r="K80">
-        <v>30.6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A81" s="1">
         <v>45484</v>
       </c>
@@ -6081,11 +6081,11 @@
         <f t="shared" si="2"/>
         <v>-1.2450000000000001</v>
       </c>
-      <c r="K81" t="s">
+      <c r="H81" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A82" s="1">
         <v>45502</v>
       </c>
@@ -6105,16 +6105,16 @@
         <v>0.04</v>
       </c>
       <c r="H82">
+        <v>25.8</v>
+      </c>
+      <c r="I82">
         <v>5.36</v>
       </c>
-      <c r="I82">
+      <c r="J82">
         <v>515</v>
       </c>
-      <c r="K82">
-        <v>25.8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A83" s="1">
         <v>45502</v>
       </c>
@@ -6134,16 +6134,16 @@
         <v>0.23499999999999999</v>
       </c>
       <c r="H83">
+        <v>26</v>
+      </c>
+      <c r="I83">
         <v>5</v>
       </c>
-      <c r="I83">
+      <c r="J83">
         <v>2950</v>
       </c>
-      <c r="K83">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A84" s="1">
         <v>45502</v>
       </c>
@@ -6163,16 +6163,16 @@
         <v>0.19</v>
       </c>
       <c r="H84">
+        <v>24</v>
+      </c>
+      <c r="I84">
         <v>4.5999999999999996</v>
       </c>
-      <c r="I84">
+      <c r="J84">
         <v>934</v>
       </c>
-      <c r="K84">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A85" s="1">
         <v>45502</v>
       </c>
@@ -6196,16 +6196,16 @@
         <v>-0.4</v>
       </c>
       <c r="H85">
+        <v>26</v>
+      </c>
+      <c r="I85">
         <v>4.84</v>
       </c>
-      <c r="I85">
+      <c r="J85">
         <v>1310</v>
       </c>
-      <c r="K85">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A86" s="1">
         <v>45502</v>
       </c>
@@ -6225,16 +6225,16 @@
         <v>0.36</v>
       </c>
       <c r="H86">
+        <v>25.72</v>
+      </c>
+      <c r="I86">
         <v>4.58</v>
       </c>
-      <c r="I86">
+      <c r="J86">
         <v>1290</v>
       </c>
-      <c r="K86">
-        <v>25.72</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A87" s="1">
         <v>45502</v>
       </c>
@@ -6258,16 +6258,16 @@
         <v>-0.10499999999999998</v>
       </c>
       <c r="H87">
+        <v>24</v>
+      </c>
+      <c r="I87">
         <v>5</v>
       </c>
-      <c r="I87">
+      <c r="J87">
         <v>530</v>
       </c>
-      <c r="K87">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A88" s="1">
         <v>45502</v>
       </c>
@@ -6286,17 +6286,17 @@
       <c r="G88">
         <v>0.19800000000000001</v>
       </c>
-      <c r="H88">
+      <c r="H88" t="s">
+        <v>12</v>
+      </c>
+      <c r="I88">
         <v>5</v>
       </c>
-      <c r="I88" t="s">
+      <c r="J88" t="s">
         <v>12</v>
       </c>
-      <c r="K88" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A89" s="1">
         <v>45502</v>
       </c>
@@ -6320,16 +6320,16 @@
         <v>-0.41</v>
       </c>
       <c r="H89">
+        <v>34.33</v>
+      </c>
+      <c r="I89">
         <v>4.5</v>
       </c>
-      <c r="I89">
+      <c r="J89">
         <v>5453</v>
       </c>
-      <c r="K89">
-        <v>34.33</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A90" s="1">
         <v>45502</v>
       </c>
@@ -6349,16 +6349,16 @@
         <v>-0.09</v>
       </c>
       <c r="H90">
+        <v>32.46</v>
+      </c>
+      <c r="I90">
         <v>4.97</v>
       </c>
-      <c r="I90">
+      <c r="J90">
         <v>4554</v>
       </c>
-      <c r="K90">
-        <v>32.46</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A91" s="1">
         <v>45502</v>
       </c>
@@ -6378,16 +6378,16 @@
         <v>-0.06</v>
       </c>
       <c r="H91">
+        <v>29.26</v>
+      </c>
+      <c r="I91">
         <v>4.08</v>
       </c>
-      <c r="I91">
+      <c r="J91">
         <v>909</v>
       </c>
-      <c r="K91">
-        <v>29.26</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A92" s="1">
         <v>45502</v>
       </c>
@@ -6411,16 +6411,16 @@
         <v>-0.59999999999999987</v>
       </c>
       <c r="H92">
+        <v>28</v>
+      </c>
+      <c r="I92">
         <v>3.48</v>
       </c>
-      <c r="I92">
+      <c r="J92">
         <v>1541</v>
       </c>
-      <c r="K92">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A93" s="1">
         <v>45502</v>
       </c>
@@ -6444,7 +6444,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A94" s="1">
         <v>45502</v>
       </c>
@@ -6468,16 +6468,16 @@
         <v>-0.29500000000000004</v>
       </c>
       <c r="H94">
+        <v>28</v>
+      </c>
+      <c r="I94">
         <v>3.92</v>
       </c>
-      <c r="I94">
+      <c r="J94">
         <v>1519</v>
       </c>
-      <c r="K94">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A95" s="1">
         <v>45502</v>
       </c>
@@ -6501,16 +6501,16 @@
         <v>-0.59</v>
       </c>
       <c r="H95">
+        <v>28</v>
+      </c>
+      <c r="I95">
         <v>3.75</v>
       </c>
-      <c r="I95">
+      <c r="J95">
         <v>1531</v>
       </c>
-      <c r="K95">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A96" s="1">
         <v>45502</v>
       </c>
@@ -6530,16 +6530,16 @@
         <v>0.77</v>
       </c>
       <c r="H96">
+        <v>28</v>
+      </c>
+      <c r="I96">
         <v>3.8</v>
       </c>
-      <c r="I96">
+      <c r="J96">
         <v>3013</v>
       </c>
-      <c r="K96">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A97" s="1">
         <v>45502</v>
       </c>
@@ -6562,11 +6562,11 @@
         <f>E97-F97</f>
         <v>-1.0349999999999999</v>
       </c>
-      <c r="H97">
+      <c r="I97">
         <v>5.41</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A98" s="1">
         <v>45534</v>
       </c>
@@ -6586,16 +6586,16 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="H98">
+        <v>26.04</v>
+      </c>
+      <c r="I98">
         <v>5.41</v>
       </c>
-      <c r="I98">
+      <c r="J98">
         <v>1280</v>
       </c>
-      <c r="K98">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A99" s="1">
         <v>45534</v>
       </c>
@@ -6615,16 +6615,16 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="H99">
+        <v>26.2</v>
+      </c>
+      <c r="I99">
         <v>5.34</v>
       </c>
-      <c r="I99">
+      <c r="J99">
         <v>1776</v>
       </c>
-      <c r="K99">
-        <v>26.2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A100" s="1">
         <v>45534</v>
       </c>
@@ -6649,16 +6649,16 @@
         <v>-0.64500000000000002</v>
       </c>
       <c r="H100">
+        <v>25.9</v>
+      </c>
+      <c r="I100">
         <v>5.37</v>
       </c>
-      <c r="I100">
+      <c r="J100">
         <v>647.4</v>
       </c>
-      <c r="K100">
-        <v>25.9</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A101" s="1">
         <v>45534</v>
       </c>
@@ -6683,16 +6683,16 @@
         <v>0.53999999999999992</v>
       </c>
       <c r="H101">
+        <v>25.7</v>
+      </c>
+      <c r="I101">
         <v>5.16</v>
       </c>
-      <c r="I101">
+      <c r="J101">
         <v>1738</v>
       </c>
-      <c r="K101">
-        <v>25.7</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A102" s="1">
         <v>45534</v>
       </c>
@@ -6717,16 +6717,16 @@
         <v>-0.69000000000000006</v>
       </c>
       <c r="H102">
+        <v>26.43</v>
+      </c>
+      <c r="I102">
         <v>4.45</v>
       </c>
-      <c r="I102">
+      <c r="J102">
         <v>1572</v>
       </c>
-      <c r="K102">
-        <v>26.43</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A103" s="1">
         <v>45534</v>
       </c>
@@ -6746,16 +6746,16 @@
         <v>0</v>
       </c>
       <c r="H103">
+        <v>26.8</v>
+      </c>
+      <c r="I103">
         <v>4.1900000000000004</v>
       </c>
-      <c r="I103">
+      <c r="J103">
         <v>1488</v>
       </c>
-      <c r="K103">
-        <v>26.8</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A104" s="1">
         <v>45534</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A105" s="1">
         <v>45534</v>
       </c>
@@ -6792,16 +6792,16 @@
         <v>-0.19</v>
       </c>
       <c r="H105">
+        <v>27.11</v>
+      </c>
+      <c r="I105">
         <v>4.22</v>
       </c>
-      <c r="I105">
+      <c r="J105">
         <v>1330</v>
       </c>
-      <c r="K105">
-        <v>27.11</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A106" s="1">
         <v>45534</v>
       </c>
@@ -6821,16 +6821,16 @@
         <v>0.06</v>
       </c>
       <c r="H106">
+        <v>26.01</v>
+      </c>
+      <c r="I106">
         <v>4.37</v>
       </c>
-      <c r="I106">
+      <c r="J106">
         <v>4850</v>
       </c>
-      <c r="K106">
-        <v>26.01</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A107" s="1">
         <v>45534</v>
       </c>
@@ -6850,16 +6850,16 @@
         <v>-0.51</v>
       </c>
       <c r="H107">
+        <v>26.23</v>
+      </c>
+      <c r="I107">
         <v>4.71</v>
       </c>
-      <c r="I107">
+      <c r="J107">
         <v>830</v>
       </c>
-      <c r="K107">
-        <v>26.23</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A108" s="1">
         <v>45534</v>
       </c>
@@ -6879,16 +6879,16 @@
         <v>-0.04</v>
       </c>
       <c r="H108">
+        <v>26.62</v>
+      </c>
+      <c r="I108">
         <v>4.41</v>
       </c>
-      <c r="I108">
+      <c r="J108">
         <v>500</v>
       </c>
-      <c r="K108">
-        <v>26.62</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A109" s="1">
         <v>45534</v>
       </c>
@@ -6909,16 +6909,16 @@
         <v>-0.98</v>
       </c>
       <c r="H109">
+        <v>29</v>
+      </c>
+      <c r="I109">
         <v>4.34</v>
       </c>
-      <c r="I109">
+      <c r="J109">
         <v>1144</v>
       </c>
-      <c r="K109">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A110" s="1">
         <v>45534</v>
       </c>
@@ -6939,16 +6939,16 @@
         <v>-0.16000000000000003</v>
       </c>
       <c r="H110">
+        <v>29.07</v>
+      </c>
+      <c r="I110">
         <v>3.83</v>
       </c>
-      <c r="I110">
+      <c r="J110">
         <v>2900</v>
       </c>
-      <c r="K110">
-        <v>29.07</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A111" s="1">
         <v>45534</v>
       </c>
@@ -6968,16 +6968,16 @@
         <v>-0.4</v>
       </c>
       <c r="H111">
+        <v>28.69</v>
+      </c>
+      <c r="I111">
         <v>3.97</v>
       </c>
-      <c r="I111">
+      <c r="J111">
         <v>3560</v>
       </c>
-      <c r="K111">
-        <v>28.69</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A112" s="1">
         <v>45534</v>
       </c>
@@ -6997,16 +6997,16 @@
         <v>-0.39</v>
       </c>
       <c r="H112">
+        <v>30</v>
+      </c>
+      <c r="I112">
         <v>3.85</v>
       </c>
-      <c r="I112">
+      <c r="J112">
         <v>3732</v>
       </c>
-      <c r="K112">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.75">
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A113" s="1">
         <v>45534</v>
       </c>
@@ -7023,7 +7023,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A114" s="1">
         <v>45569</v>
       </c>
@@ -7043,14 +7043,14 @@
         <f>6.5/100</f>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="H114">
+      <c r="I114">
         <v>6.6</v>
       </c>
-      <c r="I114">
+      <c r="J114">
         <v>1000</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A115" s="1">
         <v>45569</v>
       </c>
@@ -7069,14 +7069,14 @@
       <c r="G115">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="H115">
+      <c r="I115">
         <v>5.97</v>
       </c>
-      <c r="I115">
+      <c r="J115">
         <v>718</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A116" s="1">
         <v>45569</v>
       </c>
@@ -7099,14 +7099,14 @@
         <f>E116-F116</f>
         <v>-9.4999999999999973E-2</v>
       </c>
-      <c r="H116">
+      <c r="I116">
         <v>5.82</v>
       </c>
-      <c r="I116">
+      <c r="J116">
         <v>2910</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A117" s="1">
         <v>45569</v>
       </c>
@@ -7129,14 +7129,14 @@
         <f t="shared" ref="G117:G121" si="4">E117-F117</f>
         <v>-1.3800000000000001</v>
       </c>
-      <c r="H117">
+      <c r="I117">
         <v>5.19</v>
       </c>
-      <c r="I117">
+      <c r="J117">
         <v>2200</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A118" s="1">
         <v>45569</v>
       </c>
@@ -7159,14 +7159,14 @@
         <f t="shared" si="4"/>
         <v>-4.0000000000000036E-2</v>
       </c>
-      <c r="H118">
+      <c r="I118">
         <v>4.2</v>
       </c>
-      <c r="I118">
+      <c r="J118">
         <v>3400</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A119" s="1">
         <v>45569</v>
       </c>
@@ -7189,14 +7189,14 @@
         <f t="shared" si="4"/>
         <v>-1.1599999999999999</v>
       </c>
-      <c r="H119">
+      <c r="I119">
         <v>4.42</v>
       </c>
-      <c r="I119">
+      <c r="J119">
         <v>4203</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A120" s="1">
         <v>45569</v>
       </c>
@@ -7219,11 +7219,11 @@
         <f t="shared" si="4"/>
         <v>-0.875</v>
       </c>
-      <c r="H120">
+      <c r="I120">
         <v>6.12</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A121" s="1">
         <v>45569</v>
       </c>
@@ -7246,14 +7246,14 @@
         <f t="shared" si="4"/>
         <v>-0.29499999999999998</v>
       </c>
-      <c r="H121">
+      <c r="I121">
         <v>3.94</v>
       </c>
-      <c r="I121">
+      <c r="J121">
         <v>1485</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A122" s="1">
         <v>45569</v>
       </c>
@@ -7272,14 +7272,14 @@
       <c r="G122">
         <v>0.03</v>
       </c>
-      <c r="H122">
+      <c r="I122">
         <v>4.01</v>
       </c>
-      <c r="I122">
+      <c r="J122">
         <v>3426</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A123" s="1">
         <v>45569</v>
       </c>
@@ -7302,14 +7302,14 @@
         <f>E123-F123</f>
         <v>-1.345</v>
       </c>
-      <c r="H123">
+      <c r="I123">
         <v>6.45</v>
       </c>
-      <c r="I123">
+      <c r="J123">
         <v>1373.6</v>
       </c>
     </row>
-    <row r="124" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A124" s="3">
         <v>45569</v>
       </c>
@@ -7331,14 +7331,14 @@
       <c r="G124" s="4">
         <v>0</v>
       </c>
-      <c r="H124" s="4">
+      <c r="I124" s="4">
         <v>4.29</v>
       </c>
-      <c r="I124">
+      <c r="J124">
         <v>2755</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A125" s="1">
         <v>45569</v>
       </c>
@@ -7361,14 +7361,14 @@
         <f t="shared" ref="G125:G133" si="5">E125-F125</f>
         <v>-0.39999999999999991</v>
       </c>
-      <c r="H125">
+      <c r="I125">
         <v>4.1900000000000004</v>
       </c>
-      <c r="I125" s="4">
+      <c r="J125" s="4">
         <v>2249</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A126" s="1">
         <v>45569</v>
       </c>
@@ -7391,14 +7391,14 @@
         <f t="shared" si="5"/>
         <v>-0.78999999999999992</v>
       </c>
-      <c r="H126">
+      <c r="I126">
         <v>3.79</v>
       </c>
-      <c r="I126">
+      <c r="J126">
         <v>833</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A127" s="1">
         <v>45569</v>
       </c>
@@ -7421,14 +7421,14 @@
         <f t="shared" si="5"/>
         <v>-1.17</v>
       </c>
-      <c r="H127">
+      <c r="I127">
         <v>3.93</v>
       </c>
-      <c r="I127">
+      <c r="J127">
         <v>3161</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A128" s="1">
         <v>45569</v>
       </c>
@@ -7451,14 +7451,14 @@
         <f t="shared" si="5"/>
         <v>-1.29</v>
       </c>
-      <c r="H128">
+      <c r="I128">
         <v>3.88</v>
       </c>
-      <c r="I128">
+      <c r="J128">
         <v>688</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A129" s="1">
         <v>45569</v>
       </c>
@@ -7481,14 +7481,14 @@
         <f t="shared" si="5"/>
         <v>-1.4550000000000001</v>
       </c>
-      <c r="H129">
+      <c r="I129">
         <v>4.34</v>
       </c>
-      <c r="I129">
+      <c r="J129">
         <v>1012</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A130" s="1">
         <v>45597</v>
       </c>
@@ -7512,13 +7512,13 @@
         <v>-0.79200000000000004</v>
       </c>
       <c r="H130">
+        <v>21</v>
+      </c>
+      <c r="I130">
         <v>6.48</v>
       </c>
-      <c r="K130">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A131" s="1">
         <v>45597</v>
       </c>
@@ -7542,17 +7542,17 @@
         <v>-0.28499999999999998</v>
       </c>
       <c r="H131">
+        <v>21.5</v>
+      </c>
+      <c r="I131">
         <v>6.22</v>
       </c>
-      <c r="I131">
+      <c r="J131">
         <f>AVERAGE(937,959,948)</f>
         <v>948</v>
       </c>
-      <c r="K131">
-        <v>21.5</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A132" s="1">
         <v>45597</v>
       </c>
@@ -7573,17 +7573,17 @@
         <v>0.755</v>
       </c>
       <c r="H132">
+        <v>21.3</v>
+      </c>
+      <c r="I132">
         <v>7.24</v>
       </c>
-      <c r="I132">
+      <c r="J132">
         <f>AVERAGE(740.5,797.3, 831)</f>
         <v>789.6</v>
       </c>
-      <c r="K132">
-        <v>21.3</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A133" s="1">
         <v>45597</v>
       </c>
@@ -7604,16 +7604,16 @@
         <v>0.24</v>
       </c>
       <c r="H133">
+        <v>22.3</v>
+      </c>
+      <c r="I133">
         <v>5.24</v>
       </c>
-      <c r="I133">
+      <c r="J133">
         <v>1342</v>
       </c>
-      <c r="K133">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A134" s="1">
         <v>45597</v>
       </c>
@@ -7630,17 +7630,17 @@
         <v>0.75</v>
       </c>
       <c r="H134">
+        <v>21.9</v>
+      </c>
+      <c r="I134">
         <v>4.34</v>
       </c>
-      <c r="I134">
+      <c r="J134">
         <f>AVERAGE(2828,2617,2734)</f>
         <v>2726.3333333333335</v>
       </c>
-      <c r="K134">
-        <v>21.9</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A135" s="1">
         <v>45597</v>
       </c>
@@ -7657,13 +7657,13 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H135">
+        <v>22.5</v>
+      </c>
+      <c r="I135">
         <v>4.6399999999999997</v>
       </c>
-      <c r="K135">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A136" s="1">
         <v>45597</v>
       </c>
@@ -7683,17 +7683,17 @@
         <v>0.183</v>
       </c>
       <c r="H136">
+        <v>19.8</v>
+      </c>
+      <c r="I136">
         <v>5.97</v>
       </c>
-      <c r="I136">
+      <c r="J136">
         <f>AVERAGE(572.7,570,549)</f>
         <v>563.9</v>
       </c>
-      <c r="K136">
-        <v>19.8</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A137" s="1">
         <v>45597</v>
       </c>
@@ -7713,21 +7713,21 @@
         <v>0.5</v>
       </c>
       <c r="G137">
-        <f t="shared" ref="G137:G163" si="6">E137-F137</f>
+        <f t="shared" ref="G137:G180" si="6">E137-F137</f>
         <v>-0.42</v>
       </c>
       <c r="H137">
+        <v>21.6</v>
+      </c>
+      <c r="I137">
         <v>4.2699999999999996</v>
       </c>
-      <c r="I137">
+      <c r="J137">
         <f>AVERAGE(2584,2605,2558)</f>
         <v>2582.3333333333335</v>
       </c>
-      <c r="K137">
-        <v>21.6</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A138" s="1">
         <v>45597</v>
       </c>
@@ -7751,17 +7751,17 @@
         <v>-6.0000000000000053E-2</v>
       </c>
       <c r="H138">
+        <v>21.6</v>
+      </c>
+      <c r="I138">
         <v>4.42</v>
       </c>
-      <c r="I138">
+      <c r="J138">
         <f>AVERAGE(1359,1304,1317)</f>
         <v>1326.6666666666667</v>
       </c>
-      <c r="K138">
-        <v>21.6</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A139" s="1">
         <v>45597</v>
       </c>
@@ -7786,17 +7786,17 @@
         <v>-0.68500000000000005</v>
       </c>
       <c r="H139">
+        <v>22.2</v>
+      </c>
+      <c r="I139">
         <v>4.4400000000000004</v>
       </c>
-      <c r="I139">
+      <c r="J139">
         <f>AVERAGE(2273,2284,2224)</f>
         <v>2260.3333333333335</v>
       </c>
-      <c r="K139">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A140" s="1">
         <v>45597</v>
       </c>
@@ -7820,17 +7820,17 @@
         <v>0.35400000000000004</v>
       </c>
       <c r="H140">
+        <v>21.7</v>
+      </c>
+      <c r="I140">
         <v>4.84</v>
       </c>
-      <c r="I140">
+      <c r="J140">
         <f>AVERAGE(1749,1772,1799)</f>
         <v>1773.3333333333333</v>
       </c>
-      <c r="K140">
-        <v>21.7</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A141" s="1">
         <v>45597</v>
       </c>
@@ -7854,17 +7854,17 @@
         <v>-1.3199999999999998</v>
       </c>
       <c r="H141">
+        <v>22.8</v>
+      </c>
+      <c r="I141">
         <v>4.92</v>
       </c>
-      <c r="I141">
+      <c r="J141">
         <f>AVERAGE(3721,3982,4086,3979)</f>
         <v>3942</v>
       </c>
-      <c r="K141">
-        <v>22.8</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A142" s="1">
         <v>45597</v>
       </c>
@@ -7888,17 +7888,17 @@
         <v>-0.29300000000000004</v>
       </c>
       <c r="H142">
+        <v>21.5</v>
+      </c>
+      <c r="I142">
         <v>3.89</v>
       </c>
-      <c r="I142">
+      <c r="J142">
         <f>AVERAGE(2060,2073,2041,2280)</f>
         <v>2113.5</v>
       </c>
-      <c r="K142">
-        <v>21.5</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A143" s="1">
         <v>45597</v>
       </c>
@@ -7922,17 +7922,17 @@
         <v>-0.55600000000000005</v>
       </c>
       <c r="H143">
+        <v>23.3</v>
+      </c>
+      <c r="I143">
         <v>4.05</v>
       </c>
-      <c r="I143">
+      <c r="J143">
         <f>AVERAGE(2259,2255,2260)</f>
         <v>2258</v>
       </c>
-      <c r="K143">
-        <v>23.3</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A144" s="1">
         <v>45597</v>
       </c>
@@ -7956,17 +7956,17 @@
         <v>-0.64</v>
       </c>
       <c r="H144">
+        <v>23.6</v>
+      </c>
+      <c r="I144">
         <v>3.98</v>
       </c>
-      <c r="I144">
+      <c r="J144">
         <f>AVERAGE(3300,3261,3241)</f>
         <v>3267.3333333333335</v>
       </c>
-      <c r="K144">
-        <v>23.6</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A145" s="1">
         <v>45597</v>
       </c>
@@ -7990,17 +7990,17 @@
         <v>-0.83499999999999996</v>
       </c>
       <c r="H145">
+        <v>22.8</v>
+      </c>
+      <c r="I145">
         <v>4.3600000000000003</v>
       </c>
-      <c r="I145">
+      <c r="J145">
         <f>AVERAGE(2396,2381,2362)</f>
         <v>2379.6666666666665</v>
       </c>
-      <c r="K145">
-        <v>22.8</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A146" s="1">
         <v>45635</v>
       </c>
@@ -8024,13 +8024,13 @@
         <v>-1.01</v>
       </c>
       <c r="H146">
+        <v>15.9</v>
+      </c>
+      <c r="I146">
         <v>6.64</v>
       </c>
-      <c r="K146">
-        <v>15.9</v>
-      </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A147" s="1">
         <v>45635</v>
       </c>
@@ -8054,13 +8054,13 @@
         <v>-0.25</v>
       </c>
       <c r="H147">
+        <v>17</v>
+      </c>
+      <c r="I147">
         <v>6.36</v>
       </c>
-      <c r="K147">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A148" s="1">
         <v>45635</v>
       </c>
@@ -8084,13 +8084,13 @@
         <v>-0.48000000000000009</v>
       </c>
       <c r="H148">
+        <v>15.8</v>
+      </c>
+      <c r="I148">
         <v>6.78</v>
       </c>
-      <c r="K148">
-        <v>15.8</v>
-      </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A149" s="1">
         <v>45635</v>
       </c>
@@ -8114,13 +8114,13 @@
         <v>-0.8600000000000001</v>
       </c>
       <c r="H149">
+        <v>17.5</v>
+      </c>
+      <c r="I149">
         <v>5.13</v>
       </c>
-      <c r="K149">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A150" s="1">
         <v>45635</v>
       </c>
@@ -8144,13 +8144,13 @@
         <v>-0.24</v>
       </c>
       <c r="H150">
+        <v>17.8</v>
+      </c>
+      <c r="I150">
         <v>4.2300000000000004</v>
       </c>
-      <c r="K150">
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A151" s="1">
         <v>45635</v>
       </c>
@@ -8174,13 +8174,13 @@
         <v>-0.8899999999999999</v>
       </c>
       <c r="H151">
+        <v>18.5</v>
+      </c>
+      <c r="I151">
         <v>4.9800000000000004</v>
       </c>
-      <c r="K151">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A152" s="1">
         <v>45635</v>
       </c>
@@ -8204,13 +8204,13 @@
         <v>-0.20999999999999996</v>
       </c>
       <c r="H152">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="I152">
         <v>5.76</v>
       </c>
-      <c r="K152">
-        <v>16.899999999999999</v>
-      </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A153" s="1">
         <v>45635</v>
       </c>
@@ -8234,13 +8234,13 @@
         <v>-0.55000000000000004</v>
       </c>
       <c r="H153">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="I153">
         <v>5.89</v>
       </c>
-      <c r="K153">
-        <v>17.100000000000001</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A154" s="1">
         <v>45635</v>
       </c>
@@ -8264,13 +8264,13 @@
         <v>-1.04</v>
       </c>
       <c r="H154">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="I154">
         <v>4.13</v>
       </c>
-      <c r="K154">
-        <v>18.899999999999999</v>
-      </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A155" s="1">
         <v>45635</v>
       </c>
@@ -8294,13 +8294,13 @@
         <v>-0.8</v>
       </c>
       <c r="H155">
+        <v>18.8</v>
+      </c>
+      <c r="I155">
         <v>4.3600000000000003</v>
       </c>
-      <c r="K155">
-        <v>18.8</v>
-      </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A156" s="1">
         <v>45635</v>
       </c>
@@ -8324,13 +8324,13 @@
         <v>-1.03</v>
       </c>
       <c r="H156">
+        <v>20.2</v>
+      </c>
+      <c r="I156">
         <v>4.9400000000000004</v>
       </c>
-      <c r="K156">
-        <v>20.2</v>
-      </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A157" s="1">
         <v>45635</v>
       </c>
@@ -8354,13 +8354,13 @@
         <v>-0.46</v>
       </c>
       <c r="H157">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="I157">
         <v>4.1100000000000003</v>
       </c>
-      <c r="K157">
-        <v>19.399999999999999</v>
-      </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A158" s="1">
         <v>45635</v>
       </c>
@@ -8384,13 +8384,13 @@
         <v>-2.08</v>
       </c>
       <c r="H158">
+        <v>21.4</v>
+      </c>
+      <c r="I158">
         <v>4.51</v>
       </c>
-      <c r="K158">
-        <v>21.4</v>
-      </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A159" s="1">
         <v>45635</v>
       </c>
@@ -8414,13 +8414,13 @@
         <v>-0.38</v>
       </c>
       <c r="H159">
+        <v>14.8</v>
+      </c>
+      <c r="I159">
         <v>4.45</v>
       </c>
-      <c r="K159">
-        <v>14.8</v>
-      </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A160" s="1">
         <v>45635</v>
       </c>
@@ -8444,13 +8444,13 @@
         <v>-0.65</v>
       </c>
       <c r="H160">
+        <v>20</v>
+      </c>
+      <c r="I160">
         <v>4.0999999999999996</v>
       </c>
-      <c r="K160">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A161" s="1">
         <v>45635</v>
       </c>
@@ -8474,13 +8474,13 @@
         <v>-0.77999999999999992</v>
       </c>
       <c r="H161">
+        <v>19.8</v>
+      </c>
+      <c r="I161">
         <v>3.71</v>
       </c>
-      <c r="K161">
-        <v>19.8</v>
-      </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A162" s="1">
         <v>45635</v>
       </c>
@@ -8504,13 +8504,13 @@
         <v>-0.96000000000000008</v>
       </c>
       <c r="H162">
+        <v>18.5</v>
+      </c>
+      <c r="I162">
         <v>4.04</v>
       </c>
-      <c r="K162">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A163" s="1">
         <v>45635</v>
       </c>
@@ -8534,10 +8534,513 @@
         <v>-1.3</v>
       </c>
       <c r="H163">
+        <v>19.2</v>
+      </c>
+      <c r="I163">
         <v>4.41</v>
       </c>
-      <c r="K163">
-        <v>19.2</v>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A164" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B164">
+        <v>5</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+      <c r="D164" t="s">
+        <v>6</v>
+      </c>
+      <c r="E164">
+        <v>0.44</v>
+      </c>
+      <c r="F164">
+        <v>1</v>
+      </c>
+      <c r="G164">
+        <f t="shared" si="6"/>
+        <v>-0.56000000000000005</v>
+      </c>
+      <c r="H164">
+        <v>17.8</v>
+      </c>
+      <c r="I164">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A165" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B165">
+        <v>5</v>
+      </c>
+      <c r="C165">
+        <v>2</v>
+      </c>
+      <c r="D165" t="s">
+        <v>7</v>
+      </c>
+      <c r="E165">
+        <v>0.39</v>
+      </c>
+      <c r="F165">
+        <v>0.78</v>
+      </c>
+      <c r="G165">
+        <f t="shared" si="6"/>
+        <v>-0.39</v>
+      </c>
+      <c r="H165">
+        <v>15.2</v>
+      </c>
+      <c r="I165">
+        <v>6.22</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A166" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B166">
+        <v>5</v>
+      </c>
+      <c r="C166">
+        <v>3</v>
+      </c>
+      <c r="D166" t="s">
+        <v>8</v>
+      </c>
+      <c r="E166">
+        <v>0.75</v>
+      </c>
+      <c r="F166">
+        <v>1.04</v>
+      </c>
+      <c r="G166">
+        <f t="shared" si="6"/>
+        <v>-0.29000000000000004</v>
+      </c>
+      <c r="H166">
+        <v>17.5</v>
+      </c>
+      <c r="I166">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A167" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B167">
+        <v>5</v>
+      </c>
+      <c r="C167">
+        <v>4</v>
+      </c>
+      <c r="D167" t="s">
+        <v>9</v>
+      </c>
+      <c r="E167">
+        <v>0.21</v>
+      </c>
+      <c r="F167">
+        <v>1.08</v>
+      </c>
+      <c r="G167">
+        <f t="shared" si="6"/>
+        <v>-0.87000000000000011</v>
+      </c>
+      <c r="H167">
+        <v>16.5</v>
+      </c>
+      <c r="I167">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A168" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B168">
+        <v>5</v>
+      </c>
+      <c r="C168">
+        <v>5</v>
+      </c>
+      <c r="D168" t="s">
+        <v>10</v>
+      </c>
+      <c r="E168">
+        <v>0.09</v>
+      </c>
+      <c r="F168">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G168">
+        <f t="shared" si="6"/>
+        <v>-0.19999999999999998</v>
+      </c>
+      <c r="H168">
+        <v>15.9</v>
+      </c>
+      <c r="I168">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A169" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B169">
+        <v>5</v>
+      </c>
+      <c r="C169">
+        <v>6</v>
+      </c>
+      <c r="D169" t="s">
+        <v>11</v>
+      </c>
+      <c r="E169">
+        <v>0.04</v>
+      </c>
+      <c r="F169">
+        <v>0.82</v>
+      </c>
+      <c r="G169">
+        <f t="shared" si="6"/>
+        <v>-0.77999999999999992</v>
+      </c>
+      <c r="H169">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="I169">
+        <v>4.8899999999999997</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A170" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B170">
+        <v>5</v>
+      </c>
+      <c r="C170">
+        <v>7</v>
+      </c>
+      <c r="D170" t="s">
+        <v>11</v>
+      </c>
+      <c r="G170">
+        <v>0.19</v>
+      </c>
+      <c r="H170">
+        <v>13.7</v>
+      </c>
+      <c r="I170">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A171" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B171">
+        <v>5</v>
+      </c>
+      <c r="C171">
+        <v>8</v>
+      </c>
+      <c r="D171" t="s">
+        <v>36</v>
+      </c>
+      <c r="E171">
+        <v>0.83</v>
+      </c>
+      <c r="F171">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="G171">
+        <f t="shared" si="6"/>
+        <v>-0.28000000000000014</v>
+      </c>
+      <c r="H171">
+        <v>14.5</v>
+      </c>
+      <c r="I171">
+        <v>5.82</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A172" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B172">
+        <v>6</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+      <c r="D172" t="s">
+        <v>14</v>
+      </c>
+      <c r="E172">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F172">
+        <v>1.41</v>
+      </c>
+      <c r="G172">
+        <f t="shared" si="6"/>
+        <v>-1.27</v>
+      </c>
+      <c r="H172">
+        <v>17.8</v>
+      </c>
+      <c r="I172">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A173" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B173">
+        <v>6</v>
+      </c>
+      <c r="C173">
+        <v>2</v>
+      </c>
+      <c r="D173" t="s">
+        <v>15</v>
+      </c>
+      <c r="E173">
+        <v>0.79</v>
+      </c>
+      <c r="F173">
+        <v>1.83</v>
+      </c>
+      <c r="G173">
+        <f t="shared" si="6"/>
+        <v>-1.04</v>
+      </c>
+      <c r="H173">
+        <v>17.8</v>
+      </c>
+      <c r="I173">
+        <v>4.45</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A174" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B174">
+        <v>6</v>
+      </c>
+      <c r="C174">
+        <v>3</v>
+      </c>
+      <c r="D174" t="s">
+        <v>16</v>
+      </c>
+      <c r="E174">
+        <v>0.02</v>
+      </c>
+      <c r="F174">
+        <v>1.03</v>
+      </c>
+      <c r="G174">
+        <f t="shared" si="6"/>
+        <v>-1.01</v>
+      </c>
+      <c r="H174">
+        <v>18.8</v>
+      </c>
+      <c r="I174">
+        <v>5.21</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A175" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B175">
+        <v>6</v>
+      </c>
+      <c r="C175">
+        <v>4</v>
+      </c>
+      <c r="D175" t="s">
+        <v>17</v>
+      </c>
+      <c r="E175">
+        <v>0.2</v>
+      </c>
+      <c r="F175">
+        <v>0.66</v>
+      </c>
+      <c r="G175">
+        <f t="shared" si="6"/>
+        <v>-0.46</v>
+      </c>
+      <c r="H175">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="I175">
+        <v>4.2300000000000004</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A176" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B176">
+        <v>9</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+      <c r="D176" t="s">
+        <v>19</v>
+      </c>
+      <c r="E176">
+        <v>0.27</v>
+      </c>
+      <c r="F176">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="G176">
+        <f t="shared" si="6"/>
+        <v>-0.34499999999999997</v>
+      </c>
+      <c r="H176">
+        <v>13</v>
+      </c>
+      <c r="I176">
+        <v>4.37</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A177" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B177">
+        <v>9</v>
+      </c>
+      <c r="C177">
+        <v>2</v>
+      </c>
+      <c r="D177" t="s">
+        <v>20</v>
+      </c>
+      <c r="E177">
+        <v>0</v>
+      </c>
+      <c r="F177">
+        <v>0.65</v>
+      </c>
+      <c r="G177">
+        <f t="shared" si="6"/>
+        <v>-0.65</v>
+      </c>
+      <c r="H177">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="I177">
+        <v>4.1100000000000003</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A178" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B178">
+        <v>9</v>
+      </c>
+      <c r="C178">
+        <v>3</v>
+      </c>
+      <c r="D178" t="s">
+        <v>21</v>
+      </c>
+      <c r="E178">
+        <v>0</v>
+      </c>
+      <c r="F178">
+        <v>0.84</v>
+      </c>
+      <c r="G178">
+        <f t="shared" si="6"/>
+        <v>-0.84</v>
+      </c>
+      <c r="H178">
+        <v>18</v>
+      </c>
+      <c r="I178">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A179" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B179">
+        <v>9</v>
+      </c>
+      <c r="C179">
+        <v>4</v>
+      </c>
+      <c r="D179" t="s">
+        <v>22</v>
+      </c>
+      <c r="E179">
+        <v>0.31</v>
+      </c>
+      <c r="F179">
+        <v>1.4</v>
+      </c>
+      <c r="G179">
+        <f t="shared" si="6"/>
+        <v>-1.0899999999999999</v>
+      </c>
+      <c r="H179">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="I179">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A180" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B180">
+        <v>9</v>
+      </c>
+      <c r="C180">
+        <v>5</v>
+      </c>
+      <c r="D180" t="s">
+        <v>37</v>
+      </c>
+      <c r="E180">
+        <v>0.03</v>
+      </c>
+      <c r="F180">
+        <v>1.47</v>
+      </c>
+      <c r="G180">
+        <f t="shared" si="6"/>
+        <v>-1.44</v>
+      </c>
+      <c r="H180">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="I180">
+        <v>4.4800000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on long teritiary diagrams. finised RC code
</commit_message>
<xml_diff>
--- a/01_Raw_data/RC log.xlsx
+++ b/01_Raw_data/RC log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Howley_Bradford_Streams\Howley_Bradford_Streams\01_Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C98234-5589-4202-B07D-A573C512C215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37534C80-662C-4FCC-8CE8-BF183DF50E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3405" windowWidth="29040" windowHeight="15720" xr2:uid="{A079E74B-2391-4069-81A1-6515CCD90540}"/>
+    <workbookView xWindow="-24045" yWindow="3900" windowWidth="19185" windowHeight="10065" activeTab="1" xr2:uid="{A079E74B-2391-4069-81A1-6515CCD90540}"/>
   </bookViews>
   <sheets>
     <sheet name="RC log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>WT to Well Top (m)</t>
+  </si>
+  <si>
+    <t>DistanceID</t>
   </si>
 </sst>
 </file>
@@ -803,7 +806,7 @@
           </c:trendline>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$J:$J</c:f>
+              <c:f>Sheet1!$K:$K</c:f>
               <c:strCache>
                 <c:ptCount val="297"/>
                 <c:pt idx="0">
@@ -1702,7 +1705,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I:$I</c:f>
+              <c:f>Sheet1!$J:$J</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048576"/>
@@ -3354,13 +3357,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
@@ -3710,7 +3713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04E7760-F87C-4D84-A63F-D473D279D553}">
   <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K181" sqref="K181"/>
     </sheetView>
@@ -9063,10 +9066,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DED55BC-E84B-4096-92BA-96DACA0090BF}">
-  <dimension ref="A1:J297"/>
+  <dimension ref="A1:K297"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -9074,12 +9077,14 @@
     <col min="2" max="2" width="10.40625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -9104,14 +9109,17 @@
       <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -9133,13 +9141,16 @@
         <v>1.6500000000000001</v>
       </c>
       <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
         <v>532.32979999999998</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>79.863910000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -9161,13 +9172,16 @@
         <v>1.6800000000000002</v>
       </c>
       <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
         <v>547.30619999999999</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>76.943730000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -9189,13 +9203,16 @@
         <v>1.1949999999999998</v>
       </c>
       <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
         <v>547.31349999999998</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>88.202100000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -9217,13 +9234,16 @@
         <v>2.0099999999999998</v>
       </c>
       <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
         <v>577.80020000000002</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>76.922430000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -9245,13 +9265,16 @@
         <v>0.59000000000000008</v>
       </c>
       <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
         <v>623.08079999999995</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>92.059330000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -9273,13 +9296,16 @@
         <v>1.95</v>
       </c>
       <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
         <v>653.02340000000004</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>76.370699999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -9298,13 +9324,16 @@
         <v>0</v>
       </c>
       <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
         <v>698.30179999999996</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>93.197450000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -9326,13 +9355,16 @@
         <v>1.8299999999999998</v>
       </c>
       <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
         <v>698.75670000000002</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>76.815430000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -9354,13 +9386,16 @@
         <v>0.63</v>
       </c>
       <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
         <v>744.30139999999994</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>76.590829999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -9382,13 +9417,16 @@
         <v>2.75</v>
       </c>
       <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
         <v>728.80870000000004</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>76.606219999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -9410,13 +9448,16 @@
         <v>-8.0000000000000071E-2</v>
       </c>
       <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
         <v>728.81809999999996</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>76.513019999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -9438,13 +9479,16 @@
         <v>2.38</v>
       </c>
       <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
         <v>728.81179999999995</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>76.622630000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -9466,13 +9510,16 @@
         <v>1.605</v>
       </c>
       <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
         <v>759.42010000000005</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>66.857730000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -9494,13 +9541,16 @@
         <v>2.1</v>
       </c>
       <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
         <v>744.24469999999997</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>67.045649999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -9522,13 +9572,16 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
         <v>698.35050000000001</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>67.109120000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -9547,3369 +9600,3398 @@
         <v>1.905</v>
       </c>
       <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
         <v>667.92629999999997</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>66.502930000000006</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <f>B8+15.14</f>
+        <v>55.14</v>
+      </c>
+      <c r="C18">
+        <f>CONVERT(B18,"ft","m")</f>
+        <v>16.806671999999999</v>
+      </c>
+      <c r="D18">
+        <v>0.44</v>
+      </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44</v>
       </c>
       <c r="I18">
+        <v>8</v>
+      </c>
+      <c r="J18">
         <v>652.93119999999999</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>66.842190000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19">
+        <v>0.02</v>
+      </c>
       <c r="H19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
         <v>653.20910000000003</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>66.69511</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.75">
       <c r="H20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>607.95830000000001</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>67.072839999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.75">
       <c r="H21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>607.56110000000001</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>66.492159999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.75">
       <c r="H22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>638.08180000000004</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>66.821780000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
       <c r="H23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>638.25340000000006</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>66.970429999999993</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
       <c r="H24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>623.13530000000003</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>66.743210000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.75">
       <c r="H25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>607.76750000000004</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>66.741129999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.75">
       <c r="H26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>592.50710000000004</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>66.642009999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.75">
       <c r="H27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>577.47490000000005</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>66.604929999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.75">
       <c r="H28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>562.39620000000002</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>66.727909999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.75">
       <c r="H29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>562.76610000000005</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>66.755129999999994</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.75">
       <c r="H30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>562.50009999999997</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>66.565960000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.75">
       <c r="H31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>562.36329999999998</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>66.708879999999994</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.75">
       <c r="H32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>577.42870000000005</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>66.438630000000003</v>
       </c>
     </row>
-    <row r="33" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="33" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>577.51340000000005</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>66.721999999999994</v>
       </c>
     </row>
-    <row r="34" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="34" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>622.80349999999999</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>66.502319999999997</v>
       </c>
     </row>
-    <row r="35" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="35" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>698.44579999999996</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>66.603359999999995</v>
       </c>
     </row>
-    <row r="36" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="36" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>728.82050000000004</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>66.735640000000004</v>
       </c>
     </row>
-    <row r="37" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="37" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>744.46180000000004</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>67.009540000000001</v>
       </c>
     </row>
-    <row r="38" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="38" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>728.54539999999997</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>66.730959999999996</v>
       </c>
     </row>
-    <row r="39" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="39" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H39">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>728.59079999999994</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>66.700519999999997</v>
       </c>
     </row>
-    <row r="40" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="40" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>728.52480000000003</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>66.432400000000001</v>
       </c>
     </row>
-    <row r="41" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="41" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H41">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>744.04729999999995</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>66.440209999999993</v>
       </c>
     </row>
-    <row r="42" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="42" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H42">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>744.07650000000001</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>66.810680000000005</v>
       </c>
     </row>
-    <row r="43" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="43" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>759.36440000000005</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>66.765969999999996</v>
       </c>
     </row>
-    <row r="44" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="44" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H44">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>774.61670000000004</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>66.688059999999993</v>
       </c>
     </row>
-    <row r="45" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="45" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <v>774.67240000000004</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>66.708640000000003</v>
       </c>
     </row>
-    <row r="46" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="46" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H46">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>789.6807</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>66.707120000000003</v>
       </c>
     </row>
-    <row r="47" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="47" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H47">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>834.55520000000001</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>66.699510000000004</v>
       </c>
     </row>
-    <row r="48" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="48" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>834.96130000000005</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>67.011229999999998</v>
       </c>
     </row>
-    <row r="49" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="49" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H49">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>850.197</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>66.578879999999998</v>
       </c>
     </row>
-    <row r="50" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="50" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <v>865.02120000000002</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>66.439570000000003</v>
       </c>
     </row>
-    <row r="51" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="51" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H51">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <v>865.25400000000002</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>66.421679999999995</v>
       </c>
     </row>
-    <row r="52" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="52" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>880.46839999999997</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>66.699039999999997</v>
       </c>
     </row>
-    <row r="53" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="53" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H53">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>895.39089999999999</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>66.41798</v>
       </c>
     </row>
-    <row r="54" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="54" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H54">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>895.33799999999997</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>66.555769999999995</v>
       </c>
     </row>
-    <row r="55" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="55" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <v>910.66690000000006</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <v>66.713909999999998</v>
       </c>
     </row>
-    <row r="56" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="56" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I56">
+      <c r="J56">
         <v>925.98109999999997</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>66.679460000000006</v>
       </c>
     </row>
-    <row r="57" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="57" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H57">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I57">
+      <c r="J57">
         <v>940.77919999999995</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>66.716350000000006</v>
       </c>
     </row>
-    <row r="58" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="58" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I58">
+      <c r="J58">
         <v>955.72770000000003</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <v>66.600700000000003</v>
       </c>
     </row>
-    <row r="59" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="59" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I59">
+      <c r="J59">
         <v>970.87699999999995</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <v>67.232489999999999</v>
       </c>
     </row>
-    <row r="60" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="60" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I60">
+      <c r="J60">
         <v>986.60170000000005</v>
       </c>
-      <c r="J60">
+      <c r="K60">
         <v>66.475719999999995</v>
       </c>
     </row>
-    <row r="61" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="61" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I61">
+      <c r="J61">
         <v>1001.513</v>
       </c>
-      <c r="J61">
+      <c r="K61">
         <v>69.48903</v>
       </c>
     </row>
-    <row r="62" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="62" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I62">
+      <c r="J62">
         <v>1016.558</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <v>66.661689999999993</v>
       </c>
     </row>
-    <row r="63" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="63" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H63">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <v>1031.5419999999999</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <v>77.511840000000007</v>
       </c>
     </row>
-    <row r="64" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="64" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H64">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <v>1047.2439999999999</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>66.713200000000001</v>
       </c>
     </row>
-    <row r="65" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="65" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I65">
+      <c r="J65">
         <v>1061.7260000000001</v>
       </c>
-      <c r="J65">
+      <c r="K65">
         <v>80.544539999999998</v>
       </c>
     </row>
-    <row r="66" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="66" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H66">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I66">
+      <c r="J66">
         <v>1077.3230000000001</v>
       </c>
-      <c r="J66">
+      <c r="K66">
         <v>66.882890000000003</v>
       </c>
     </row>
-    <row r="67" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="67" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H67">
         <f t="shared" ref="H67:H130" si="2">D67-F67</f>
         <v>0</v>
       </c>
-      <c r="I67">
+      <c r="J67">
         <v>1107.306</v>
       </c>
-      <c r="J67">
+      <c r="K67">
         <v>82.613020000000006</v>
       </c>
     </row>
-    <row r="68" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="68" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I68">
+      <c r="J68">
         <v>1122.7550000000001</v>
       </c>
-      <c r="J68">
+      <c r="K68">
         <v>66.875720000000001</v>
       </c>
     </row>
-    <row r="69" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="69" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H69">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I69">
+      <c r="J69">
         <v>1167.7729999999999</v>
       </c>
-      <c r="J69">
+      <c r="K69">
         <v>81.679119999999998</v>
       </c>
     </row>
-    <row r="70" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="70" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I70">
+      <c r="J70">
         <v>1183.0219999999999</v>
       </c>
-      <c r="J70">
+      <c r="K70">
         <v>76.520039999999995</v>
       </c>
     </row>
-    <row r="71" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="71" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H71">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I71">
+      <c r="J71">
         <v>1183.3119999999999</v>
       </c>
-      <c r="J71">
+      <c r="K71">
         <v>76.523030000000006</v>
       </c>
     </row>
-    <row r="72" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="72" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H72">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I72">
+      <c r="J72">
         <v>1198.4190000000001</v>
       </c>
-      <c r="J72">
+      <c r="K72">
         <v>76.558539999999994</v>
       </c>
     </row>
-    <row r="73" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="73" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H73">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I73">
+      <c r="J73">
         <v>1213.2</v>
       </c>
-      <c r="J73">
+      <c r="K73">
         <v>76.322270000000003</v>
       </c>
     </row>
-    <row r="74" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="74" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H74">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I74">
+      <c r="J74">
         <v>1213.443</v>
       </c>
-      <c r="J74">
+      <c r="K74">
         <v>76.840400000000002</v>
       </c>
     </row>
-    <row r="75" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="75" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H75">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I75">
+      <c r="J75">
         <v>1228.8979999999999</v>
       </c>
-      <c r="J75">
+      <c r="K75">
         <v>76.866280000000003</v>
       </c>
     </row>
-    <row r="76" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="76" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H76">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I76">
+      <c r="J76">
         <v>1244.1220000000001</v>
       </c>
-      <c r="J76">
+      <c r="K76">
         <v>76.297600000000003</v>
       </c>
     </row>
-    <row r="77" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="77" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I77">
+      <c r="J77">
         <v>1259.123</v>
       </c>
-      <c r="J77">
+      <c r="K77">
         <v>76.881839999999997</v>
       </c>
     </row>
-    <row r="78" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="78" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H78">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I78">
+      <c r="J78">
         <v>1258.752</v>
       </c>
-      <c r="J78">
+      <c r="K78">
         <v>76.468999999999994</v>
       </c>
     </row>
-    <row r="79" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="79" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H79">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I79">
+      <c r="J79">
         <v>1304.1369999999999</v>
       </c>
-      <c r="J79">
+      <c r="K79">
         <v>76.618129999999994</v>
       </c>
     </row>
-    <row r="80" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="80" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H80">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I80">
+      <c r="J80">
         <v>1349.9849999999999</v>
       </c>
-      <c r="J80">
+      <c r="K80">
         <v>76.480620000000002</v>
       </c>
     </row>
-    <row r="81" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="81" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I81">
+      <c r="J81">
         <v>1350.0229999999999</v>
       </c>
-      <c r="J81">
+      <c r="K81">
         <v>76.648570000000007</v>
       </c>
     </row>
-    <row r="82" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="82" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H82">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I82">
+      <c r="J82">
         <v>1364.8150000000001</v>
       </c>
-      <c r="J82">
+      <c r="K82">
         <v>76.311499999999995</v>
       </c>
     </row>
-    <row r="83" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="83" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H83">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I83">
+      <c r="J83">
         <v>1380.152</v>
       </c>
-      <c r="J83">
+      <c r="K83">
         <v>76.679150000000007</v>
       </c>
     </row>
-    <row r="84" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="84" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H84">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I84">
+      <c r="J84">
         <v>1380.086</v>
       </c>
-      <c r="J84">
+      <c r="K84">
         <v>76.621639999999999</v>
       </c>
     </row>
-    <row r="85" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="85" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H85">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I85">
+      <c r="J85">
         <v>1379.7149999999999</v>
       </c>
-      <c r="J85">
+      <c r="K85">
         <v>76.371279999999999</v>
       </c>
     </row>
-    <row r="86" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="86" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H86">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I86">
+      <c r="J86">
         <v>1394.9970000000001</v>
       </c>
-      <c r="J86">
+      <c r="K86">
         <v>76.636949999999999</v>
       </c>
     </row>
-    <row r="87" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="87" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H87">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I87">
+      <c r="J87">
         <v>1410.3409999999999</v>
       </c>
-      <c r="J87">
+      <c r="K87">
         <v>76.882059999999996</v>
       </c>
     </row>
-    <row r="88" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="88" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H88">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I88">
+      <c r="J88">
         <v>1425.6030000000001</v>
       </c>
-      <c r="J88">
+      <c r="K88">
         <v>76.91395</v>
       </c>
     </row>
-    <row r="89" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="89" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H89">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I89">
+      <c r="J89">
         <v>1409.979</v>
       </c>
-      <c r="J89">
+      <c r="K89">
         <v>76.394909999999996</v>
       </c>
     </row>
-    <row r="90" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="90" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H90">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I90">
+      <c r="J90">
         <v>1410.248</v>
       </c>
-      <c r="J90">
+      <c r="K90">
         <v>76.664580000000001</v>
       </c>
     </row>
-    <row r="91" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="91" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H91">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I91">
+      <c r="J91">
         <v>1455.58</v>
       </c>
-      <c r="J91">
+      <c r="K91">
         <v>76.792010000000005</v>
       </c>
     </row>
-    <row r="92" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="92" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H92">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I92">
+      <c r="J92">
         <v>1486.2159999999999</v>
       </c>
-      <c r="J92">
+      <c r="K92">
         <v>86.622889999999998</v>
       </c>
     </row>
-    <row r="93" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="93" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I93">
+      <c r="J93">
         <v>1485.806</v>
       </c>
-      <c r="J93">
+      <c r="K93">
         <v>86.426929999999999</v>
       </c>
     </row>
-    <row r="94" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="94" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I94">
+      <c r="J94">
         <v>1516.0709999999999</v>
       </c>
-      <c r="J94">
+      <c r="K94">
         <v>86.291049999999998</v>
       </c>
     </row>
-    <row r="95" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="95" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H95">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I95">
+      <c r="J95">
         <v>1515.9280000000001</v>
       </c>
-      <c r="J95">
+      <c r="K95">
         <v>86.616039999999998</v>
       </c>
     </row>
-    <row r="96" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="96" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H96">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I96">
+      <c r="J96">
         <v>1516.348</v>
       </c>
-      <c r="J96">
+      <c r="K96">
         <v>86.725769999999997</v>
       </c>
     </row>
-    <row r="97" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="97" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H97">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I97">
+      <c r="J97">
         <v>1531.32</v>
       </c>
-      <c r="J97">
+      <c r="K97">
         <v>86.364840000000001</v>
       </c>
     </row>
-    <row r="98" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="98" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H98">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I98">
+      <c r="J98">
         <v>1531.4570000000001</v>
       </c>
-      <c r="J98">
+      <c r="K98">
         <v>86.454610000000002</v>
       </c>
     </row>
-    <row r="99" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="99" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H99">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I99">
+      <c r="J99">
         <v>1531.6220000000001</v>
       </c>
-      <c r="J99">
+      <c r="K99">
         <v>86.403989999999993</v>
       </c>
     </row>
-    <row r="100" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="100" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H100">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I100">
+      <c r="J100">
         <v>1531.232</v>
       </c>
-      <c r="J100">
+      <c r="K100">
         <v>86.471239999999995</v>
       </c>
     </row>
-    <row r="101" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="101" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H101">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I101">
+      <c r="J101">
         <v>1531.4369999999999</v>
       </c>
-      <c r="J101">
+      <c r="K101">
         <v>86.733379999999997</v>
       </c>
     </row>
-    <row r="102" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="102" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H102">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I102">
+      <c r="J102">
         <v>1531.0519999999999</v>
       </c>
-      <c r="J102">
+      <c r="K102">
         <v>86.402079999999998</v>
       </c>
     </row>
-    <row r="103" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="103" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H103">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I103">
+      <c r="J103">
         <v>1531.268</v>
       </c>
-      <c r="J103">
+      <c r="K103">
         <v>86.439710000000005</v>
       </c>
     </row>
-    <row r="104" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="104" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H104">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I104">
+      <c r="J104">
         <v>1546.579</v>
       </c>
-      <c r="J104">
+      <c r="K104">
         <v>86.730919999999998</v>
       </c>
     </row>
-    <row r="105" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="105" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H105">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I105">
+      <c r="J105">
         <v>1546.319</v>
       </c>
-      <c r="J105">
+      <c r="K105">
         <v>86.136409999999998</v>
       </c>
     </row>
-    <row r="106" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="106" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H106">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I106">
+      <c r="J106">
         <v>1576.8009999999999</v>
       </c>
-      <c r="J106">
+      <c r="K106">
         <v>86.486429999999999</v>
       </c>
     </row>
-    <row r="107" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="107" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H107">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I107">
+      <c r="J107">
         <v>1591.886</v>
       </c>
-      <c r="J107">
+      <c r="K107">
         <v>86.408940000000001</v>
       </c>
     </row>
-    <row r="108" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="108" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H108">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I108">
+      <c r="J108">
         <v>1607.3309999999999</v>
       </c>
-      <c r="J108">
+      <c r="K108">
         <v>86.266360000000006</v>
       </c>
     </row>
-    <row r="109" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="109" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H109">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I109">
+      <c r="J109">
         <v>1607.1669999999999</v>
       </c>
-      <c r="J109">
+      <c r="K109">
         <v>96.321259999999995</v>
       </c>
     </row>
-    <row r="110" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="110" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H110">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I110">
+      <c r="J110">
         <v>1622.027</v>
       </c>
-      <c r="J110">
+      <c r="K110">
         <v>95.994619999999998</v>
       </c>
     </row>
-    <row r="111" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="111" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H111">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I111">
+      <c r="J111">
         <v>1622.26</v>
       </c>
-      <c r="J111">
+      <c r="K111">
         <v>96.47484</v>
       </c>
     </row>
-    <row r="112" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="112" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H112">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I112">
+      <c r="J112">
         <v>1637.01</v>
       </c>
-      <c r="J112">
+      <c r="K112">
         <v>96.487459999999999</v>
       </c>
     </row>
-    <row r="113" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="113" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I113">
+      <c r="J113">
         <v>1637.1120000000001</v>
       </c>
-      <c r="J113">
+      <c r="K113">
         <v>95.942539999999994</v>
       </c>
     </row>
-    <row r="114" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="114" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H114">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I114">
+      <c r="J114">
         <v>1652.441</v>
       </c>
-      <c r="J114">
+      <c r="K114">
         <v>96.212249999999997</v>
       </c>
     </row>
-    <row r="115" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="115" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H115">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I115">
+      <c r="J115">
         <v>1652.6880000000001</v>
       </c>
-      <c r="J115">
+      <c r="K115">
         <v>96.16</v>
       </c>
     </row>
-    <row r="116" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="116" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I116">
+      <c r="J116">
         <v>1652.4690000000001</v>
       </c>
-      <c r="J116">
+      <c r="K116">
         <v>96.532060000000001</v>
       </c>
     </row>
-    <row r="117" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="117" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H117">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I117">
+      <c r="J117">
         <v>1667.163</v>
       </c>
-      <c r="J117">
+      <c r="K117">
         <v>96.261859999999999</v>
       </c>
     </row>
-    <row r="118" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="118" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H118">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I118">
+      <c r="J118">
         <v>1682.24</v>
       </c>
-      <c r="J118">
+      <c r="K118">
         <v>96.204570000000004</v>
       </c>
     </row>
-    <row r="119" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="119" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H119">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I119">
+      <c r="J119">
         <v>1682.7049999999999</v>
       </c>
-      <c r="J119">
+      <c r="K119">
         <v>95.947130000000001</v>
       </c>
     </row>
-    <row r="120" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="120" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H120">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I120">
+      <c r="J120">
         <v>1697.7449999999999</v>
       </c>
-      <c r="J120">
+      <c r="K120">
         <v>102.5564</v>
       </c>
     </row>
-    <row r="121" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="121" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H121">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I121">
+      <c r="J121">
         <v>1697.4570000000001</v>
       </c>
-      <c r="J121">
+      <c r="K121">
         <v>96.26979</v>
       </c>
     </row>
-    <row r="122" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="122" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H122">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I122">
+      <c r="J122">
         <v>1697.8979999999999</v>
       </c>
-      <c r="J122">
+      <c r="K122">
         <v>107.5222</v>
       </c>
     </row>
-    <row r="123" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="123" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H123">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I123">
+      <c r="J123">
         <v>1713.067</v>
       </c>
-      <c r="J123">
+      <c r="K123">
         <v>96.174220000000005</v>
       </c>
     </row>
-    <row r="124" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="124" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H124">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I124">
+      <c r="J124">
         <v>1713.4069999999999</v>
       </c>
-      <c r="J124">
+      <c r="K124">
         <v>111.3181</v>
       </c>
     </row>
-    <row r="125" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="125" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H125">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I125">
+      <c r="J125">
         <v>1713.269</v>
       </c>
-      <c r="J125">
+      <c r="K125">
         <v>96.214839999999995</v>
       </c>
     </row>
-    <row r="126" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="126" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H126">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I126">
+      <c r="J126">
         <v>1742.9939999999999</v>
       </c>
-      <c r="J126">
+      <c r="K126">
         <v>122.13800000000001</v>
       </c>
     </row>
-    <row r="127" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="127" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H127">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I127">
+      <c r="J127">
         <v>1773.7049999999999</v>
       </c>
-      <c r="J127">
+      <c r="K127">
         <v>105.7696</v>
       </c>
     </row>
-    <row r="128" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="128" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H128">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I128">
+      <c r="J128">
         <v>1788.712</v>
       </c>
-      <c r="J128">
+      <c r="K128">
         <v>106.3018</v>
       </c>
     </row>
-    <row r="129" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="129" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H129">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I129">
+      <c r="J129">
         <v>1803.973</v>
       </c>
-      <c r="J129">
+      <c r="K129">
         <v>106.0164</v>
       </c>
     </row>
-    <row r="130" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="130" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H130">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I130">
+      <c r="J130">
         <v>1803.799</v>
       </c>
-      <c r="J130">
+      <c r="K130">
         <v>106.0008</v>
       </c>
     </row>
-    <row r="131" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="131" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H131">
         <f t="shared" ref="H131:H194" si="3">D131-F131</f>
         <v>0</v>
       </c>
-      <c r="I131">
+      <c r="J131">
         <v>1788.7460000000001</v>
       </c>
-      <c r="J131">
+      <c r="K131">
         <v>106.2757</v>
       </c>
     </row>
-    <row r="132" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="132" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H132">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I132">
+      <c r="J132">
         <v>1803.846</v>
       </c>
-      <c r="J132">
+      <c r="K132">
         <v>105.7705</v>
       </c>
     </row>
-    <row r="133" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="133" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H133">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I133">
+      <c r="J133">
         <v>1788.356</v>
       </c>
-      <c r="J133">
+      <c r="K133">
         <v>106.0813</v>
       </c>
     </row>
-    <row r="134" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="134" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H134">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I134">
+      <c r="J134">
         <v>1773.8130000000001</v>
       </c>
-      <c r="J134">
+      <c r="K134">
         <v>106.3004</v>
       </c>
     </row>
-    <row r="135" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="135" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H135">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I135">
+      <c r="J135">
         <v>1773.46</v>
       </c>
-      <c r="J135">
+      <c r="K135">
         <v>105.8387</v>
       </c>
     </row>
-    <row r="136" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="136" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H136">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I136">
+      <c r="J136">
         <v>1773.855</v>
       </c>
-      <c r="J136">
+      <c r="K136">
         <v>106.3312</v>
       </c>
     </row>
-    <row r="137" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="137" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H137">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I137">
+      <c r="J137">
         <v>1758.252</v>
       </c>
-      <c r="J137">
+      <c r="K137">
         <v>105.94289999999999</v>
       </c>
     </row>
-    <row r="138" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="138" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H138">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I138">
+      <c r="J138">
         <v>1758.42</v>
       </c>
-      <c r="J138">
+      <c r="K138">
         <v>105.88379999999999</v>
       </c>
     </row>
-    <row r="139" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="139" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H139">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I139">
+      <c r="J139">
         <v>1743.6389999999999</v>
       </c>
-      <c r="J139">
+      <c r="K139">
         <v>105.9689</v>
       </c>
     </row>
-    <row r="140" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="140" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H140">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I140">
+      <c r="J140">
         <v>1743.116</v>
       </c>
-      <c r="J140">
+      <c r="K140">
         <v>106.07550000000001</v>
       </c>
     </row>
-    <row r="141" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="141" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H141">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I141">
+      <c r="J141">
         <v>1743.41</v>
       </c>
-      <c r="J141">
+      <c r="K141">
         <v>105.9944</v>
       </c>
     </row>
-    <row r="142" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="142" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H142">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I142">
+      <c r="J142">
         <v>1758.229</v>
       </c>
-      <c r="J142">
+      <c r="K142">
         <v>105.9682</v>
       </c>
     </row>
-    <row r="143" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="143" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H143">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I143">
+      <c r="J143">
         <v>1758.6110000000001</v>
       </c>
-      <c r="J143">
+      <c r="K143">
         <v>106.0844</v>
       </c>
     </row>
-    <row r="144" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="144" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H144">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I144">
+      <c r="J144">
         <v>1758.502</v>
       </c>
-      <c r="J144">
+      <c r="K144">
         <v>106.253</v>
       </c>
     </row>
-    <row r="145" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="145" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H145">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I145">
+      <c r="J145">
         <v>1758.336</v>
       </c>
-      <c r="J145">
+      <c r="K145">
         <v>105.9712</v>
       </c>
     </row>
-    <row r="146" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="146" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H146">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I146">
+      <c r="J146">
         <v>1743.46</v>
       </c>
-      <c r="J146">
+      <c r="K146">
         <v>105.7208</v>
       </c>
     </row>
-    <row r="147" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="147" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H147">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I147">
+      <c r="J147">
         <v>1743.7249999999999</v>
       </c>
-      <c r="J147">
+      <c r="K147">
         <v>106.00369999999999</v>
       </c>
     </row>
-    <row r="148" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="148" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H148">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I148">
+      <c r="J148">
         <v>1743.2550000000001</v>
       </c>
-      <c r="J148">
+      <c r="K148">
         <v>105.74850000000001</v>
       </c>
     </row>
-    <row r="149" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="149" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H149">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I149">
+      <c r="J149">
         <v>1743.2</v>
       </c>
-      <c r="J149">
+      <c r="K149">
         <v>105.6892</v>
       </c>
     </row>
-    <row r="150" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="150" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H150">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I150">
+      <c r="J150">
         <v>1743.645</v>
       </c>
-      <c r="J150">
+      <c r="K150">
         <v>115.9367</v>
       </c>
     </row>
-    <row r="151" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="151" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H151">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I151">
+      <c r="J151">
         <v>1743.6010000000001</v>
       </c>
-      <c r="J151">
+      <c r="K151">
         <v>115.7723</v>
       </c>
     </row>
-    <row r="152" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="152" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H152">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I152">
+      <c r="J152">
         <v>1743.2650000000001</v>
       </c>
-      <c r="J152">
+      <c r="K152">
         <v>115.5065</v>
       </c>
     </row>
-    <row r="153" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="153" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H153">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I153">
+      <c r="J153">
         <v>1743.1210000000001</v>
       </c>
-      <c r="J153">
+      <c r="K153">
         <v>116.05670000000001</v>
       </c>
     </row>
-    <row r="154" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="154" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H154">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I154">
+      <c r="J154">
         <v>1743.5830000000001</v>
       </c>
-      <c r="J154">
+      <c r="K154">
         <v>115.9269</v>
       </c>
     </row>
-    <row r="155" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="155" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H155">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I155">
+      <c r="J155">
         <v>1743.1949999999999</v>
       </c>
-      <c r="J155">
+      <c r="K155">
         <v>115.9965</v>
       </c>
     </row>
-    <row r="156" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="156" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H156">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I156">
+      <c r="J156">
         <v>1758.404</v>
       </c>
-      <c r="J156">
+      <c r="K156">
         <v>115.4991</v>
       </c>
     </row>
-    <row r="157" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="157" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H157">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I157">
+      <c r="J157">
         <v>1743.6780000000001</v>
       </c>
-      <c r="J157">
+      <c r="K157">
         <v>115.5228</v>
       </c>
     </row>
-    <row r="158" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="158" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H158">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I158">
+      <c r="J158">
         <v>1743.75</v>
       </c>
-      <c r="J158">
+      <c r="K158">
         <v>115.83710000000001</v>
       </c>
     </row>
-    <row r="159" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="159" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H159">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I159">
+      <c r="J159">
         <v>1743.4010000000001</v>
       </c>
-      <c r="J159">
+      <c r="K159">
         <v>115.67700000000001</v>
       </c>
     </row>
-    <row r="160" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="160" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H160">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I160">
+      <c r="J160">
         <v>1758.3130000000001</v>
       </c>
-      <c r="J160">
+      <c r="K160">
         <v>115.5472</v>
       </c>
     </row>
-    <row r="161" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="161" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H161">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I161">
+      <c r="J161">
         <v>1758.4659999999999</v>
       </c>
-      <c r="J161">
+      <c r="K161">
         <v>116.02809999999999</v>
       </c>
     </row>
-    <row r="162" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="162" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H162">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I162">
+      <c r="J162">
         <v>1758.309</v>
       </c>
-      <c r="J162">
+      <c r="K162">
         <v>115.7191</v>
       </c>
     </row>
-    <row r="163" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="163" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H163">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I163">
+      <c r="J163">
         <v>1758.383</v>
       </c>
-      <c r="J163">
+      <c r="K163">
         <v>115.8503</v>
       </c>
     </row>
-    <row r="164" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="164" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H164">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I164">
+      <c r="J164">
         <v>1758.7819999999999</v>
       </c>
-      <c r="J164">
+      <c r="K164">
         <v>116.01349999999999</v>
       </c>
     </row>
-    <row r="165" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="165" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H165">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I165">
+      <c r="J165">
         <v>1788.462</v>
       </c>
-      <c r="J165">
+      <c r="K165">
         <v>116.0718</v>
       </c>
     </row>
-    <row r="166" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="166" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H166">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I166">
+      <c r="J166">
         <v>1804.0540000000001</v>
       </c>
-      <c r="J166">
+      <c r="K166">
         <v>115.88200000000001</v>
       </c>
     </row>
-    <row r="167" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="167" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H167">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I167">
+      <c r="J167">
         <v>1804.001</v>
       </c>
-      <c r="J167">
+      <c r="K167">
         <v>115.82640000000001</v>
       </c>
     </row>
-    <row r="168" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="168" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H168">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I168">
+      <c r="J168">
         <v>1818.5730000000001</v>
       </c>
-      <c r="J168">
+      <c r="K168">
         <v>116.0414</v>
       </c>
     </row>
-    <row r="169" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="169" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H169">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I169">
+      <c r="J169">
         <v>1818.624</v>
       </c>
-      <c r="J169">
+      <c r="K169">
         <v>115.7786</v>
       </c>
     </row>
-    <row r="170" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="170" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H170">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I170">
+      <c r="J170">
         <v>1818.7860000000001</v>
       </c>
-      <c r="J170">
+      <c r="K170">
         <v>115.92440000000001</v>
       </c>
     </row>
-    <row r="171" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="171" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H171">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I171">
+      <c r="J171">
         <v>1834.075</v>
       </c>
-      <c r="J171">
+      <c r="K171">
         <v>116.0988</v>
       </c>
     </row>
-    <row r="172" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="172" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H172">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I172">
+      <c r="J172">
         <v>1834.6020000000001</v>
       </c>
-      <c r="J172">
+      <c r="K172">
         <v>115.9281</v>
       </c>
     </row>
-    <row r="173" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="173" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H173">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I173">
+      <c r="J173">
         <v>1834.0730000000001</v>
       </c>
-      <c r="J173">
+      <c r="K173">
         <v>115.8377</v>
       </c>
     </row>
-    <row r="174" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="174" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H174">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I174">
+      <c r="J174">
         <v>1834.4480000000001</v>
       </c>
-      <c r="J174">
+      <c r="K174">
         <v>116.0936</v>
       </c>
     </row>
-    <row r="175" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="175" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H175">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I175">
+      <c r="J175">
         <v>1834.4960000000001</v>
       </c>
-      <c r="J175">
+      <c r="K175">
         <v>115.8402</v>
       </c>
     </row>
-    <row r="176" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="176" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H176">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I176">
+      <c r="J176">
         <v>1849.4380000000001</v>
       </c>
-      <c r="J176">
+      <c r="K176">
         <v>116.17019999999999</v>
       </c>
     </row>
-    <row r="177" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="177" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H177">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I177">
+      <c r="J177">
         <v>1864.201</v>
       </c>
-      <c r="J177">
+      <c r="K177">
         <v>115.6253</v>
       </c>
     </row>
-    <row r="178" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="178" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H178">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I178">
+      <c r="J178">
         <v>1864.7149999999999</v>
       </c>
-      <c r="J178">
+      <c r="K178">
         <v>116.0719</v>
       </c>
     </row>
-    <row r="179" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="179" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H179">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I179">
+      <c r="J179">
         <v>1879.3689999999999</v>
       </c>
-      <c r="J179">
+      <c r="K179">
         <v>116.3058</v>
       </c>
     </row>
-    <row r="180" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="180" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H180">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I180">
+      <c r="J180">
         <v>1894.5129999999999</v>
       </c>
-      <c r="J180">
+      <c r="K180">
         <v>115.8853</v>
       </c>
     </row>
-    <row r="181" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="181" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H181">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I181">
+      <c r="J181">
         <v>1894.61</v>
       </c>
-      <c r="J181">
+      <c r="K181">
         <v>116.38339999999999</v>
       </c>
     </row>
-    <row r="182" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="182" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H182">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I182">
+      <c r="J182">
         <v>1895.0039999999999</v>
       </c>
-      <c r="J182">
+      <c r="K182">
         <v>116.1009</v>
       </c>
     </row>
-    <row r="183" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="183" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H183">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I183">
+      <c r="J183">
         <v>1909.9960000000001</v>
       </c>
-      <c r="J183">
+      <c r="K183">
         <v>126.40130000000001</v>
       </c>
     </row>
-    <row r="184" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="184" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H184">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I184">
+      <c r="J184">
         <v>1909.953</v>
       </c>
-      <c r="J184">
+      <c r="K184">
         <v>115.6763</v>
       </c>
     </row>
-    <row r="185" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="185" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H185">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I185">
+      <c r="J185">
         <v>1909.9480000000001</v>
       </c>
-      <c r="J185">
+      <c r="K185">
         <v>128.953</v>
       </c>
     </row>
-    <row r="186" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="186" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H186">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I186">
+      <c r="J186">
         <v>1925.124</v>
       </c>
-      <c r="J186">
+      <c r="K186">
         <v>115.9194</v>
       </c>
     </row>
-    <row r="187" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="187" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H187">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I187">
+      <c r="J187">
         <v>1924.905</v>
       </c>
-      <c r="J187">
+      <c r="K187">
         <v>131.6455</v>
       </c>
     </row>
-    <row r="188" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="188" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H188">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I188">
+      <c r="J188">
         <v>1939.692</v>
       </c>
-      <c r="J188">
+      <c r="K188">
         <v>115.86109999999999</v>
       </c>
     </row>
-    <row r="189" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="189" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H189">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I189">
+      <c r="J189">
         <v>1939.9169999999999</v>
       </c>
-      <c r="J189">
+      <c r="K189">
         <v>115.68819999999999</v>
       </c>
     </row>
-    <row r="190" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="190" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H190">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I190">
+      <c r="J190">
         <v>1955.596</v>
       </c>
-      <c r="J190">
+      <c r="K190">
         <v>116.19329999999999</v>
       </c>
     </row>
-    <row r="191" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="191" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H191">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I191">
+      <c r="J191">
         <v>1970.683</v>
       </c>
-      <c r="J191">
+      <c r="K191">
         <v>116.134</v>
       </c>
     </row>
-    <row r="192" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="192" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H192">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I192">
+      <c r="J192">
         <v>1970.617</v>
       </c>
-      <c r="J192">
+      <c r="K192">
         <v>116.1763</v>
       </c>
     </row>
-    <row r="193" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="193" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H193">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I193">
+      <c r="J193">
         <v>1970.1420000000001</v>
       </c>
-      <c r="J193">
+      <c r="K193">
         <v>116.0438</v>
       </c>
     </row>
-    <row r="194" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="194" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H194">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I194">
+      <c r="J194">
         <v>1985.317</v>
       </c>
-      <c r="J194">
+      <c r="K194">
         <v>115.9259</v>
       </c>
     </row>
-    <row r="195" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="195" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H195">
         <f t="shared" ref="H195:H258" si="4">D195-F195</f>
         <v>0</v>
       </c>
-      <c r="I195">
+      <c r="J195">
         <v>1985.1020000000001</v>
       </c>
-      <c r="J195">
+      <c r="K195">
         <v>116.0008</v>
       </c>
     </row>
-    <row r="196" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="196" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H196">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I196">
+      <c r="J196">
         <v>2000.7739999999999</v>
       </c>
-      <c r="J196">
+      <c r="K196">
         <v>116.0121</v>
       </c>
     </row>
-    <row r="197" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="197" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H197">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I197">
+      <c r="J197">
         <v>2000.3019999999999</v>
       </c>
-      <c r="J197">
+      <c r="K197">
         <v>115.7264</v>
       </c>
     </row>
-    <row r="198" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="198" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H198">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I198">
+      <c r="J198">
         <v>2015.693</v>
       </c>
-      <c r="J198">
+      <c r="K198">
         <v>115.9374</v>
       </c>
     </row>
-    <row r="199" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="199" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H199">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I199">
+      <c r="J199">
         <v>2030.57</v>
       </c>
-      <c r="J199">
+      <c r="K199">
         <v>115.91459999999999</v>
       </c>
     </row>
-    <row r="200" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="200" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H200">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I200">
+      <c r="J200">
         <v>2046.1120000000001</v>
       </c>
-      <c r="J200">
+      <c r="K200">
         <v>115.63939999999999</v>
       </c>
     </row>
-    <row r="201" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="201" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H201">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I201">
+      <c r="J201">
         <v>2076.0819999999999</v>
       </c>
-      <c r="J201">
+      <c r="K201">
         <v>116.1581</v>
       </c>
     </row>
-    <row r="202" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="202" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H202">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I202">
+      <c r="J202">
         <v>2091.7159999999999</v>
       </c>
-      <c r="J202">
+      <c r="K202">
         <v>115.8416</v>
       </c>
     </row>
-    <row r="203" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="203" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H203">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I203">
+      <c r="J203">
         <v>2106.19</v>
       </c>
-      <c r="J203">
+      <c r="K203">
         <v>115.8566</v>
       </c>
     </row>
-    <row r="204" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="204" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H204">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I204">
+      <c r="J204">
         <v>2106.2840000000001</v>
       </c>
-      <c r="J204">
+      <c r="K204">
         <v>115.8509</v>
       </c>
     </row>
-    <row r="205" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="205" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H205">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I205">
+      <c r="J205">
         <v>2121.7220000000002</v>
       </c>
-      <c r="J205">
+      <c r="K205">
         <v>115.8514</v>
       </c>
     </row>
-    <row r="206" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="206" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H206">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I206">
+      <c r="J206">
         <v>2136.712</v>
       </c>
-      <c r="J206">
+      <c r="K206">
         <v>125.86709999999999</v>
       </c>
     </row>
-    <row r="207" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="207" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H207">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I207">
+      <c r="J207">
         <v>2136.752</v>
       </c>
-      <c r="J207">
+      <c r="K207">
         <v>125.4483</v>
       </c>
     </row>
-    <row r="208" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="208" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H208">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I208">
+      <c r="J208">
         <v>2136.913</v>
       </c>
-      <c r="J208">
+      <c r="K208">
         <v>125.4024</v>
       </c>
     </row>
-    <row r="209" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="209" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H209">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I209">
+      <c r="J209">
         <v>2167.261</v>
       </c>
-      <c r="J209">
+      <c r="K209">
         <v>125.7238</v>
       </c>
     </row>
-    <row r="210" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="210" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H210">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I210">
+      <c r="J210">
         <v>2181.7249999999999</v>
       </c>
-      <c r="J210">
+      <c r="K210">
         <v>125.682</v>
       </c>
     </row>
-    <row r="211" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="211" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H211">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I211">
+      <c r="J211">
         <v>2182.0329999999999</v>
       </c>
-      <c r="J211">
+      <c r="K211">
         <v>125.6857</v>
       </c>
     </row>
-    <row r="212" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="212" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H212">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I212">
+      <c r="J212">
         <v>2197.1640000000002</v>
       </c>
-      <c r="J212">
+      <c r="K212">
         <v>125.4738</v>
       </c>
     </row>
-    <row r="213" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="213" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H213">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I213">
+      <c r="J213">
         <v>2212.6770000000001</v>
       </c>
-      <c r="J213">
+      <c r="K213">
         <v>125.9331</v>
       </c>
     </row>
-    <row r="214" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="214" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H214">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I214">
+      <c r="J214">
         <v>2227.3980000000001</v>
       </c>
-      <c r="J214">
+      <c r="K214">
         <v>125.37139999999999</v>
       </c>
     </row>
-    <row r="215" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="215" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H215">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I215">
+      <c r="J215">
         <v>2242.422</v>
       </c>
-      <c r="J215">
+      <c r="K215">
         <v>125.9153</v>
       </c>
     </row>
-    <row r="216" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="216" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H216">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I216">
+      <c r="J216">
         <v>2257.8890000000001</v>
       </c>
-      <c r="J216">
+      <c r="K216">
         <v>125.6576</v>
       </c>
     </row>
-    <row r="217" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="217" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H217">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I217">
+      <c r="J217">
         <v>2272.59</v>
       </c>
-      <c r="J217">
+      <c r="K217">
         <v>125.5729</v>
       </c>
     </row>
-    <row r="218" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="218" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H218">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I218">
+      <c r="J218">
         <v>2288.2159999999999</v>
       </c>
-      <c r="J218">
+      <c r="K218">
         <v>125.9589</v>
       </c>
     </row>
-    <row r="219" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="219" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H219">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I219">
+      <c r="J219">
         <v>2302.7950000000001</v>
       </c>
-      <c r="J219">
+      <c r="K219">
         <v>135.2037</v>
       </c>
     </row>
-    <row r="220" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="220" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H220">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I220">
+      <c r="J220">
         <v>2318.6460000000002</v>
       </c>
-      <c r="J220">
+      <c r="K220">
         <v>135.52789999999999</v>
       </c>
     </row>
-    <row r="221" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="221" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H221">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I221">
+      <c r="J221">
         <v>2333.2890000000002</v>
       </c>
-      <c r="J221">
+      <c r="K221">
         <v>135.4736</v>
       </c>
     </row>
-    <row r="222" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="222" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H222">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I222">
+      <c r="J222">
         <v>2348.8989999999999</v>
       </c>
-      <c r="J222">
+      <c r="K222">
         <v>135.52209999999999</v>
       </c>
     </row>
-    <row r="223" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="223" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H223">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I223">
+      <c r="J223">
         <v>2363.453</v>
       </c>
-      <c r="J223">
+      <c r="K223">
         <v>135.203</v>
       </c>
     </row>
-    <row r="224" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="224" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H224">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I224">
+      <c r="J224">
         <v>2379.2429999999999</v>
       </c>
-      <c r="J224">
+      <c r="K224">
         <v>135.62870000000001</v>
       </c>
     </row>
-    <row r="225" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="225" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H225">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I225">
+      <c r="J225">
         <v>2378.7959999999998</v>
       </c>
-      <c r="J225">
+      <c r="K225">
         <v>135.7516</v>
       </c>
     </row>
-    <row r="226" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="226" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H226">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I226">
+      <c r="J226">
         <v>2379.1619999999998</v>
       </c>
-      <c r="J226">
+      <c r="K226">
         <v>135.196</v>
       </c>
     </row>
-    <row r="227" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="227" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H227">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I227">
+      <c r="J227">
         <v>2363.471</v>
       </c>
-      <c r="J227">
+      <c r="K227">
         <v>135.72149999999999</v>
       </c>
     </row>
-    <row r="228" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="228" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H228">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I228">
+      <c r="J228">
         <v>2318.3110000000001</v>
       </c>
-      <c r="J228">
+      <c r="K228">
         <v>135.15219999999999</v>
       </c>
     </row>
-    <row r="229" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="229" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H229">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I229">
+      <c r="J229">
         <v>2303.3679999999999</v>
       </c>
-      <c r="J229">
+      <c r="K229">
         <v>135.52850000000001</v>
       </c>
     </row>
-    <row r="230" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="230" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H230">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I230">
+      <c r="J230">
         <v>2303.4119999999998</v>
       </c>
-      <c r="J230">
+      <c r="K230">
         <v>135.50040000000001</v>
       </c>
     </row>
-    <row r="231" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="231" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H231">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I231">
+      <c r="J231">
         <v>2272.797</v>
       </c>
-      <c r="J231">
+      <c r="K231">
         <v>135.14279999999999</v>
       </c>
     </row>
-    <row r="232" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="232" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H232">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I232">
+      <c r="J232">
         <v>2257.855</v>
       </c>
-      <c r="J232">
+      <c r="K232">
         <v>135.7586</v>
       </c>
     </row>
-    <row r="233" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="233" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H233">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I233">
+      <c r="J233">
         <v>2257.732</v>
       </c>
-      <c r="J233">
+      <c r="K233">
         <v>135.2062</v>
       </c>
     </row>
-    <row r="234" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="234" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H234">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I234">
+      <c r="J234">
         <v>2243.0100000000002</v>
       </c>
-      <c r="J234">
+      <c r="K234">
         <v>135.19049999999999</v>
       </c>
     </row>
-    <row r="235" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="235" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H235">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I235">
+      <c r="J235">
         <v>2227.8380000000002</v>
       </c>
-      <c r="J235">
+      <c r="K235">
         <v>135.5018</v>
       </c>
     </row>
-    <row r="236" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="236" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H236">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I236">
+      <c r="J236">
         <v>2227.8609999999999</v>
       </c>
-      <c r="J236">
+      <c r="K236">
         <v>135.70230000000001</v>
       </c>
     </row>
-    <row r="237" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="237" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H237">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I237">
+      <c r="J237">
         <v>2227.7280000000001</v>
       </c>
-      <c r="J237">
+      <c r="K237">
         <v>135.14320000000001</v>
       </c>
     </row>
-    <row r="238" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="238" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H238">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I238">
+      <c r="J238">
         <v>2212.5929999999998</v>
       </c>
-      <c r="J238">
+      <c r="K238">
         <v>135.9186</v>
       </c>
     </row>
-    <row r="239" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="239" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H239">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I239">
+      <c r="J239">
         <v>2212.4630000000002</v>
       </c>
-      <c r="J239">
+      <c r="K239">
         <v>135.1687</v>
       </c>
     </row>
-    <row r="240" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="240" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H240">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I240">
+      <c r="J240">
         <v>2197.69</v>
       </c>
-      <c r="J240">
+      <c r="K240">
         <v>136.13910000000001</v>
       </c>
     </row>
-    <row r="241" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="241" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H241">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I241">
+      <c r="J241">
         <v>2197.442</v>
       </c>
-      <c r="J241">
+      <c r="K241">
         <v>135.43340000000001</v>
       </c>
     </row>
-    <row r="242" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="242" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H242">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I242">
+      <c r="J242">
         <v>2197.8220000000001</v>
       </c>
-      <c r="J242">
+      <c r="K242">
         <v>146.0427</v>
       </c>
     </row>
-    <row r="243" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="243" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H243">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I243">
+      <c r="J243">
         <v>2181.6410000000001</v>
       </c>
-      <c r="J243">
+      <c r="K243">
         <v>135.41380000000001</v>
       </c>
     </row>
-    <row r="244" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="244" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H244">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I244">
+      <c r="J244">
         <v>2181.77</v>
       </c>
-      <c r="J244">
+      <c r="K244">
         <v>148.27549999999999</v>
       </c>
     </row>
-    <row r="245" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="245" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H245">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I245">
+      <c r="J245">
         <v>2182.2109999999998</v>
       </c>
-      <c r="J245">
+      <c r="K245">
         <v>135.7269</v>
       </c>
     </row>
-    <row r="246" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="246" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H246">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I246">
+      <c r="J246">
         <v>2166.9209999999998</v>
       </c>
-      <c r="J246">
+      <c r="K246">
         <v>150.4016</v>
       </c>
     </row>
-    <row r="247" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="247" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H247">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I247">
+      <c r="J247">
         <v>2167.4630000000002</v>
       </c>
-      <c r="J247">
+      <c r="K247">
         <v>135.68629999999999</v>
       </c>
     </row>
-    <row r="248" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="248" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H248">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I248">
+      <c r="J248">
         <v>2166.9349999999999</v>
       </c>
-      <c r="J248">
+      <c r="K248">
         <v>149.3246</v>
       </c>
     </row>
-    <row r="249" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="249" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H249">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I249">
+      <c r="J249">
         <v>2152.0659999999998</v>
       </c>
-      <c r="J249">
+      <c r="K249">
         <v>135.16829999999999</v>
       </c>
     </row>
-    <row r="250" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="250" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H250">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I250">
+      <c r="J250">
         <v>2151.8969999999999</v>
       </c>
-      <c r="J250">
+      <c r="K250">
         <v>135.63730000000001</v>
       </c>
     </row>
-    <row r="251" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="251" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H251">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I251">
+      <c r="J251">
         <v>2151.701</v>
       </c>
-      <c r="J251">
+      <c r="K251">
         <v>135.42089999999999</v>
       </c>
     </row>
-    <row r="252" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="252" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H252">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I252">
+      <c r="J252">
         <v>2152.1179999999999</v>
       </c>
-      <c r="J252">
+      <c r="K252">
         <v>135.44110000000001</v>
       </c>
     </row>
-    <row r="253" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="253" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H253">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I253">
+      <c r="J253">
         <v>2137.1120000000001</v>
       </c>
-      <c r="J253">
+      <c r="K253">
         <v>135.73140000000001</v>
       </c>
     </row>
-    <row r="254" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="254" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H254">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I254">
+      <c r="J254">
         <v>2152.1480000000001</v>
       </c>
-      <c r="J254">
+      <c r="K254">
         <v>135.52979999999999</v>
       </c>
     </row>
-    <row r="255" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="255" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H255">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I255">
+      <c r="J255">
         <v>2136.7139999999999</v>
       </c>
-      <c r="J255">
+      <c r="K255">
         <v>135.16589999999999</v>
       </c>
     </row>
-    <row r="256" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="256" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H256">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I256">
+      <c r="J256">
         <v>2136.7220000000002</v>
       </c>
-      <c r="J256">
+      <c r="K256">
         <v>135.43109999999999</v>
       </c>
     </row>
-    <row r="257" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="257" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H257">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I257">
+      <c r="J257">
         <v>2137.1190000000001</v>
       </c>
-      <c r="J257">
+      <c r="K257">
         <v>135.6944</v>
       </c>
     </row>
-    <row r="258" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="258" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H258">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I258">
+      <c r="J258">
         <v>2137.2060000000001</v>
       </c>
-      <c r="J258">
+      <c r="K258">
         <v>135.5111</v>
       </c>
     </row>
-    <row r="259" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="259" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H259">
         <f t="shared" ref="H259:H297" si="5">D259-F259</f>
         <v>0</v>
       </c>
-      <c r="I259">
+      <c r="J259">
         <v>2137.136</v>
       </c>
-      <c r="J259">
+      <c r="K259">
         <v>135.74529999999999</v>
       </c>
     </row>
-    <row r="260" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="260" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H260">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I260">
+      <c r="J260">
         <v>2136.998</v>
       </c>
-      <c r="J260">
+      <c r="K260">
         <v>135.589</v>
       </c>
     </row>
-    <row r="261" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="261" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H261">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I261">
+      <c r="J261">
         <v>2137.0430000000001</v>
       </c>
-      <c r="J261">
+      <c r="K261">
         <v>135.4787</v>
       </c>
     </row>
-    <row r="262" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="262" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H262">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I262">
+      <c r="J262">
         <v>2136.9940000000001</v>
       </c>
-      <c r="J262">
+      <c r="K262">
         <v>135.501</v>
       </c>
     </row>
-    <row r="263" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="263" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H263">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I263">
+      <c r="J263">
         <v>2151.7600000000002</v>
       </c>
-      <c r="J263">
+      <c r="K263">
         <v>135.68340000000001</v>
       </c>
     </row>
-    <row r="264" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="264" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H264">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I264">
+      <c r="J264">
         <v>2136.674</v>
       </c>
-      <c r="J264">
+      <c r="K264">
         <v>135.40479999999999</v>
       </c>
     </row>
-    <row r="265" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="265" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H265">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I265">
+      <c r="J265">
         <v>2151.973</v>
       </c>
-      <c r="J265">
+      <c r="K265">
         <v>135.34440000000001</v>
       </c>
     </row>
-    <row r="266" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="266" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H266">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I266">
+      <c r="J266">
         <v>2151.9319999999998</v>
       </c>
-      <c r="J266">
+      <c r="K266">
         <v>135.4581</v>
       </c>
     </row>
-    <row r="267" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="267" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H267">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I267">
+      <c r="J267">
         <v>2151.9209999999998</v>
       </c>
-      <c r="J267">
+      <c r="K267">
         <v>135.1977</v>
       </c>
     </row>
-    <row r="268" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="268" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H268">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I268">
+      <c r="J268">
         <v>2151.9989999999998</v>
       </c>
-      <c r="J268">
+      <c r="K268">
         <v>135.34399999999999</v>
       </c>
     </row>
-    <row r="269" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="269" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H269">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I269">
+      <c r="J269">
         <v>2166.6460000000002</v>
       </c>
-      <c r="J269">
+      <c r="K269">
         <v>135.76349999999999</v>
       </c>
     </row>
-    <row r="270" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="270" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H270">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I270">
+      <c r="J270">
         <v>2152.134</v>
       </c>
-      <c r="J270">
+      <c r="K270">
         <v>135.49199999999999</v>
       </c>
     </row>
-    <row r="271" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="271" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H271">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I271">
+      <c r="J271">
         <v>2167.125</v>
       </c>
-      <c r="J271">
+      <c r="K271">
         <v>135.47919999999999</v>
       </c>
     </row>
-    <row r="272" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="272" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H272">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I272">
+      <c r="J272">
         <v>2166.8739999999998</v>
       </c>
-      <c r="J272">
+      <c r="K272">
         <v>135.7834</v>
       </c>
     </row>
-    <row r="273" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="273" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H273">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I273">
+      <c r="J273">
         <v>2182.17</v>
       </c>
-      <c r="J273">
+      <c r="K273">
         <v>135.50450000000001</v>
       </c>
     </row>
-    <row r="274" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="274" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H274">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I274">
+      <c r="J274">
         <v>2182.067</v>
       </c>
-      <c r="J274">
+      <c r="K274">
         <v>135.22200000000001</v>
       </c>
     </row>
-    <row r="275" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="275" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H275">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I275">
+      <c r="J275">
         <v>2197.5309999999999</v>
       </c>
-      <c r="J275">
+      <c r="K275">
         <v>135.49209999999999</v>
       </c>
     </row>
-    <row r="276" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="276" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H276">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I276">
+      <c r="J276">
         <v>2197.299</v>
       </c>
-      <c r="J276">
+      <c r="K276">
         <v>135.19800000000001</v>
       </c>
     </row>
-    <row r="277" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="277" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H277">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I277">
+      <c r="J277">
         <v>2212.5549999999998</v>
       </c>
-      <c r="J277">
+      <c r="K277">
         <v>135.47669999999999</v>
       </c>
     </row>
-    <row r="278" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="278" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H278">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I278">
+      <c r="J278">
         <v>2227.5909999999999</v>
       </c>
-      <c r="J278">
+      <c r="K278">
         <v>135.24359999999999</v>
       </c>
     </row>
-    <row r="279" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="279" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H279">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I279">
+      <c r="J279">
         <v>2242.674</v>
       </c>
-      <c r="J279">
+      <c r="K279">
         <v>135.78200000000001</v>
       </c>
     </row>
-    <row r="280" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="280" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H280">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I280">
+      <c r="J280">
         <v>2242.6320000000001</v>
       </c>
-      <c r="J280">
+      <c r="K280">
         <v>135.61869999999999</v>
       </c>
     </row>
-    <row r="281" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="281" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H281">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I281">
+      <c r="J281">
         <v>2257.8119999999999</v>
       </c>
-      <c r="J281">
+      <c r="K281">
         <v>135.5112</v>
       </c>
     </row>
-    <row r="282" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="282" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H282">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I282">
+      <c r="J282">
         <v>2257.9879999999998</v>
       </c>
-      <c r="J282">
+      <c r="K282">
         <v>135.25960000000001</v>
       </c>
     </row>
-    <row r="283" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="283" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H283">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I283">
+      <c r="J283">
         <v>2273.31</v>
       </c>
-      <c r="J283">
+      <c r="K283">
         <v>135.57429999999999</v>
       </c>
     </row>
-    <row r="284" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="284" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H284">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I284">
+      <c r="J284">
         <v>2272.7620000000002</v>
       </c>
-      <c r="J284">
+      <c r="K284">
         <v>135.48140000000001</v>
       </c>
     </row>
-    <row r="285" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="285" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H285">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I285">
+      <c r="J285">
         <v>2272.7910000000002</v>
       </c>
-      <c r="J285">
+      <c r="K285">
         <v>135.24860000000001</v>
       </c>
     </row>
-    <row r="286" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="286" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H286">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I286">
+      <c r="J286">
         <v>2303.0889999999999</v>
       </c>
-      <c r="J286">
+      <c r="K286">
         <v>135.2543</v>
       </c>
     </row>
-    <row r="287" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="287" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H287">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I287">
+      <c r="J287">
         <v>2318.8209999999999</v>
       </c>
-      <c r="J287">
+      <c r="K287">
         <v>135.78460000000001</v>
       </c>
     </row>
-    <row r="288" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="288" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H288">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I288">
+      <c r="J288">
         <v>2334.0030000000002</v>
       </c>
-      <c r="J288">
+      <c r="K288">
         <v>135.56190000000001</v>
       </c>
     </row>
-    <row r="289" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="289" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H289">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I289">
+      <c r="J289">
         <v>2348.922</v>
       </c>
-      <c r="J289">
+      <c r="K289">
         <v>135.61609999999999</v>
       </c>
     </row>
-    <row r="290" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="290" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H290">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I290">
+      <c r="J290">
         <v>2348.8249999999998</v>
       </c>
-      <c r="J290">
+      <c r="K290">
         <v>135.52010000000001</v>
       </c>
     </row>
-    <row r="291" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="291" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H291">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I291">
+      <c r="J291">
         <v>2348.7159999999999</v>
       </c>
-      <c r="J291">
+      <c r="K291">
         <v>135.76300000000001</v>
       </c>
     </row>
-    <row r="292" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="292" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H292">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I292">
+      <c r="J292">
         <v>2363.6129999999998</v>
       </c>
-      <c r="J292">
+      <c r="K292">
         <v>135.53290000000001</v>
       </c>
     </row>
-    <row r="293" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="293" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H293">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I293">
+      <c r="J293">
         <v>2378.8510000000001</v>
       </c>
-      <c r="J293">
+      <c r="K293">
         <v>135.28210000000001</v>
       </c>
     </row>
-    <row r="294" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="294" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H294">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I294">
+      <c r="J294">
         <v>2379.19</v>
       </c>
-      <c r="J294">
+      <c r="K294">
         <v>135.48609999999999</v>
       </c>
     </row>
-    <row r="295" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="295" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H295">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I295">
+      <c r="J295">
         <v>2394.2730000000001</v>
       </c>
-      <c r="J295">
+      <c r="K295">
         <v>135.55950000000001</v>
       </c>
     </row>
-    <row r="296" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="296" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H296">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I296">
+      <c r="J296">
         <v>2393.9299999999998</v>
       </c>
-      <c r="J296">
+      <c r="K296">
         <v>135.2533</v>
       </c>
     </row>
-    <row r="297" spans="8:10" x14ac:dyDescent="0.75">
+    <row r="297" spans="8:11" x14ac:dyDescent="0.75">
       <c r="H297">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I297">
+      <c r="J297">
         <v>2394.2550000000001</v>
       </c>
-      <c r="J297">
+      <c r="K297">
         <v>135.85169999999999</v>
       </c>
     </row>

</xml_diff>